<commit_message>
Gantt in Online_Shop.Projekt.FIAE_B.xlsx überarbeitet
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
+++ b/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
@@ -313,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -370,6 +370,21 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -396,7 +411,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,7 +584,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="70" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,7 +596,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -593,6 +612,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,10 +625,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -768,7 +787,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8207280" y="325080"/>
+          <a:off x="8215920" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -792,13 +811,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>885960</xdr:colOff>
+      <xdr:colOff>886320</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>902520</xdr:colOff>
+      <xdr:colOff>902880</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -809,8 +828,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5451840" y="479520"/>
-          <a:ext cx="5514120" cy="0"/>
+          <a:off x="5457240" y="479520"/>
+          <a:ext cx="5522040" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -850,7 +869,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5473080" y="488160"/>
+          <a:off x="5478120" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -891,7 +910,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483160" y="488160"/>
+          <a:off x="5489640" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -932,7 +951,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="488160"/>
+          <a:off x="8242200" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -973,7 +992,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10980720" y="488160"/>
+          <a:off x="10994400" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1014,7 +1033,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483160" y="1122120"/>
+          <a:off x="5489640" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1055,7 +1074,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483160" y="1609560"/>
+          <a:off x="5489640" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1096,7 +1115,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483160" y="2097720"/>
+          <a:off x="5489640" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1137,7 +1156,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5483160" y="2584800"/>
+          <a:off x="5489640" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1178,7 +1197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="1122120"/>
+          <a:off x="8242200" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1219,7 +1238,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="1609560"/>
+          <a:off x="8242200" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1260,7 +1279,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="2097720"/>
+          <a:off x="8242200" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1301,7 +1320,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="2584800"/>
+          <a:off x="8242200" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1342,7 +1361,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="3072240"/>
+          <a:off x="8242200" y="3072240"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1383,7 +1402,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="3560400"/>
+          <a:off x="8242200" y="3560400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1424,7 +1443,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="4047480"/>
+          <a:off x="8242200" y="4047480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1465,7 +1484,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="4534920"/>
+          <a:off x="8242200" y="4534920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1506,7 +1525,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8232120" y="5023080"/>
+          <a:off x="8242200" y="5023080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1547,7 +1566,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10981080" y="2097360"/>
+          <a:off x="10994760" y="2097360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1588,7 +1607,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10981080" y="1609560"/>
+          <a:off x="10994760" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1629,7 +1648,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10981080" y="1121760"/>
+          <a:off x="10994760" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1660,13 +1679,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>10080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>4680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1675,7 +1694,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9592560" y="478800"/>
+          <a:off x="9597600" y="479160"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1700,15 +1719,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1717,7 +1736,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10932120" y="484920"/>
+          <a:off x="10937520" y="485280"/>
           <a:ext cx="541080" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1742,15 +1761,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
+      <xdr:colOff>255600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1759,7 +1778,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9837360" y="505080"/>
+          <a:off x="9842760" y="505440"/>
           <a:ext cx="18360" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1784,13 +1803,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>11880</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
+      <xdr:colOff>264240</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
@@ -1801,7 +1820,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9864360" y="2435040"/>
+          <a:off x="9869760" y="2435040"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1828,13 +1847,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>244800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1843,7 +1862,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12292920" y="478800"/>
+          <a:off x="12297960" y="479160"/>
           <a:ext cx="1862640" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1868,13 +1887,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
@@ -1885,7 +1904,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10931760" y="2435760"/>
+          <a:off x="10937160" y="2435760"/>
           <a:ext cx="541080" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1927,7 +1946,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12282840" y="2435760"/>
+          <a:off x="12287880" y="2435760"/>
           <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1954,13 +1973,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1969,7 +1988,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11192040" y="482760"/>
+          <a:off x="11197440" y="483120"/>
           <a:ext cx="0" cy="982440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1996,13 +2015,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>253440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>258120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2011,8 +2030,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11188080" y="1455120"/>
-          <a:ext cx="275400" cy="3960"/>
+          <a:off x="11193840" y="1455480"/>
+          <a:ext cx="275040" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2053,7 +2072,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12274920" y="1455840"/>
+          <a:off x="12279960" y="1455840"/>
           <a:ext cx="565920" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2095,7 +2114,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14983560" y="480240"/>
+          <a:off x="14988600" y="480240"/>
           <a:ext cx="560520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2137,7 +2156,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12551760" y="1926720"/>
+          <a:off x="12556800" y="1926720"/>
           <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2162,15 +2181,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2179,7 +2198,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="12552120" y="1943280"/>
+          <a:off x="12557520" y="1943640"/>
           <a:ext cx="1345320" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2204,15 +2223,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2221,7 +2240,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13903560" y="471240"/>
+          <a:off x="13908960" y="471600"/>
           <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2263,7 +2282,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13642200" y="1463040"/>
+          <a:off x="13647240" y="1463040"/>
           <a:ext cx="277920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2305,7 +2324,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16355520" y="478440"/>
+          <a:off x="16360560" y="478440"/>
           <a:ext cx="559800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2347,7 +2366,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17700120" y="478080"/>
+          <a:off x="17705160" y="478080"/>
           <a:ext cx="556560" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2374,13 +2393,13 @@
       <xdr:col>49</xdr:col>
       <xdr:colOff>20520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2389,7 +2408,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19071000" y="484920"/>
+          <a:off x="19076040" y="485280"/>
           <a:ext cx="529200" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2414,15 +2433,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>250920</xdr:colOff>
+      <xdr:colOff>251280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>20160</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2431,7 +2450,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20383200" y="480240"/>
+          <a:off x="20388600" y="480600"/>
           <a:ext cx="580680" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2458,13 +2477,13 @@
       <xdr:col>58</xdr:col>
       <xdr:colOff>251640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
       <xdr:colOff>262080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2473,7 +2492,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="21736800" y="481320"/>
+          <a:off x="21741840" y="481680"/>
           <a:ext cx="551520" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2498,15 +2517,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>66</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2515,7 +2534,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="23109120" y="481320"/>
+          <a:off x="23114520" y="481680"/>
           <a:ext cx="541080" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2540,13 +2559,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>269280</xdr:colOff>
+      <xdr:colOff>269640</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
@@ -2557,7 +2576,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23370840" y="490320"/>
+          <a:off x="23376240" y="490320"/>
           <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2584,13 +2603,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>7920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>259920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2599,7 +2618,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10942920" y="484920"/>
+          <a:off x="10948320" y="485280"/>
           <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2624,15 +2643,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>268920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>254160</xdr:colOff>
+      <xdr:colOff>254520</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2641,7 +2660,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13637880" y="2437560"/>
+          <a:off x="13643280" y="2437920"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2681,27 +2700,9 @@
           <cell r="G2">
             <v>5</v>
           </cell>
-          <cell r="H2" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I2">
-            <v>1</v>
-          </cell>
-          <cell r="J2">
-            <v>5</v>
-          </cell>
         </row>
         <row r="3">
           <cell r="G3">
-            <v>1</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I3">
-            <v>1</v>
-          </cell>
-          <cell r="J3">
             <v>1</v>
           </cell>
         </row>
@@ -2709,27 +2710,9 @@
           <cell r="G4">
             <v>4</v>
           </cell>
-          <cell r="H4" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I4">
-            <v>1</v>
-          </cell>
-          <cell r="J4">
-            <v>4</v>
-          </cell>
         </row>
         <row r="5">
           <cell r="G5">
-            <v>3</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I5">
-            <v>1</v>
-          </cell>
-          <cell r="J5">
             <v>3</v>
           </cell>
         </row>
@@ -2737,27 +2720,9 @@
           <cell r="G6">
             <v>7</v>
           </cell>
-          <cell r="H6" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I6">
-            <v>1</v>
-          </cell>
-          <cell r="J6">
-            <v>7</v>
-          </cell>
         </row>
         <row r="7">
           <cell r="G7">
-            <v>1</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I7">
-            <v>1</v>
-          </cell>
-          <cell r="J7">
             <v>1</v>
           </cell>
         </row>
@@ -2765,27 +2730,9 @@
           <cell r="G8">
             <v>3</v>
           </cell>
-          <cell r="H8" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I8">
-            <v>1</v>
-          </cell>
-          <cell r="J8">
-            <v>3</v>
-          </cell>
         </row>
         <row r="9">
           <cell r="G9">
-            <v>2</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I9">
-            <v>1</v>
-          </cell>
-          <cell r="J9">
             <v>2</v>
           </cell>
         </row>
@@ -2793,27 +2740,9 @@
           <cell r="G10">
             <v>2</v>
           </cell>
-          <cell r="H10" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I10">
-            <v>1</v>
-          </cell>
-          <cell r="J10">
-            <v>2</v>
-          </cell>
         </row>
         <row r="11">
           <cell r="G11">
-            <v>2</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I11">
-            <v>1</v>
-          </cell>
-          <cell r="J11">
             <v>2</v>
           </cell>
         </row>
@@ -2821,27 +2750,9 @@
           <cell r="G12">
             <v>10</v>
           </cell>
-          <cell r="H12" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I12">
-            <v>1</v>
-          </cell>
-          <cell r="J12">
-            <v>10</v>
-          </cell>
         </row>
         <row r="13">
           <cell r="G13">
-            <v>3</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I13">
-            <v>1</v>
-          </cell>
-          <cell r="J13">
             <v>3</v>
           </cell>
         </row>
@@ -2849,27 +2760,9 @@
           <cell r="G14">
             <v>3</v>
           </cell>
-          <cell r="H14" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I14">
-            <v>1</v>
-          </cell>
-          <cell r="J14">
-            <v>3</v>
-          </cell>
         </row>
         <row r="15">
           <cell r="G15">
-            <v>1</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I15">
-            <v>1</v>
-          </cell>
-          <cell r="J15">
             <v>1</v>
           </cell>
         </row>
@@ -2877,27 +2770,9 @@
           <cell r="G16">
             <v>5</v>
           </cell>
-          <cell r="H16" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I16">
-            <v>1</v>
-          </cell>
-          <cell r="J16">
-            <v>5</v>
-          </cell>
         </row>
         <row r="17">
           <cell r="G17">
-            <v>1</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>1</v>
-          </cell>
-          <cell r="I17">
-            <v>1</v>
-          </cell>
-          <cell r="J17">
             <v>1</v>
           </cell>
         </row>
@@ -2919,7 +2794,7 @@
       <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3462,11 +3337,11 @@
   </sheetPr>
   <dimension ref="A1:BQ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
@@ -4594,23 +4469,23 @@
   <dimension ref="A1:BN17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="0" topLeftCell="AP1" activePane="topRight" state="frozen"/>
+      <pane xSplit="11" ySplit="0" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AX15" activeCellId="0" sqref="AX15"/>
+      <selection pane="topRight" activeCell="BN1" activeCellId="0" sqref="BN1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="5" min="5" style="0" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="9" min="7" style="0" width="11.52"/>
     <col collapsed="true" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.59"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="11" min="11" style="0" width="3.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="11" style="0" width="3.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="12" style="0" width="3.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="18.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
@@ -4800,11 +4675,11 @@
       <c r="BM1" s="41" t="n">
         <v>44568</v>
       </c>
-      <c r="BN1" s="0" t="s">
+      <c r="BN1" s="43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
@@ -4822,87 +4697,87 @@
         <v>5</v>
       </c>
       <c r="H2" s="31" t="str">
-        <f aca="false">[1]Netzplan!H2</f>
+        <f aca="false">Netzplan!H2</f>
         <v>1</v>
       </c>
       <c r="I2" s="28" t="n">
-        <f aca="false">[1]Netzplan!I2</f>
-        <v>1</v>
-      </c>
-      <c r="J2" s="43" t="n">
-        <f aca="false">[1]Netzplan!J2</f>
+        <f aca="false">Netzplan!I2</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="44" t="n">
+        <f aca="false">ROUND(G2/(H2*I2),0)</f>
         <v>5</v>
       </c>
-      <c r="K2" s="44" t="n">
+      <c r="K2" s="45" t="n">
         <f aca="false">SUM(L2:BM2)</f>
         <v>5</v>
       </c>
-      <c r="L2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="46"/>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="46"/>
-      <c r="AN2" s="46"/>
-      <c r="AO2" s="46"/>
-      <c r="AP2" s="46"/>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="46"/>
-      <c r="AV2" s="46"/>
-      <c r="AW2" s="46"/>
-      <c r="AX2" s="46"/>
-      <c r="AY2" s="47"/>
-      <c r="AZ2" s="46"/>
-      <c r="BA2" s="46"/>
-      <c r="BB2" s="46"/>
-      <c r="BC2" s="46"/>
-      <c r="BD2" s="46"/>
-      <c r="BE2" s="46"/>
-      <c r="BF2" s="47"/>
-      <c r="BG2" s="46"/>
-      <c r="BH2" s="46"/>
-      <c r="BI2" s="46"/>
-      <c r="BJ2" s="46"/>
-      <c r="BK2" s="46"/>
-      <c r="BL2" s="47"/>
-      <c r="BM2" s="48"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="47"/>
+      <c r="AY2" s="48"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="47"/>
+      <c r="BD2" s="47"/>
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="48"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="47"/>
+      <c r="BJ2" s="47"/>
+      <c r="BK2" s="47"/>
+      <c r="BL2" s="48"/>
+      <c r="BM2" s="49"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -4922,79 +4797,79 @@
         <v>1</v>
       </c>
       <c r="H3" s="31" t="str">
-        <f aca="false">[1]Netzplan!H3</f>
+        <f aca="false">Netzplan!H3</f>
         <v>1</v>
       </c>
       <c r="I3" s="28" t="n">
-        <f aca="false">[1]Netzplan!I3</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="43" t="n">
-        <f aca="false">[1]Netzplan!J3</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="44" t="n">
+        <f aca="false">Netzplan!I3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="44" t="n">
+        <f aca="false">ROUND(G3/(H3*I3),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="45" t="n">
         <f aca="false">SUM(L3:BM3)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="46"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="46"/>
-      <c r="AJ3" s="46"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="46"/>
-      <c r="AM3" s="46"/>
-      <c r="AN3" s="46"/>
-      <c r="AO3" s="46"/>
-      <c r="AP3" s="46"/>
-      <c r="AQ3" s="46"/>
-      <c r="AR3" s="46"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="46"/>
-      <c r="AU3" s="46"/>
-      <c r="AV3" s="46"/>
-      <c r="AW3" s="46"/>
-      <c r="AX3" s="46"/>
-      <c r="AY3" s="47"/>
-      <c r="AZ3" s="46"/>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="46"/>
-      <c r="BC3" s="46"/>
-      <c r="BD3" s="46"/>
-      <c r="BE3" s="46"/>
-      <c r="BF3" s="47"/>
-      <c r="BG3" s="46"/>
-      <c r="BH3" s="46"/>
-      <c r="BI3" s="46"/>
-      <c r="BJ3" s="46"/>
-      <c r="BK3" s="46"/>
-      <c r="BL3" s="47"/>
-      <c r="BM3" s="48"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="47"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="48"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="47"/>
+      <c r="BB3" s="47"/>
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="47"/>
+      <c r="BH3" s="47"/>
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="49"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
@@ -5014,85 +4889,85 @@
         <v>4</v>
       </c>
       <c r="H4" s="31" t="str">
-        <f aca="false">[1]Netzplan!H4</f>
+        <f aca="false">Netzplan!H4</f>
         <v>1</v>
       </c>
       <c r="I4" s="28" t="n">
-        <f aca="false">[1]Netzplan!I4</f>
-        <v>1</v>
-      </c>
-      <c r="J4" s="43" t="n">
-        <f aca="false">[1]Netzplan!J4</f>
+        <f aca="false">Netzplan!I4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="44" t="n">
+        <f aca="false">ROUND(G4/(H4*I4),0)</f>
         <v>4</v>
       </c>
-      <c r="K4" s="44" t="n">
+      <c r="K4" s="45" t="n">
         <f aca="false">SUM(L4:BM4)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="46"/>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="46"/>
-      <c r="AF4" s="46"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="46"/>
-      <c r="AJ4" s="46"/>
-      <c r="AK4" s="46"/>
-      <c r="AL4" s="46"/>
-      <c r="AM4" s="46"/>
-      <c r="AN4" s="46"/>
-      <c r="AO4" s="46"/>
-      <c r="AP4" s="46"/>
-      <c r="AQ4" s="46"/>
-      <c r="AR4" s="46"/>
-      <c r="AS4" s="46"/>
-      <c r="AT4" s="46"/>
-      <c r="AU4" s="46"/>
-      <c r="AV4" s="46"/>
-      <c r="AW4" s="46"/>
-      <c r="AX4" s="46"/>
-      <c r="AY4" s="47"/>
-      <c r="AZ4" s="46"/>
-      <c r="BA4" s="46"/>
-      <c r="BB4" s="46"/>
-      <c r="BC4" s="46"/>
-      <c r="BD4" s="46"/>
-      <c r="BE4" s="46"/>
-      <c r="BF4" s="47"/>
-      <c r="BG4" s="46"/>
-      <c r="BH4" s="46"/>
-      <c r="BI4" s="46"/>
-      <c r="BJ4" s="46"/>
-      <c r="BK4" s="46"/>
-      <c r="BL4" s="47"/>
-      <c r="BM4" s="48"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="47"/>
+      <c r="AL4" s="47"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="47"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="47"/>
+      <c r="AY4" s="48"/>
+      <c r="AZ4" s="47"/>
+      <c r="BA4" s="47"/>
+      <c r="BB4" s="47"/>
+      <c r="BC4" s="47"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="48"/>
+      <c r="BG4" s="47"/>
+      <c r="BH4" s="47"/>
+      <c r="BI4" s="47"/>
+      <c r="BJ4" s="47"/>
+      <c r="BK4" s="47"/>
+      <c r="BL4" s="48"/>
+      <c r="BM4" s="49"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -5112,81 +4987,81 @@
         <v>3</v>
       </c>
       <c r="H5" s="31" t="str">
-        <f aca="false">[1]Netzplan!H5</f>
+        <f aca="false">Netzplan!H5</f>
         <v>1</v>
       </c>
       <c r="I5" s="28" t="n">
-        <f aca="false">[1]Netzplan!I5</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="43" t="n">
-        <f aca="false">[1]Netzplan!J5</f>
+        <f aca="false">Netzplan!I5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="44" t="n">
+        <f aca="false">ROUND(G5/(H5*I5),0)</f>
         <v>3</v>
       </c>
-      <c r="K5" s="44" t="n">
+      <c r="K5" s="45" t="n">
         <f aca="false">SUM(L5:BM5)</f>
         <v>3</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="46"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="46"/>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="46"/>
-      <c r="AL5" s="46"/>
-      <c r="AM5" s="46"/>
-      <c r="AN5" s="46"/>
-      <c r="AO5" s="46"/>
-      <c r="AP5" s="46"/>
-      <c r="AQ5" s="46"/>
-      <c r="AR5" s="46"/>
-      <c r="AS5" s="46"/>
-      <c r="AT5" s="46"/>
-      <c r="AU5" s="46"/>
-      <c r="AV5" s="46"/>
-      <c r="AW5" s="46"/>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="47"/>
-      <c r="AZ5" s="46"/>
-      <c r="BA5" s="46"/>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="46"/>
-      <c r="BD5" s="46"/>
-      <c r="BE5" s="46"/>
-      <c r="BF5" s="47"/>
-      <c r="BG5" s="46"/>
-      <c r="BH5" s="46"/>
-      <c r="BI5" s="46"/>
-      <c r="BJ5" s="46"/>
-      <c r="BK5" s="46"/>
-      <c r="BL5" s="47"/>
-      <c r="BM5" s="48"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="48"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="48"/>
+      <c r="BG5" s="47"/>
+      <c r="BH5" s="47"/>
+      <c r="BI5" s="47"/>
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="47"/>
+      <c r="BL5" s="48"/>
+      <c r="BM5" s="49"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
@@ -5208,91 +5083,87 @@
         <v>7</v>
       </c>
       <c r="H6" s="31" t="str">
-        <f aca="false">[1]Netzplan!H6</f>
-        <v>1</v>
+        <f aca="false">Netzplan!H6</f>
+        <v>2</v>
       </c>
       <c r="I6" s="28" t="n">
-        <f aca="false">[1]Netzplan!I6</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="43" t="n">
-        <f aca="false">[1]Netzplan!J6</f>
-        <v>7</v>
-      </c>
-      <c r="K6" s="44" t="n">
+        <f aca="false">Netzplan!I6</f>
+        <v>0.75</v>
+      </c>
+      <c r="J6" s="44" t="n">
+        <f aca="false">ROUND(G6/(H6*I6),0)</f>
+        <v>5</v>
+      </c>
+      <c r="K6" s="45" t="n">
         <f aca="false">SUM(L6:BM6)</f>
-        <v>7</v>
-      </c>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="46"/>
-      <c r="W6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="X6" s="46"/>
-      <c r="Y6" s="46"/>
-      <c r="Z6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="46"/>
-      <c r="AG6" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="46"/>
-      <c r="AJ6" s="46"/>
-      <c r="AK6" s="46"/>
-      <c r="AL6" s="46"/>
-      <c r="AM6" s="46"/>
-      <c r="AN6" s="46"/>
-      <c r="AO6" s="46"/>
-      <c r="AP6" s="46"/>
-      <c r="AQ6" s="46"/>
-      <c r="AR6" s="46"/>
-      <c r="AS6" s="46"/>
-      <c r="AT6" s="46"/>
-      <c r="AU6" s="46"/>
-      <c r="AV6" s="46"/>
-      <c r="AW6" s="46"/>
-      <c r="AX6" s="46"/>
-      <c r="AY6" s="47"/>
-      <c r="AZ6" s="46"/>
-      <c r="BA6" s="46"/>
-      <c r="BB6" s="46"/>
-      <c r="BC6" s="46"/>
-      <c r="BD6" s="46"/>
-      <c r="BE6" s="46"/>
-      <c r="BF6" s="47"/>
-      <c r="BG6" s="46"/>
-      <c r="BH6" s="46"/>
-      <c r="BI6" s="46"/>
-      <c r="BJ6" s="46"/>
-      <c r="BK6" s="46"/>
-      <c r="BL6" s="47"/>
-      <c r="BM6" s="48"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="47"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="50"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
+      <c r="AG6" s="47"/>
+      <c r="AH6" s="47"/>
+      <c r="AI6" s="47"/>
+      <c r="AJ6" s="47"/>
+      <c r="AK6" s="47"/>
+      <c r="AL6" s="47"/>
+      <c r="AM6" s="47"/>
+      <c r="AN6" s="47"/>
+      <c r="AO6" s="47"/>
+      <c r="AP6" s="47"/>
+      <c r="AQ6" s="47"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="48"/>
+      <c r="AZ6" s="47"/>
+      <c r="BA6" s="47"/>
+      <c r="BB6" s="47"/>
+      <c r="BC6" s="47"/>
+      <c r="BD6" s="47"/>
+      <c r="BE6" s="47"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="47"/>
+      <c r="BH6" s="47"/>
+      <c r="BI6" s="47"/>
+      <c r="BJ6" s="47"/>
+      <c r="BK6" s="47"/>
+      <c r="BL6" s="48"/>
+      <c r="BM6" s="49"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
         <v>22</v>
       </c>
@@ -5312,79 +5183,79 @@
         <v>1</v>
       </c>
       <c r="H7" s="31" t="str">
-        <f aca="false">[1]Netzplan!H7</f>
+        <f aca="false">Netzplan!H7</f>
         <v>1</v>
       </c>
       <c r="I7" s="28" t="n">
-        <f aca="false">[1]Netzplan!I7</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="43" t="n">
-        <f aca="false">[1]Netzplan!J7</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="44" t="n">
+        <f aca="false">Netzplan!I7</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="44" t="n">
+        <f aca="false">ROUND(G7/(H7*I7),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="45" t="n">
         <f aca="false">SUM(L7:BM7)</f>
         <v>1</v>
       </c>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="46"/>
-      <c r="W7" s="46"/>
-      <c r="X7" s="46"/>
-      <c r="Y7" s="46"/>
-      <c r="Z7" s="46"/>
-      <c r="AA7" s="46"/>
-      <c r="AB7" s="46"/>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="46"/>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46"/>
-      <c r="AG7" s="46"/>
-      <c r="AH7" s="46"/>
-      <c r="AI7" s="46"/>
-      <c r="AJ7" s="46"/>
-      <c r="AK7" s="46"/>
-      <c r="AL7" s="46"/>
-      <c r="AM7" s="46"/>
-      <c r="AN7" s="46"/>
-      <c r="AO7" s="46"/>
-      <c r="AP7" s="46"/>
-      <c r="AQ7" s="46"/>
-      <c r="AR7" s="46"/>
-      <c r="AS7" s="46"/>
-      <c r="AT7" s="46"/>
-      <c r="AU7" s="46"/>
-      <c r="AV7" s="46"/>
-      <c r="AW7" s="46"/>
-      <c r="AX7" s="46"/>
-      <c r="AY7" s="47"/>
-      <c r="AZ7" s="46"/>
-      <c r="BA7" s="46"/>
-      <c r="BB7" s="46"/>
-      <c r="BC7" s="46"/>
-      <c r="BD7" s="46"/>
-      <c r="BE7" s="46"/>
-      <c r="BF7" s="47"/>
-      <c r="BG7" s="46"/>
-      <c r="BH7" s="46"/>
-      <c r="BI7" s="46"/>
-      <c r="BJ7" s="46"/>
-      <c r="BK7" s="46"/>
-      <c r="BL7" s="47"/>
-      <c r="BM7" s="48"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="47"/>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="47"/>
+      <c r="AJ7" s="47"/>
+      <c r="AK7" s="47"/>
+      <c r="AL7" s="47"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="47"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="47"/>
+      <c r="AQ7" s="47"/>
+      <c r="AR7" s="47"/>
+      <c r="AS7" s="47"/>
+      <c r="AT7" s="47"/>
+      <c r="AU7" s="47"/>
+      <c r="AV7" s="47"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="47"/>
+      <c r="AY7" s="48"/>
+      <c r="AZ7" s="47"/>
+      <c r="BA7" s="47"/>
+      <c r="BB7" s="47"/>
+      <c r="BC7" s="47"/>
+      <c r="BD7" s="47"/>
+      <c r="BE7" s="47"/>
+      <c r="BF7" s="48"/>
+      <c r="BG7" s="47"/>
+      <c r="BH7" s="47"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="47"/>
+      <c r="BK7" s="47"/>
+      <c r="BL7" s="48"/>
+      <c r="BM7" s="49"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
         <v>28</v>
       </c>
@@ -5404,81 +5275,81 @@
         <v>3</v>
       </c>
       <c r="H8" s="31" t="str">
-        <f aca="false">[1]Netzplan!H8</f>
+        <f aca="false">Netzplan!H8</f>
         <v>1</v>
       </c>
       <c r="I8" s="28" t="n">
-        <f aca="false">[1]Netzplan!I8</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="43" t="n">
-        <f aca="false">[1]Netzplan!J8</f>
+        <f aca="false">Netzplan!I8</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="44" t="n">
+        <f aca="false">ROUND(G8/(H8*I8),0)</f>
         <v>3</v>
       </c>
-      <c r="K8" s="44" t="n">
+      <c r="K8" s="45" t="n">
         <f aca="false">SUM(L8:BM8)</f>
         <v>3</v>
       </c>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="U8" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46"/>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="46"/>
-      <c r="AN8" s="46"/>
-      <c r="AO8" s="46"/>
-      <c r="AP8" s="46"/>
-      <c r="AQ8" s="46"/>
-      <c r="AR8" s="46"/>
-      <c r="AS8" s="46"/>
-      <c r="AT8" s="46"/>
-      <c r="AU8" s="46"/>
-      <c r="AV8" s="46"/>
-      <c r="AW8" s="46"/>
-      <c r="AX8" s="46"/>
-      <c r="AY8" s="47"/>
-      <c r="AZ8" s="46"/>
-      <c r="BA8" s="46"/>
-      <c r="BB8" s="46"/>
-      <c r="BC8" s="46"/>
-      <c r="BD8" s="46"/>
-      <c r="BE8" s="46"/>
-      <c r="BF8" s="47"/>
-      <c r="BG8" s="46"/>
-      <c r="BH8" s="46"/>
-      <c r="BI8" s="46"/>
-      <c r="BJ8" s="46"/>
-      <c r="BK8" s="46"/>
-      <c r="BL8" s="47"/>
-      <c r="BM8" s="48"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+      <c r="AJ8" s="47"/>
+      <c r="AK8" s="47"/>
+      <c r="AL8" s="47"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="47"/>
+      <c r="AO8" s="47"/>
+      <c r="AP8" s="47"/>
+      <c r="AQ8" s="47"/>
+      <c r="AR8" s="47"/>
+      <c r="AS8" s="47"/>
+      <c r="AT8" s="47"/>
+      <c r="AU8" s="47"/>
+      <c r="AV8" s="47"/>
+      <c r="AW8" s="47"/>
+      <c r="AX8" s="47"/>
+      <c r="AY8" s="48"/>
+      <c r="AZ8" s="47"/>
+      <c r="BA8" s="47"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="47"/>
+      <c r="BD8" s="47"/>
+      <c r="BE8" s="47"/>
+      <c r="BF8" s="48"/>
+      <c r="BG8" s="47"/>
+      <c r="BH8" s="47"/>
+      <c r="BI8" s="47"/>
+      <c r="BJ8" s="47"/>
+      <c r="BK8" s="47"/>
+      <c r="BL8" s="48"/>
+      <c r="BM8" s="49"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
@@ -5495,84 +5366,82 @@
       <c r="F9" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="49" t="n">
+      <c r="G9" s="51" t="n">
         <f aca="false">[1]Netzplan!G9</f>
         <v>2</v>
       </c>
-      <c r="H9" s="49" t="str">
-        <f aca="false">[1]Netzplan!H9</f>
-        <v>1</v>
+      <c r="H9" s="31" t="str">
+        <f aca="false">Netzplan!H9</f>
+        <v>2</v>
       </c>
       <c r="I9" s="28" t="n">
-        <f aca="false">[1]Netzplan!I9</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="43" t="n">
-        <f aca="false">[1]Netzplan!J9</f>
-        <v>2</v>
-      </c>
-      <c r="K9" s="44" t="n">
+        <f aca="false">Netzplan!I9</f>
+        <v>0.75</v>
+      </c>
+      <c r="J9" s="44" t="n">
+        <f aca="false">ROUND(G9/(H9*I9),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="45" t="n">
         <f aca="false">SUM(L9:BM9)</f>
-        <v>2</v>
-      </c>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="46"/>
-      <c r="X9" s="46"/>
-      <c r="Y9" s="46"/>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
-      <c r="AB9" s="45"/>
-      <c r="AC9" s="45"/>
-      <c r="AD9" s="45"/>
-      <c r="AE9" s="46"/>
-      <c r="AF9" s="46"/>
-      <c r="AG9" s="45"/>
-      <c r="AH9" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ9" s="46"/>
-      <c r="AK9" s="46"/>
-      <c r="AL9" s="46"/>
-      <c r="AM9" s="46"/>
-      <c r="AN9" s="46"/>
-      <c r="AO9" s="46"/>
-      <c r="AP9" s="46"/>
-      <c r="AQ9" s="46"/>
-      <c r="AR9" s="46"/>
-      <c r="AS9" s="46"/>
-      <c r="AT9" s="46"/>
-      <c r="AU9" s="46"/>
-      <c r="AV9" s="46"/>
-      <c r="AW9" s="46"/>
-      <c r="AX9" s="46"/>
-      <c r="AY9" s="47"/>
-      <c r="AZ9" s="46"/>
-      <c r="BA9" s="46"/>
-      <c r="BB9" s="46"/>
-      <c r="BC9" s="46"/>
-      <c r="BD9" s="46"/>
-      <c r="BE9" s="46"/>
-      <c r="BF9" s="47"/>
-      <c r="BG9" s="46"/>
-      <c r="BH9" s="46"/>
-      <c r="BI9" s="46"/>
-      <c r="BJ9" s="46"/>
-      <c r="BK9" s="46"/>
-      <c r="BL9" s="47"/>
-      <c r="BM9" s="48"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="50"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="50"/>
+      <c r="AC9" s="50"/>
+      <c r="AD9" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
+      <c r="AG9" s="50"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
+      <c r="AK9" s="47"/>
+      <c r="AL9" s="47"/>
+      <c r="AM9" s="47"/>
+      <c r="AN9" s="47"/>
+      <c r="AO9" s="47"/>
+      <c r="AP9" s="47"/>
+      <c r="AQ9" s="47"/>
+      <c r="AR9" s="47"/>
+      <c r="AS9" s="47"/>
+      <c r="AT9" s="47"/>
+      <c r="AU9" s="47"/>
+      <c r="AV9" s="47"/>
+      <c r="AW9" s="47"/>
+      <c r="AX9" s="47"/>
+      <c r="AY9" s="48"/>
+      <c r="AZ9" s="47"/>
+      <c r="BA9" s="47"/>
+      <c r="BB9" s="47"/>
+      <c r="BC9" s="47"/>
+      <c r="BD9" s="47"/>
+      <c r="BE9" s="47"/>
+      <c r="BF9" s="48"/>
+      <c r="BG9" s="47"/>
+      <c r="BH9" s="47"/>
+      <c r="BI9" s="47"/>
+      <c r="BJ9" s="47"/>
+      <c r="BK9" s="47"/>
+      <c r="BL9" s="48"/>
+      <c r="BM9" s="49"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
@@ -5589,84 +5458,82 @@
       <c r="F10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="49" t="n">
+      <c r="G10" s="51" t="n">
         <f aca="false">[1]Netzplan!G10</f>
         <v>2</v>
       </c>
-      <c r="H10" s="49" t="str">
-        <f aca="false">[1]Netzplan!H10</f>
-        <v>1</v>
+      <c r="H10" s="31" t="str">
+        <f aca="false">Netzplan!H10</f>
+        <v>2</v>
       </c>
       <c r="I10" s="28" t="n">
-        <f aca="false">[1]Netzplan!I10</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="43" t="n">
-        <f aca="false">[1]Netzplan!J10</f>
-        <v>2</v>
-      </c>
-      <c r="K10" s="44" t="n">
+        <f aca="false">Netzplan!I10</f>
+        <v>0.75</v>
+      </c>
+      <c r="J10" s="44" t="n">
+        <f aca="false">ROUND(G10/(H10*I10),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="45" t="n">
         <f aca="false">SUM(L10:BM10)</f>
-        <v>2</v>
-      </c>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="46"/>
-      <c r="AB10" s="46"/>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="46"/>
-      <c r="AH10" s="45"/>
-      <c r="AI10" s="45"/>
-      <c r="AJ10" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK10" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="46"/>
-      <c r="AM10" s="46"/>
-      <c r="AN10" s="46"/>
-      <c r="AO10" s="46"/>
-      <c r="AP10" s="46"/>
-      <c r="AQ10" s="46"/>
-      <c r="AR10" s="46"/>
-      <c r="AS10" s="46"/>
-      <c r="AT10" s="46"/>
-      <c r="AU10" s="46"/>
-      <c r="AV10" s="46"/>
-      <c r="AW10" s="46"/>
-      <c r="AX10" s="46"/>
-      <c r="AY10" s="47"/>
-      <c r="AZ10" s="46"/>
-      <c r="BA10" s="46"/>
-      <c r="BB10" s="46"/>
-      <c r="BC10" s="46"/>
-      <c r="BD10" s="46"/>
-      <c r="BE10" s="46"/>
-      <c r="BF10" s="47"/>
-      <c r="BG10" s="46"/>
-      <c r="BH10" s="46"/>
-      <c r="BI10" s="46"/>
-      <c r="BJ10" s="46"/>
-      <c r="BK10" s="46"/>
-      <c r="BL10" s="47"/>
-      <c r="BM10" s="48"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="47"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
+      <c r="AG10" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="50"/>
+      <c r="AJ10" s="47"/>
+      <c r="AK10" s="47"/>
+      <c r="AL10" s="47"/>
+      <c r="AM10" s="47"/>
+      <c r="AN10" s="47"/>
+      <c r="AO10" s="47"/>
+      <c r="AP10" s="47"/>
+      <c r="AQ10" s="47"/>
+      <c r="AR10" s="47"/>
+      <c r="AS10" s="47"/>
+      <c r="AT10" s="47"/>
+      <c r="AU10" s="47"/>
+      <c r="AV10" s="47"/>
+      <c r="AW10" s="47"/>
+      <c r="AX10" s="47"/>
+      <c r="AY10" s="48"/>
+      <c r="AZ10" s="47"/>
+      <c r="BA10" s="47"/>
+      <c r="BB10" s="47"/>
+      <c r="BC10" s="47"/>
+      <c r="BD10" s="47"/>
+      <c r="BE10" s="47"/>
+      <c r="BF10" s="48"/>
+      <c r="BG10" s="47"/>
+      <c r="BH10" s="47"/>
+      <c r="BI10" s="47"/>
+      <c r="BJ10" s="47"/>
+      <c r="BK10" s="47"/>
+      <c r="BL10" s="48"/>
+      <c r="BM10" s="49"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
@@ -5683,86 +5550,84 @@
       <c r="F11" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="49" t="n">
+      <c r="G11" s="51" t="n">
         <f aca="false">[1]Netzplan!G11</f>
         <v>2</v>
       </c>
-      <c r="H11" s="49" t="str">
-        <f aca="false">[1]Netzplan!H11</f>
-        <v>1</v>
+      <c r="H11" s="31" t="str">
+        <f aca="false">Netzplan!H11</f>
+        <v>2</v>
       </c>
       <c r="I11" s="28" t="n">
-        <f aca="false">[1]Netzplan!I11</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="43" t="n">
-        <f aca="false">[1]Netzplan!J11</f>
-        <v>2</v>
-      </c>
-      <c r="K11" s="44" t="n">
+        <f aca="false">Netzplan!I11</f>
+        <v>0.75</v>
+      </c>
+      <c r="J11" s="44" t="n">
+        <f aca="false">ROUND(G11/(H11*I11),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="45" t="n">
         <f aca="false">SUM(L11:BM11)</f>
-        <v>2</v>
-      </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="46"/>
-      <c r="AB11" s="46"/>
-      <c r="AC11" s="46"/>
-      <c r="AD11" s="46"/>
-      <c r="AE11" s="46"/>
-      <c r="AF11" s="46"/>
-      <c r="AG11" s="46"/>
-      <c r="AH11" s="46"/>
-      <c r="AI11" s="50"/>
-      <c r="AJ11" s="45"/>
-      <c r="AK11" s="45"/>
-      <c r="AL11" s="46"/>
-      <c r="AM11" s="46"/>
-      <c r="AN11" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO11" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP11" s="46"/>
-      <c r="AQ11" s="46"/>
-      <c r="AR11" s="46"/>
-      <c r="AS11" s="46"/>
-      <c r="AT11" s="46"/>
-      <c r="AU11" s="46"/>
-      <c r="AV11" s="46"/>
-      <c r="AW11" s="46"/>
-      <c r="AX11" s="46"/>
-      <c r="AY11" s="47"/>
-      <c r="AZ11" s="46"/>
-      <c r="BA11" s="46"/>
-      <c r="BB11" s="46"/>
-      <c r="BC11" s="46"/>
-      <c r="BD11" s="46"/>
-      <c r="BE11" s="46"/>
-      <c r="BF11" s="47"/>
-      <c r="BG11" s="46"/>
-      <c r="BH11" s="46"/>
-      <c r="BI11" s="46"/>
-      <c r="BJ11" s="46"/>
-      <c r="BK11" s="46"/>
-      <c r="BL11" s="47"/>
-      <c r="BM11" s="48"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="47"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
+      <c r="AE11" s="47"/>
+      <c r="AF11" s="47"/>
+      <c r="AG11" s="47"/>
+      <c r="AH11" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="52"/>
+      <c r="AJ11" s="50"/>
+      <c r="AK11" s="50"/>
+      <c r="AL11" s="47"/>
+      <c r="AM11" s="47"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="47"/>
+      <c r="AP11" s="47"/>
+      <c r="AQ11" s="47"/>
+      <c r="AR11" s="47"/>
+      <c r="AS11" s="47"/>
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="47"/>
+      <c r="AW11" s="47"/>
+      <c r="AX11" s="47"/>
+      <c r="AY11" s="48"/>
+      <c r="AZ11" s="47"/>
+      <c r="BA11" s="47"/>
+      <c r="BB11" s="47"/>
+      <c r="BC11" s="47"/>
+      <c r="BD11" s="47"/>
+      <c r="BE11" s="47"/>
+      <c r="BF11" s="48"/>
+      <c r="BG11" s="47"/>
+      <c r="BH11" s="47"/>
+      <c r="BI11" s="47"/>
+      <c r="BJ11" s="47"/>
+      <c r="BK11" s="47"/>
+      <c r="BL11" s="48"/>
+      <c r="BM11" s="49"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
@@ -5777,97 +5642,120 @@
       <c r="F12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="49" t="n">
+      <c r="G12" s="51" t="n">
         <f aca="false">[1]Netzplan!G12</f>
         <v>10</v>
       </c>
-      <c r="H12" s="49" t="str">
-        <f aca="false">[1]Netzplan!H12</f>
+      <c r="H12" s="31" t="str">
+        <f aca="false">Netzplan!H12</f>
         <v>1</v>
       </c>
       <c r="I12" s="28" t="n">
-        <f aca="false">[1]Netzplan!I12</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="43" t="n">
-        <f aca="false">[1]Netzplan!J12</f>
-        <v>10</v>
-      </c>
-      <c r="K12" s="44" t="n">
+        <f aca="false">Netzplan!I12</f>
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="44" t="n">
+        <f aca="false">ROUND(G12/(H12*I12),0)</f>
+        <v>20</v>
+      </c>
+      <c r="K12" s="45" t="n">
         <f aca="false">SUM(L12:BM12)</f>
-        <v>10</v>
-      </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="46"/>
-      <c r="W12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="X12" s="46"/>
-      <c r="Y12" s="46"/>
-      <c r="Z12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="46"/>
-      <c r="AF12" s="46"/>
-      <c r="AG12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="45"/>
-      <c r="AL12" s="46"/>
-      <c r="AM12" s="46"/>
-      <c r="AN12" s="45"/>
-      <c r="AO12" s="45"/>
-      <c r="AS12" s="46"/>
-      <c r="AT12" s="46"/>
-      <c r="AU12" s="45"/>
-      <c r="AV12" s="45"/>
-      <c r="AW12" s="45"/>
-      <c r="AX12" s="45"/>
-      <c r="AY12" s="47"/>
-      <c r="AZ12" s="46"/>
-      <c r="BA12" s="46"/>
-      <c r="BB12" s="46"/>
-      <c r="BC12" s="46"/>
-      <c r="BD12" s="46"/>
-      <c r="BE12" s="46"/>
-      <c r="BF12" s="47"/>
-      <c r="BG12" s="46"/>
-      <c r="BH12" s="46"/>
-      <c r="BI12" s="50"/>
-      <c r="BJ12" s="46"/>
-      <c r="BK12" s="46"/>
-      <c r="BL12" s="47"/>
-      <c r="BM12" s="48"/>
+        <v>20</v>
+      </c>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="47"/>
+      <c r="AM12" s="47"/>
+      <c r="AN12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="47"/>
+      <c r="AT12" s="47"/>
+      <c r="AU12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="48"/>
+      <c r="AZ12" s="47"/>
+      <c r="BA12" s="47"/>
+      <c r="BB12" s="47"/>
+      <c r="BC12" s="47"/>
+      <c r="BD12" s="47"/>
+      <c r="BE12" s="47"/>
+      <c r="BF12" s="48"/>
+      <c r="BG12" s="47"/>
+      <c r="BH12" s="47"/>
+      <c r="BI12" s="52"/>
+      <c r="BJ12" s="47"/>
+      <c r="BK12" s="47"/>
+      <c r="BL12" s="48"/>
+      <c r="BM12" s="49"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
@@ -5884,86 +5772,84 @@
       <c r="F13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="49" t="n">
+      <c r="G13" s="51" t="n">
         <f aca="false">[1]Netzplan!G13</f>
         <v>3</v>
       </c>
-      <c r="H13" s="49" t="str">
-        <f aca="false">[1]Netzplan!H13</f>
-        <v>1</v>
+      <c r="H13" s="31" t="str">
+        <f aca="false">Netzplan!H13</f>
+        <v>2</v>
       </c>
       <c r="I13" s="28" t="n">
-        <f aca="false">[1]Netzplan!I13</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="43" t="n">
-        <f aca="false">[1]Netzplan!J13</f>
-        <v>3</v>
-      </c>
-      <c r="K13" s="44" t="n">
+        <f aca="false">Netzplan!I13</f>
+        <v>0.75</v>
+      </c>
+      <c r="J13" s="44" t="n">
+        <f aca="false">ROUND(G13/(H13*I13),0)</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="45" t="n">
         <f aca="false">SUM(L13:BM13)</f>
-        <v>3</v>
-      </c>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="46"/>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="46"/>
-      <c r="AB13" s="46"/>
-      <c r="AC13" s="46"/>
-      <c r="AD13" s="46"/>
-      <c r="AE13" s="46"/>
-      <c r="AF13" s="46"/>
-      <c r="AG13" s="46"/>
-      <c r="AH13" s="46"/>
-      <c r="AI13" s="46"/>
-      <c r="AJ13" s="46"/>
-      <c r="AK13" s="50"/>
-      <c r="AL13" s="46"/>
-      <c r="AM13" s="46"/>
-      <c r="AN13" s="45"/>
-      <c r="AO13" s="45"/>
-      <c r="AP13" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR13" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS13" s="46"/>
-      <c r="AT13" s="46"/>
-      <c r="AU13" s="46"/>
-      <c r="AV13" s="46"/>
-      <c r="AW13" s="46"/>
-      <c r="AX13" s="46"/>
-      <c r="AY13" s="47"/>
-      <c r="AZ13" s="46"/>
-      <c r="BA13" s="46"/>
-      <c r="BB13" s="46"/>
-      <c r="BC13" s="46"/>
-      <c r="BD13" s="46"/>
-      <c r="BE13" s="46"/>
-      <c r="BF13" s="47"/>
-      <c r="BG13" s="46"/>
-      <c r="BH13" s="46"/>
-      <c r="BI13" s="46"/>
-      <c r="BJ13" s="46"/>
-      <c r="BK13" s="46"/>
-      <c r="BL13" s="47"/>
-      <c r="BM13" s="48"/>
+        <v>2</v>
+      </c>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
+      <c r="AD13" s="47"/>
+      <c r="AE13" s="47"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="47"/>
+      <c r="AH13" s="47"/>
+      <c r="AI13" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="52"/>
+      <c r="AL13" s="47"/>
+      <c r="AM13" s="47"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="50"/>
+      <c r="AP13" s="50"/>
+      <c r="AQ13" s="50"/>
+      <c r="AR13" s="50"/>
+      <c r="AS13" s="47"/>
+      <c r="AT13" s="47"/>
+      <c r="AU13" s="47"/>
+      <c r="AV13" s="47"/>
+      <c r="AW13" s="47"/>
+      <c r="AX13" s="47"/>
+      <c r="AY13" s="48"/>
+      <c r="AZ13" s="47"/>
+      <c r="BA13" s="47"/>
+      <c r="BB13" s="47"/>
+      <c r="BC13" s="47"/>
+      <c r="BD13" s="47"/>
+      <c r="BE13" s="47"/>
+      <c r="BF13" s="48"/>
+      <c r="BG13" s="47"/>
+      <c r="BH13" s="47"/>
+      <c r="BI13" s="47"/>
+      <c r="BJ13" s="47"/>
+      <c r="BK13" s="47"/>
+      <c r="BL13" s="48"/>
+      <c r="BM13" s="49"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
@@ -5980,86 +5866,84 @@
       <c r="F14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="49" t="n">
+      <c r="G14" s="51" t="n">
         <f aca="false">[1]Netzplan!G14</f>
         <v>3</v>
       </c>
-      <c r="H14" s="49" t="str">
-        <f aca="false">[1]Netzplan!H14</f>
-        <v>1</v>
+      <c r="H14" s="31" t="str">
+        <f aca="false">Netzplan!H14</f>
+        <v>2</v>
       </c>
       <c r="I14" s="28" t="n">
-        <f aca="false">[1]Netzplan!I14</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="43" t="n">
-        <f aca="false">[1]Netzplan!J14</f>
-        <v>3</v>
-      </c>
-      <c r="K14" s="44" t="n">
+        <f aca="false">Netzplan!I14</f>
+        <v>0.75</v>
+      </c>
+      <c r="J14" s="44" t="n">
+        <f aca="false">ROUND(G14/(H14*I14),0)</f>
+        <v>2</v>
+      </c>
+      <c r="K14" s="45" t="n">
         <f aca="false">SUM(L14:BM14)</f>
-        <v>3</v>
-      </c>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="46"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="46"/>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46"/>
-      <c r="AE14" s="46"/>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="46"/>
-      <c r="AI14" s="46"/>
-      <c r="AJ14" s="46"/>
-      <c r="AK14" s="46"/>
-      <c r="AL14" s="46"/>
-      <c r="AM14" s="46"/>
-      <c r="AN14" s="46"/>
-      <c r="AO14" s="46"/>
-      <c r="AP14" s="50"/>
-      <c r="AQ14" s="45"/>
-      <c r="AR14" s="45"/>
-      <c r="AS14" s="46"/>
-      <c r="AT14" s="46"/>
-      <c r="AU14" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV14" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW14" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX14" s="46"/>
-      <c r="AY14" s="47"/>
-      <c r="AZ14" s="46"/>
-      <c r="BA14" s="46"/>
-      <c r="BB14" s="46"/>
-      <c r="BC14" s="46"/>
-      <c r="BD14" s="46"/>
-      <c r="BE14" s="46"/>
-      <c r="BF14" s="47"/>
-      <c r="BG14" s="46"/>
-      <c r="BH14" s="46"/>
-      <c r="BI14" s="46"/>
-      <c r="BJ14" s="46"/>
-      <c r="BK14" s="46"/>
-      <c r="BL14" s="47"/>
-      <c r="BM14" s="48"/>
+        <v>2</v>
+      </c>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="47"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="47"/>
+      <c r="AD14" s="47"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="47"/>
+      <c r="AH14" s="47"/>
+      <c r="AI14" s="47"/>
+      <c r="AJ14" s="47"/>
+      <c r="AK14" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="47"/>
+      <c r="AM14" s="47"/>
+      <c r="AN14" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="47"/>
+      <c r="AP14" s="52"/>
+      <c r="AQ14" s="50"/>
+      <c r="AR14" s="50"/>
+      <c r="AS14" s="47"/>
+      <c r="AT14" s="47"/>
+      <c r="AU14" s="50"/>
+      <c r="AV14" s="50"/>
+      <c r="AW14" s="50"/>
+      <c r="AX14" s="47"/>
+      <c r="AY14" s="48"/>
+      <c r="AZ14" s="47"/>
+      <c r="BA14" s="47"/>
+      <c r="BB14" s="47"/>
+      <c r="BC14" s="47"/>
+      <c r="BD14" s="47"/>
+      <c r="BE14" s="47"/>
+      <c r="BF14" s="48"/>
+      <c r="BG14" s="47"/>
+      <c r="BH14" s="47"/>
+      <c r="BI14" s="47"/>
+      <c r="BJ14" s="47"/>
+      <c r="BK14" s="47"/>
+      <c r="BL14" s="48"/>
+      <c r="BM14" s="49"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
@@ -6076,82 +5960,82 @@
       <c r="F15" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="49" t="n">
+      <c r="G15" s="51" t="n">
         <f aca="false">[1]Netzplan!G15</f>
         <v>1</v>
       </c>
-      <c r="H15" s="49" t="str">
-        <f aca="false">[1]Netzplan!H15</f>
-        <v>1</v>
+      <c r="H15" s="31" t="str">
+        <f aca="false">Netzplan!H15</f>
+        <v>2</v>
       </c>
       <c r="I15" s="28" t="n">
-        <f aca="false">[1]Netzplan!I15</f>
-        <v>1</v>
-      </c>
-      <c r="J15" s="43" t="n">
-        <f aca="false">[1]Netzplan!J15</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="44" t="n">
+        <f aca="false">Netzplan!I15</f>
+        <v>0.75</v>
+      </c>
+      <c r="J15" s="44" t="n">
+        <f aca="false">ROUND(G15/(H15*I15),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="45" t="n">
         <f aca="false">SUM(L15:BM15)</f>
         <v>1</v>
       </c>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
-      <c r="V15" s="46"/>
-      <c r="W15" s="46"/>
-      <c r="X15" s="46"/>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="46"/>
-      <c r="AA15" s="46"/>
-      <c r="AB15" s="46"/>
-      <c r="AC15" s="46"/>
-      <c r="AD15" s="46"/>
-      <c r="AE15" s="46"/>
-      <c r="AF15" s="46"/>
-      <c r="AG15" s="46"/>
-      <c r="AH15" s="46"/>
-      <c r="AI15" s="46"/>
-      <c r="AJ15" s="46"/>
-      <c r="AK15" s="46"/>
-      <c r="AL15" s="46"/>
-      <c r="AM15" s="46"/>
-      <c r="AN15" s="46"/>
-      <c r="AO15" s="46"/>
-      <c r="AP15" s="46"/>
-      <c r="AQ15" s="46"/>
-      <c r="AR15" s="46"/>
-      <c r="AS15" s="46"/>
-      <c r="AT15" s="46"/>
-      <c r="AU15" s="46"/>
-      <c r="AV15" s="45"/>
-      <c r="AW15" s="46"/>
-      <c r="AX15" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY15" s="47"/>
-      <c r="AZ15" s="46"/>
-      <c r="BA15" s="46"/>
-      <c r="BB15" s="46"/>
-      <c r="BC15" s="46"/>
-      <c r="BD15" s="46"/>
-      <c r="BE15" s="46"/>
-      <c r="BF15" s="47"/>
-      <c r="BG15" s="46"/>
-      <c r="BH15" s="46"/>
-      <c r="BI15" s="46"/>
-      <c r="BJ15" s="46"/>
-      <c r="BK15" s="46"/>
-      <c r="BL15" s="47"/>
-      <c r="BM15" s="48"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="47"/>
+      <c r="AF15" s="47"/>
+      <c r="AG15" s="47"/>
+      <c r="AH15" s="47"/>
+      <c r="AI15" s="47"/>
+      <c r="AJ15" s="47"/>
+      <c r="AK15" s="47"/>
+      <c r="AL15" s="47"/>
+      <c r="AM15" s="47"/>
+      <c r="AN15" s="47"/>
+      <c r="AO15" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="47"/>
+      <c r="AQ15" s="47"/>
+      <c r="AR15" s="47"/>
+      <c r="AS15" s="47"/>
+      <c r="AT15" s="47"/>
+      <c r="AU15" s="47"/>
+      <c r="AV15" s="50"/>
+      <c r="AW15" s="47"/>
+      <c r="AX15" s="47"/>
+      <c r="AY15" s="48"/>
+      <c r="AZ15" s="47"/>
+      <c r="BA15" s="47"/>
+      <c r="BB15" s="47"/>
+      <c r="BC15" s="47"/>
+      <c r="BD15" s="47"/>
+      <c r="BE15" s="47"/>
+      <c r="BF15" s="48"/>
+      <c r="BG15" s="47"/>
+      <c r="BH15" s="47"/>
+      <c r="BI15" s="47"/>
+      <c r="BJ15" s="47"/>
+      <c r="BK15" s="47"/>
+      <c r="BL15" s="48"/>
+      <c r="BM15" s="49"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
@@ -6168,90 +6052,86 @@
       <c r="F16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="49" t="n">
+      <c r="G16" s="51" t="n">
         <f aca="false">[1]Netzplan!G16</f>
         <v>5</v>
       </c>
-      <c r="H16" s="49" t="str">
-        <f aca="false">[1]Netzplan!H16</f>
-        <v>1</v>
+      <c r="H16" s="31" t="str">
+        <f aca="false">Netzplan!H16</f>
+        <v>2</v>
       </c>
       <c r="I16" s="28" t="n">
-        <f aca="false">[1]Netzplan!I16</f>
-        <v>1</v>
-      </c>
-      <c r="J16" s="43" t="n">
-        <f aca="false">[1]Netzplan!J16</f>
-        <v>5</v>
-      </c>
-      <c r="K16" s="44" t="n">
+        <f aca="false">Netzplan!I16</f>
+        <v>0.75</v>
+      </c>
+      <c r="J16" s="44" t="n">
+        <f aca="false">ROUND(G16/(H16*I16),0)</f>
+        <v>3</v>
+      </c>
+      <c r="K16" s="45" t="n">
         <f aca="false">SUM(L16:BM16)</f>
-        <v>5</v>
-      </c>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="46"/>
-      <c r="W16" s="46"/>
-      <c r="X16" s="46"/>
-      <c r="Y16" s="46"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="46"/>
-      <c r="AB16" s="46"/>
-      <c r="AC16" s="46"/>
-      <c r="AD16" s="46"/>
-      <c r="AE16" s="46"/>
-      <c r="AF16" s="46"/>
-      <c r="AG16" s="46"/>
-      <c r="AH16" s="46"/>
-      <c r="AI16" s="46"/>
-      <c r="AJ16" s="46"/>
-      <c r="AK16" s="46"/>
-      <c r="AL16" s="46"/>
-      <c r="AM16" s="46"/>
-      <c r="AN16" s="46"/>
-      <c r="AO16" s="46"/>
-      <c r="AP16" s="46"/>
-      <c r="AQ16" s="46"/>
-      <c r="AR16" s="46"/>
-      <c r="AS16" s="46"/>
-      <c r="AT16" s="46"/>
-      <c r="AU16" s="46"/>
-      <c r="AV16" s="46"/>
-      <c r="AW16" s="45"/>
-      <c r="AX16" s="45"/>
-      <c r="AY16" s="47"/>
-      <c r="AZ16" s="46"/>
-      <c r="BA16" s="46"/>
-      <c r="BB16" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC16" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD16" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE16" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF16" s="47"/>
-      <c r="BG16" s="46"/>
-      <c r="BH16" s="46"/>
-      <c r="BI16" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ16" s="50"/>
-      <c r="BK16" s="46"/>
-      <c r="BL16" s="47"/>
-      <c r="BM16" s="48"/>
+        <v>3</v>
+      </c>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="47"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="47"/>
+      <c r="AF16" s="47"/>
+      <c r="AG16" s="47"/>
+      <c r="AH16" s="47"/>
+      <c r="AI16" s="47"/>
+      <c r="AJ16" s="47"/>
+      <c r="AK16" s="47"/>
+      <c r="AL16" s="47"/>
+      <c r="AM16" s="47"/>
+      <c r="AN16" s="47"/>
+      <c r="AO16" s="47"/>
+      <c r="AP16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="47"/>
+      <c r="AT16" s="47"/>
+      <c r="AU16" s="47"/>
+      <c r="AV16" s="47"/>
+      <c r="AW16" s="50"/>
+      <c r="AX16" s="50"/>
+      <c r="AY16" s="48"/>
+      <c r="AZ16" s="47"/>
+      <c r="BA16" s="47"/>
+      <c r="BB16" s="50"/>
+      <c r="BC16" s="50"/>
+      <c r="BD16" s="50"/>
+      <c r="BE16" s="47"/>
+      <c r="BF16" s="48"/>
+      <c r="BG16" s="47"/>
+      <c r="BH16" s="47"/>
+      <c r="BI16" s="47"/>
+      <c r="BJ16" s="52"/>
+      <c r="BK16" s="47"/>
+      <c r="BL16" s="48"/>
+      <c r="BM16" s="49"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
@@ -6266,82 +6146,82 @@
         <v>59</v>
       </c>
       <c r="F17" s="38"/>
-      <c r="G17" s="51" t="n">
+      <c r="G17" s="53" t="n">
         <f aca="false">[1]Netzplan!G17</f>
         <v>1</v>
       </c>
-      <c r="H17" s="51" t="str">
-        <f aca="false">[1]Netzplan!H17</f>
-        <v>1</v>
-      </c>
-      <c r="I17" s="40" t="n">
-        <f aca="false">[1]Netzplan!I17</f>
-        <v>1</v>
-      </c>
-      <c r="J17" s="52" t="n">
-        <f aca="false">[1]Netzplan!J17</f>
-        <v>1</v>
-      </c>
-      <c r="K17" s="44" t="n">
+      <c r="H17" s="31" t="str">
+        <f aca="false">Netzplan!H17</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="28" t="n">
+        <f aca="false">Netzplan!I17</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="44" t="n">
+        <f aca="false">ROUND(G17/(H17*I17),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="45" t="n">
         <f aca="false">SUM(L17:BM17)</f>
         <v>1</v>
       </c>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="53"/>
-      <c r="Z17" s="53"/>
-      <c r="AA17" s="53"/>
-      <c r="AB17" s="53"/>
-      <c r="AC17" s="53"/>
-      <c r="AD17" s="53"/>
-      <c r="AE17" s="53"/>
-      <c r="AF17" s="53"/>
-      <c r="AG17" s="53"/>
-      <c r="AH17" s="53"/>
-      <c r="AI17" s="53"/>
-      <c r="AJ17" s="53"/>
-      <c r="AK17" s="53"/>
-      <c r="AL17" s="53"/>
-      <c r="AM17" s="53"/>
-      <c r="AN17" s="53"/>
-      <c r="AO17" s="53"/>
-      <c r="AP17" s="53"/>
-      <c r="AQ17" s="53"/>
-      <c r="AR17" s="53"/>
-      <c r="AS17" s="53"/>
-      <c r="AT17" s="53"/>
-      <c r="AU17" s="53"/>
-      <c r="AV17" s="53"/>
-      <c r="AW17" s="53"/>
-      <c r="AX17" s="53"/>
-      <c r="AY17" s="54"/>
-      <c r="AZ17" s="53"/>
-      <c r="BA17" s="53"/>
-      <c r="BB17" s="53"/>
-      <c r="BC17" s="45"/>
-      <c r="BD17" s="53"/>
-      <c r="BE17" s="53"/>
-      <c r="BF17" s="54"/>
-      <c r="BG17" s="53"/>
-      <c r="BH17" s="53"/>
-      <c r="BI17" s="53"/>
-      <c r="BJ17" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK17" s="53"/>
-      <c r="BL17" s="54"/>
-      <c r="BM17" s="55"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="54"/>
+      <c r="AA17" s="54"/>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="54"/>
+      <c r="AD17" s="54"/>
+      <c r="AE17" s="54"/>
+      <c r="AF17" s="54"/>
+      <c r="AG17" s="54"/>
+      <c r="AH17" s="54"/>
+      <c r="AI17" s="54"/>
+      <c r="AJ17" s="54"/>
+      <c r="AK17" s="54"/>
+      <c r="AL17" s="54"/>
+      <c r="AM17" s="54"/>
+      <c r="AN17" s="54"/>
+      <c r="AO17" s="54"/>
+      <c r="AP17" s="54"/>
+      <c r="AQ17" s="54"/>
+      <c r="AR17" s="54"/>
+      <c r="AS17" s="54"/>
+      <c r="AT17" s="54"/>
+      <c r="AU17" s="54"/>
+      <c r="AV17" s="54"/>
+      <c r="AW17" s="54"/>
+      <c r="AX17" s="54"/>
+      <c r="AY17" s="55"/>
+      <c r="AZ17" s="54"/>
+      <c r="BA17" s="54"/>
+      <c r="BB17" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC17" s="50"/>
+      <c r="BD17" s="54"/>
+      <c r="BE17" s="54"/>
+      <c r="BF17" s="55"/>
+      <c r="BG17" s="54"/>
+      <c r="BH17" s="54"/>
+      <c r="BI17" s="54"/>
+      <c r="BJ17" s="54"/>
+      <c r="BK17" s="54"/>
+      <c r="BL17" s="55"/>
+      <c r="BM17" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -6363,12 +6243,12 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
   </mergeCells>
-  <conditionalFormatting sqref="AV15:BM15 L10:AH11 BF12:BH12 BJ12:BM12 BC17:BM17 BK16:BM16 L13:AJ13 L14:AO14 L15:AT15 L16:AU16 L17:BA17 AI10:BM10 AJ11:BM11 L1:BM6 L8:BM9 L7:R7 T7:BM7 AS12:BA12 L12:AO12 AL13:BM13 AQ14:BM14 AW16:BI16">
+  <conditionalFormatting sqref="AV15:BM15 L10:AH12 BF12:BH12 BJ12:BM12 BK16:BM16 L13:AJ13 L14:AO14 L15:AT15 L17:BM17 AI10:BM10 AJ11:BM11 AL13:BM13 AQ14:BM14 AW16:BI16 L16:AO16 AQ16:AU16 L1:BM9 AI12:BA12">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>IF(OR(WEEKDAY(L$1)=7,WEEKDAY(L$1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:BM11 L12:AO13 AS12:BM13 AP13:AR13 L14:BM17">
+  <conditionalFormatting sqref="L2:BM17">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Gantt in Online_Shop.Projekt.FIAE_B.xlsx: Ressourcen in Gantt
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
+++ b/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="60">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -207,23 +207,21 @@
   <si>
     <t xml:space="preserve">1.3.1, 1.2.8</t>
   </si>
-  <si>
-    <t xml:space="preserve">Ressourcen</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00\ %"/>
     <numFmt numFmtId="168" formatCode="0\ %"/>
     <numFmt numFmtId="169" formatCode="General"/>
+    <numFmt numFmtId="170" formatCode="0\ %"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -263,6 +261,27 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF127622"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF55308D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF8000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -411,7 +430,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -584,7 +603,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="70" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,7 +619,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -713,7 +740,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF127622"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -748,7 +775,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFBF00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF969696"/>
@@ -758,7 +785,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF55308D"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -4466,12 +4493,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BN17"/>
+  <dimension ref="A1:BP17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="11" ySplit="0" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="BN1" activeCellId="0" sqref="BN1"/>
+      <selection pane="topRight" activeCell="BO5" activeCellId="0" sqref="BO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -4482,7 +4509,9 @@
     <col collapsed="true" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="11" style="0" width="3.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="12" style="0" width="3.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4676,7 +4705,13 @@
         <v>44568</v>
       </c>
       <c r="BN1" s="43" t="s">
-        <v>60</v>
+        <v>7</v>
+      </c>
+      <c r="BO1" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="BP1" s="45" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4704,78 +4739,83 @@
         <f aca="false">Netzplan!I2</f>
         <v>1</v>
       </c>
-      <c r="J2" s="44" t="n">
+      <c r="J2" s="46" t="n">
         <f aca="false">ROUND(G2/(H2*I2),0)</f>
         <v>5</v>
       </c>
-      <c r="K2" s="45" t="n">
+      <c r="K2" s="47" t="n">
         <f aca="false">SUM(L2:BM2)</f>
         <v>5</v>
       </c>
-      <c r="L2" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="47"/>
-      <c r="AD2" s="47"/>
-      <c r="AE2" s="47"/>
-      <c r="AF2" s="47"/>
-      <c r="AG2" s="47"/>
-      <c r="AH2" s="47"/>
-      <c r="AI2" s="47"/>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
-      <c r="AL2" s="47"/>
-      <c r="AM2" s="47"/>
-      <c r="AN2" s="47"/>
-      <c r="AO2" s="47"/>
-      <c r="AP2" s="47"/>
-      <c r="AQ2" s="47"/>
-      <c r="AR2" s="47"/>
-      <c r="AS2" s="47"/>
-      <c r="AT2" s="47"/>
-      <c r="AU2" s="47"/>
-      <c r="AV2" s="47"/>
-      <c r="AW2" s="47"/>
-      <c r="AX2" s="47"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="47"/>
-      <c r="BA2" s="47"/>
-      <c r="BB2" s="47"/>
-      <c r="BC2" s="47"/>
-      <c r="BD2" s="47"/>
-      <c r="BE2" s="47"/>
-      <c r="BF2" s="48"/>
-      <c r="BG2" s="47"/>
-      <c r="BH2" s="47"/>
-      <c r="BI2" s="47"/>
-      <c r="BJ2" s="47"/>
-      <c r="BK2" s="47"/>
-      <c r="BL2" s="48"/>
-      <c r="BM2" s="49"/>
+      <c r="L2" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="49"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="49"/>
+      <c r="AU2" s="49"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="50"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="49"/>
+      <c r="BB2" s="49"/>
+      <c r="BC2" s="49"/>
+      <c r="BD2" s="49"/>
+      <c r="BE2" s="49"/>
+      <c r="BF2" s="50"/>
+      <c r="BG2" s="49"/>
+      <c r="BH2" s="49"/>
+      <c r="BI2" s="49"/>
+      <c r="BJ2" s="49"/>
+      <c r="BK2" s="49"/>
+      <c r="BL2" s="50"/>
+      <c r="BM2" s="51"/>
+      <c r="BN2" s="43"/>
+      <c r="BO2" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
@@ -4804,70 +4844,75 @@
         <f aca="false">Netzplan!I3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="44" t="n">
+      <c r="J3" s="46" t="n">
         <f aca="false">ROUND(G3/(H3*I3),0)</f>
         <v>1</v>
       </c>
-      <c r="K3" s="45" t="n">
+      <c r="K3" s="47" t="n">
         <f aca="false">SUM(L3:BM3)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47"/>
-      <c r="Z3" s="47"/>
-      <c r="AA3" s="47"/>
-      <c r="AB3" s="47"/>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="47"/>
-      <c r="AI3" s="47"/>
-      <c r="AJ3" s="47"/>
-      <c r="AK3" s="47"/>
-      <c r="AL3" s="47"/>
-      <c r="AM3" s="47"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="47"/>
-      <c r="AP3" s="47"/>
-      <c r="AQ3" s="47"/>
-      <c r="AR3" s="47"/>
-      <c r="AS3" s="47"/>
-      <c r="AT3" s="47"/>
-      <c r="AU3" s="47"/>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="47"/>
-      <c r="AX3" s="47"/>
-      <c r="AY3" s="48"/>
-      <c r="AZ3" s="47"/>
-      <c r="BA3" s="47"/>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="47"/>
-      <c r="BD3" s="47"/>
-      <c r="BE3" s="47"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="47"/>
-      <c r="BH3" s="47"/>
-      <c r="BI3" s="47"/>
-      <c r="BJ3" s="47"/>
-      <c r="BK3" s="47"/>
-      <c r="BL3" s="48"/>
-      <c r="BM3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="AQ3" s="49"/>
+      <c r="AR3" s="49"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="49"/>
+      <c r="AU3" s="49"/>
+      <c r="AV3" s="49"/>
+      <c r="AW3" s="49"/>
+      <c r="AX3" s="49"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="49"/>
+      <c r="BA3" s="49"/>
+      <c r="BB3" s="49"/>
+      <c r="BC3" s="49"/>
+      <c r="BD3" s="49"/>
+      <c r="BE3" s="49"/>
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="49"/>
+      <c r="BH3" s="49"/>
+      <c r="BI3" s="49"/>
+      <c r="BJ3" s="49"/>
+      <c r="BK3" s="49"/>
+      <c r="BL3" s="50"/>
+      <c r="BM3" s="51"/>
+      <c r="BN3" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO3" s="44"/>
+      <c r="BP3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
@@ -4896,76 +4941,81 @@
         <f aca="false">Netzplan!I4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="44" t="n">
+      <c r="J4" s="46" t="n">
         <f aca="false">ROUND(G4/(H4*I4),0)</f>
         <v>4</v>
       </c>
-      <c r="K4" s="45" t="n">
+      <c r="K4" s="47" t="n">
         <f aca="false">SUM(L4:BM4)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="47"/>
-      <c r="AI4" s="47"/>
-      <c r="AJ4" s="47"/>
-      <c r="AK4" s="47"/>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="47"/>
-      <c r="AT4" s="47"/>
-      <c r="AU4" s="47"/>
-      <c r="AV4" s="47"/>
-      <c r="AW4" s="47"/>
-      <c r="AX4" s="47"/>
-      <c r="AY4" s="48"/>
-      <c r="AZ4" s="47"/>
-      <c r="BA4" s="47"/>
-      <c r="BB4" s="47"/>
-      <c r="BC4" s="47"/>
-      <c r="BD4" s="47"/>
-      <c r="BE4" s="47"/>
-      <c r="BF4" s="48"/>
-      <c r="BG4" s="47"/>
-      <c r="BH4" s="47"/>
-      <c r="BI4" s="47"/>
-      <c r="BJ4" s="47"/>
-      <c r="BK4" s="47"/>
-      <c r="BL4" s="48"/>
-      <c r="BM4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="49"/>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="49"/>
+      <c r="AH4" s="49"/>
+      <c r="AI4" s="49"/>
+      <c r="AJ4" s="49"/>
+      <c r="AK4" s="49"/>
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="49"/>
+      <c r="AT4" s="49"/>
+      <c r="AU4" s="49"/>
+      <c r="AV4" s="49"/>
+      <c r="AW4" s="49"/>
+      <c r="AX4" s="49"/>
+      <c r="AY4" s="50"/>
+      <c r="AZ4" s="49"/>
+      <c r="BA4" s="49"/>
+      <c r="BB4" s="49"/>
+      <c r="BC4" s="49"/>
+      <c r="BD4" s="49"/>
+      <c r="BE4" s="49"/>
+      <c r="BF4" s="50"/>
+      <c r="BG4" s="49"/>
+      <c r="BH4" s="49"/>
+      <c r="BI4" s="49"/>
+      <c r="BJ4" s="49"/>
+      <c r="BK4" s="49"/>
+      <c r="BL4" s="50"/>
+      <c r="BM4" s="51"/>
+      <c r="BN4" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="44"/>
+      <c r="BP4" s="45"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
@@ -4994,76 +5044,81 @@
         <f aca="false">Netzplan!I5</f>
         <v>1</v>
       </c>
-      <c r="J5" s="44" t="n">
+      <c r="J5" s="46" t="n">
         <f aca="false">ROUND(G5/(H5*I5),0)</f>
         <v>3</v>
       </c>
-      <c r="K5" s="45" t="n">
+      <c r="K5" s="47" t="n">
         <f aca="false">SUM(L5:BM5)</f>
         <v>3</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="47"/>
-      <c r="AG5" s="47"/>
-      <c r="AH5" s="47"/>
-      <c r="AI5" s="47"/>
-      <c r="AJ5" s="47"/>
-      <c r="AK5" s="47"/>
-      <c r="AL5" s="47"/>
-      <c r="AM5" s="47"/>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="47"/>
-      <c r="AP5" s="47"/>
-      <c r="AQ5" s="47"/>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="47"/>
-      <c r="AV5" s="47"/>
-      <c r="AW5" s="47"/>
-      <c r="AX5" s="47"/>
-      <c r="AY5" s="48"/>
-      <c r="AZ5" s="47"/>
-      <c r="BA5" s="47"/>
-      <c r="BB5" s="47"/>
-      <c r="BC5" s="47"/>
-      <c r="BD5" s="47"/>
-      <c r="BE5" s="47"/>
-      <c r="BF5" s="48"/>
-      <c r="BG5" s="47"/>
-      <c r="BH5" s="47"/>
-      <c r="BI5" s="47"/>
-      <c r="BJ5" s="47"/>
-      <c r="BK5" s="47"/>
-      <c r="BL5" s="48"/>
-      <c r="BM5" s="49"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="49"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="49"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="50"/>
+      <c r="AZ5" s="49"/>
+      <c r="BA5" s="49"/>
+      <c r="BB5" s="49"/>
+      <c r="BC5" s="49"/>
+      <c r="BD5" s="49"/>
+      <c r="BE5" s="49"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="49"/>
+      <c r="BH5" s="49"/>
+      <c r="BI5" s="49"/>
+      <c r="BJ5" s="49"/>
+      <c r="BK5" s="49"/>
+      <c r="BL5" s="50"/>
+      <c r="BM5" s="51"/>
+      <c r="BN5" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="44"/>
+      <c r="BP5" s="45"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>32</v>
       </c>
@@ -5090,78 +5145,85 @@
         <f aca="false">Netzplan!I6</f>
         <v>0.75</v>
       </c>
-      <c r="J6" s="44" t="n">
+      <c r="J6" s="46" t="n">
         <f aca="false">ROUND(G6/(H6*I6),0)</f>
         <v>5</v>
       </c>
-      <c r="K6" s="45" t="n">
+      <c r="K6" s="47" t="n">
         <f aca="false">SUM(L6:BM6)</f>
         <v>5</v>
       </c>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="50"/>
-      <c r="AE6" s="47"/>
-      <c r="AF6" s="47"/>
-      <c r="AG6" s="47"/>
-      <c r="AH6" s="47"/>
-      <c r="AI6" s="47"/>
-      <c r="AJ6" s="47"/>
-      <c r="AK6" s="47"/>
-      <c r="AL6" s="47"/>
-      <c r="AM6" s="47"/>
-      <c r="AN6" s="47"/>
-      <c r="AO6" s="47"/>
-      <c r="AP6" s="47"/>
-      <c r="AQ6" s="47"/>
-      <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
-      <c r="AT6" s="47"/>
-      <c r="AU6" s="47"/>
-      <c r="AV6" s="47"/>
-      <c r="AW6" s="47"/>
-      <c r="AX6" s="47"/>
-      <c r="AY6" s="48"/>
-      <c r="AZ6" s="47"/>
-      <c r="BA6" s="47"/>
-      <c r="BB6" s="47"/>
-      <c r="BC6" s="47"/>
-      <c r="BD6" s="47"/>
-      <c r="BE6" s="47"/>
-      <c r="BF6" s="48"/>
-      <c r="BG6" s="47"/>
-      <c r="BH6" s="47"/>
-      <c r="BI6" s="47"/>
-      <c r="BJ6" s="47"/>
-      <c r="BK6" s="47"/>
-      <c r="BL6" s="48"/>
-      <c r="BM6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="52"/>
+      <c r="AE6" s="49"/>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="49"/>
+      <c r="AH6" s="49"/>
+      <c r="AI6" s="49"/>
+      <c r="AJ6" s="49"/>
+      <c r="AK6" s="49"/>
+      <c r="AL6" s="49"/>
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="49"/>
+      <c r="AO6" s="49"/>
+      <c r="AP6" s="49"/>
+      <c r="AQ6" s="49"/>
+      <c r="AR6" s="49"/>
+      <c r="AS6" s="49"/>
+      <c r="AT6" s="49"/>
+      <c r="AU6" s="49"/>
+      <c r="AV6" s="49"/>
+      <c r="AW6" s="49"/>
+      <c r="AX6" s="49"/>
+      <c r="AY6" s="50"/>
+      <c r="AZ6" s="49"/>
+      <c r="BA6" s="49"/>
+      <c r="BB6" s="49"/>
+      <c r="BC6" s="49"/>
+      <c r="BD6" s="49"/>
+      <c r="BE6" s="49"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="49"/>
+      <c r="BH6" s="49"/>
+      <c r="BI6" s="49"/>
+      <c r="BJ6" s="49"/>
+      <c r="BK6" s="49"/>
+      <c r="BL6" s="50"/>
+      <c r="BM6" s="51"/>
+      <c r="BN6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO6" s="44"/>
+      <c r="BP6" s="45" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
@@ -5190,70 +5252,75 @@
         <f aca="false">Netzplan!I7</f>
         <v>1</v>
       </c>
-      <c r="J7" s="44" t="n">
+      <c r="J7" s="46" t="n">
         <f aca="false">ROUND(G7/(H7*I7),0)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="45" t="n">
+      <c r="K7" s="47" t="n">
         <f aca="false">SUM(L7:BM7)</f>
         <v>1</v>
       </c>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="47"/>
-      <c r="AE7" s="47"/>
-      <c r="AF7" s="47"/>
-      <c r="AG7" s="47"/>
-      <c r="AH7" s="47"/>
-      <c r="AI7" s="47"/>
-      <c r="AJ7" s="47"/>
-      <c r="AK7" s="47"/>
-      <c r="AL7" s="47"/>
-      <c r="AM7" s="47"/>
-      <c r="AN7" s="47"/>
-      <c r="AO7" s="47"/>
-      <c r="AP7" s="47"/>
-      <c r="AQ7" s="47"/>
-      <c r="AR7" s="47"/>
-      <c r="AS7" s="47"/>
-      <c r="AT7" s="47"/>
-      <c r="AU7" s="47"/>
-      <c r="AV7" s="47"/>
-      <c r="AW7" s="47"/>
-      <c r="AX7" s="47"/>
-      <c r="AY7" s="48"/>
-      <c r="AZ7" s="47"/>
-      <c r="BA7" s="47"/>
-      <c r="BB7" s="47"/>
-      <c r="BC7" s="47"/>
-      <c r="BD7" s="47"/>
-      <c r="BE7" s="47"/>
-      <c r="BF7" s="48"/>
-      <c r="BG7" s="47"/>
-      <c r="BH7" s="47"/>
-      <c r="BI7" s="47"/>
-      <c r="BJ7" s="47"/>
-      <c r="BK7" s="47"/>
-      <c r="BL7" s="48"/>
-      <c r="BM7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="49"/>
+      <c r="AB7" s="49"/>
+      <c r="AC7" s="49"/>
+      <c r="AD7" s="49"/>
+      <c r="AE7" s="49"/>
+      <c r="AF7" s="49"/>
+      <c r="AG7" s="49"/>
+      <c r="AH7" s="49"/>
+      <c r="AI7" s="49"/>
+      <c r="AJ7" s="49"/>
+      <c r="AK7" s="49"/>
+      <c r="AL7" s="49"/>
+      <c r="AM7" s="49"/>
+      <c r="AN7" s="49"/>
+      <c r="AO7" s="49"/>
+      <c r="AP7" s="49"/>
+      <c r="AQ7" s="49"/>
+      <c r="AR7" s="49"/>
+      <c r="AS7" s="49"/>
+      <c r="AT7" s="49"/>
+      <c r="AU7" s="49"/>
+      <c r="AV7" s="49"/>
+      <c r="AW7" s="49"/>
+      <c r="AX7" s="49"/>
+      <c r="AY7" s="50"/>
+      <c r="AZ7" s="49"/>
+      <c r="BA7" s="49"/>
+      <c r="BB7" s="49"/>
+      <c r="BC7" s="49"/>
+      <c r="BD7" s="49"/>
+      <c r="BE7" s="49"/>
+      <c r="BF7" s="50"/>
+      <c r="BG7" s="49"/>
+      <c r="BH7" s="49"/>
+      <c r="BI7" s="49"/>
+      <c r="BJ7" s="49"/>
+      <c r="BK7" s="49"/>
+      <c r="BL7" s="50"/>
+      <c r="BM7" s="51"/>
+      <c r="BN7" s="43"/>
+      <c r="BO7" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP7" s="45"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
@@ -5282,76 +5349,81 @@
         <f aca="false">Netzplan!I8</f>
         <v>1</v>
       </c>
-      <c r="J8" s="44" t="n">
+      <c r="J8" s="46" t="n">
         <f aca="false">ROUND(G8/(H8*I8),0)</f>
         <v>3</v>
       </c>
-      <c r="K8" s="45" t="n">
+      <c r="K8" s="47" t="n">
         <f aca="false">SUM(L8:BM8)</f>
         <v>3</v>
       </c>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="U8" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="47"/>
-      <c r="AA8" s="47"/>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="47"/>
-      <c r="AE8" s="47"/>
-      <c r="AF8" s="47"/>
-      <c r="AG8" s="47"/>
-      <c r="AH8" s="47"/>
-      <c r="AI8" s="47"/>
-      <c r="AJ8" s="47"/>
-      <c r="AK8" s="47"/>
-      <c r="AL8" s="47"/>
-      <c r="AM8" s="47"/>
-      <c r="AN8" s="47"/>
-      <c r="AO8" s="47"/>
-      <c r="AP8" s="47"/>
-      <c r="AQ8" s="47"/>
-      <c r="AR8" s="47"/>
-      <c r="AS8" s="47"/>
-      <c r="AT8" s="47"/>
-      <c r="AU8" s="47"/>
-      <c r="AV8" s="47"/>
-      <c r="AW8" s="47"/>
-      <c r="AX8" s="47"/>
-      <c r="AY8" s="48"/>
-      <c r="AZ8" s="47"/>
-      <c r="BA8" s="47"/>
-      <c r="BB8" s="47"/>
-      <c r="BC8" s="47"/>
-      <c r="BD8" s="47"/>
-      <c r="BE8" s="47"/>
-      <c r="BF8" s="48"/>
-      <c r="BG8" s="47"/>
-      <c r="BH8" s="47"/>
-      <c r="BI8" s="47"/>
-      <c r="BJ8" s="47"/>
-      <c r="BK8" s="47"/>
-      <c r="BL8" s="48"/>
-      <c r="BM8" s="49"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="49"/>
+      <c r="AO8" s="49"/>
+      <c r="AP8" s="49"/>
+      <c r="AQ8" s="49"/>
+      <c r="AR8" s="49"/>
+      <c r="AS8" s="49"/>
+      <c r="AT8" s="49"/>
+      <c r="AU8" s="49"/>
+      <c r="AV8" s="49"/>
+      <c r="AW8" s="49"/>
+      <c r="AX8" s="49"/>
+      <c r="AY8" s="50"/>
+      <c r="AZ8" s="49"/>
+      <c r="BA8" s="49"/>
+      <c r="BB8" s="49"/>
+      <c r="BC8" s="49"/>
+      <c r="BD8" s="49"/>
+      <c r="BE8" s="49"/>
+      <c r="BF8" s="50"/>
+      <c r="BG8" s="49"/>
+      <c r="BH8" s="49"/>
+      <c r="BI8" s="49"/>
+      <c r="BJ8" s="49"/>
+      <c r="BK8" s="49"/>
+      <c r="BL8" s="50"/>
+      <c r="BM8" s="51"/>
+      <c r="BN8" s="43"/>
+      <c r="BO8" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP8" s="45"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
@@ -5366,7 +5438,7 @@
       <c r="F9" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="51" t="n">
+      <c r="G9" s="53" t="n">
         <f aca="false">[1]Netzplan!G9</f>
         <v>2</v>
       </c>
@@ -5378,72 +5450,79 @@
         <f aca="false">Netzplan!I9</f>
         <v>0.75</v>
       </c>
-      <c r="J9" s="44" t="n">
+      <c r="J9" s="46" t="n">
         <f aca="false">ROUND(G9/(H9*I9),0)</f>
         <v>1</v>
       </c>
-      <c r="K9" s="45" t="n">
+      <c r="K9" s="47" t="n">
         <f aca="false">SUM(L9:BM9)</f>
         <v>1</v>
       </c>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="50"/>
-      <c r="AA9" s="50"/>
-      <c r="AB9" s="50"/>
-      <c r="AC9" s="50"/>
-      <c r="AD9" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="47"/>
-      <c r="AF9" s="47"/>
-      <c r="AG9" s="50"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="47"/>
-      <c r="AL9" s="47"/>
-      <c r="AM9" s="47"/>
-      <c r="AN9" s="47"/>
-      <c r="AO9" s="47"/>
-      <c r="AP9" s="47"/>
-      <c r="AQ9" s="47"/>
-      <c r="AR9" s="47"/>
-      <c r="AS9" s="47"/>
-      <c r="AT9" s="47"/>
-      <c r="AU9" s="47"/>
-      <c r="AV9" s="47"/>
-      <c r="AW9" s="47"/>
-      <c r="AX9" s="47"/>
-      <c r="AY9" s="48"/>
-      <c r="AZ9" s="47"/>
-      <c r="BA9" s="47"/>
-      <c r="BB9" s="47"/>
-      <c r="BC9" s="47"/>
-      <c r="BD9" s="47"/>
-      <c r="BE9" s="47"/>
-      <c r="BF9" s="48"/>
-      <c r="BG9" s="47"/>
-      <c r="BH9" s="47"/>
-      <c r="BI9" s="47"/>
-      <c r="BJ9" s="47"/>
-      <c r="BK9" s="47"/>
-      <c r="BL9" s="48"/>
-      <c r="BM9" s="49"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="52"/>
+      <c r="AD9" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="52"/>
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="49"/>
+      <c r="AJ9" s="49"/>
+      <c r="AK9" s="49"/>
+      <c r="AL9" s="49"/>
+      <c r="AM9" s="49"/>
+      <c r="AN9" s="49"/>
+      <c r="AO9" s="49"/>
+      <c r="AP9" s="49"/>
+      <c r="AQ9" s="49"/>
+      <c r="AR9" s="49"/>
+      <c r="AS9" s="49"/>
+      <c r="AT9" s="49"/>
+      <c r="AU9" s="49"/>
+      <c r="AV9" s="49"/>
+      <c r="AW9" s="49"/>
+      <c r="AX9" s="49"/>
+      <c r="AY9" s="50"/>
+      <c r="AZ9" s="49"/>
+      <c r="BA9" s="49"/>
+      <c r="BB9" s="49"/>
+      <c r="BC9" s="49"/>
+      <c r="BD9" s="49"/>
+      <c r="BE9" s="49"/>
+      <c r="BF9" s="50"/>
+      <c r="BG9" s="49"/>
+      <c r="BH9" s="49"/>
+      <c r="BI9" s="49"/>
+      <c r="BJ9" s="49"/>
+      <c r="BK9" s="49"/>
+      <c r="BL9" s="50"/>
+      <c r="BM9" s="51"/>
+      <c r="BN9" s="43"/>
+      <c r="BO9" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP9" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>35</v>
       </c>
@@ -5458,7 +5537,7 @@
       <c r="F10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="51" t="n">
+      <c r="G10" s="53" t="n">
         <f aca="false">[1]Netzplan!G10</f>
         <v>2</v>
       </c>
@@ -5470,72 +5549,79 @@
         <f aca="false">Netzplan!I10</f>
         <v>0.75</v>
       </c>
-      <c r="J10" s="44" t="n">
+      <c r="J10" s="46" t="n">
         <f aca="false">ROUND(G10/(H10*I10),0)</f>
         <v>1</v>
       </c>
-      <c r="K10" s="45" t="n">
+      <c r="K10" s="47" t="n">
         <f aca="false">SUM(L10:BM10)</f>
         <v>1</v>
       </c>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="47"/>
-      <c r="V10" s="47"/>
-      <c r="W10" s="47"/>
-      <c r="X10" s="47"/>
-      <c r="Y10" s="47"/>
-      <c r="Z10" s="47"/>
-      <c r="AA10" s="47"/>
-      <c r="AB10" s="47"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="47"/>
-      <c r="AE10" s="47"/>
-      <c r="AF10" s="47"/>
-      <c r="AG10" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="50"/>
-      <c r="AI10" s="50"/>
-      <c r="AJ10" s="47"/>
-      <c r="AK10" s="47"/>
-      <c r="AL10" s="47"/>
-      <c r="AM10" s="47"/>
-      <c r="AN10" s="47"/>
-      <c r="AO10" s="47"/>
-      <c r="AP10" s="47"/>
-      <c r="AQ10" s="47"/>
-      <c r="AR10" s="47"/>
-      <c r="AS10" s="47"/>
-      <c r="AT10" s="47"/>
-      <c r="AU10" s="47"/>
-      <c r="AV10" s="47"/>
-      <c r="AW10" s="47"/>
-      <c r="AX10" s="47"/>
-      <c r="AY10" s="48"/>
-      <c r="AZ10" s="47"/>
-      <c r="BA10" s="47"/>
-      <c r="BB10" s="47"/>
-      <c r="BC10" s="47"/>
-      <c r="BD10" s="47"/>
-      <c r="BE10" s="47"/>
-      <c r="BF10" s="48"/>
-      <c r="BG10" s="47"/>
-      <c r="BH10" s="47"/>
-      <c r="BI10" s="47"/>
-      <c r="BJ10" s="47"/>
-      <c r="BK10" s="47"/>
-      <c r="BL10" s="48"/>
-      <c r="BM10" s="49"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="52"/>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="49"/>
+      <c r="AN10" s="49"/>
+      <c r="AO10" s="49"/>
+      <c r="AP10" s="49"/>
+      <c r="AQ10" s="49"/>
+      <c r="AR10" s="49"/>
+      <c r="AS10" s="49"/>
+      <c r="AT10" s="49"/>
+      <c r="AU10" s="49"/>
+      <c r="AV10" s="49"/>
+      <c r="AW10" s="49"/>
+      <c r="AX10" s="49"/>
+      <c r="AY10" s="50"/>
+      <c r="AZ10" s="49"/>
+      <c r="BA10" s="49"/>
+      <c r="BB10" s="49"/>
+      <c r="BC10" s="49"/>
+      <c r="BD10" s="49"/>
+      <c r="BE10" s="49"/>
+      <c r="BF10" s="50"/>
+      <c r="BG10" s="49"/>
+      <c r="BH10" s="49"/>
+      <c r="BI10" s="49"/>
+      <c r="BJ10" s="49"/>
+      <c r="BK10" s="49"/>
+      <c r="BL10" s="50"/>
+      <c r="BM10" s="51"/>
+      <c r="BN10" s="43"/>
+      <c r="BO10" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP10" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
@@ -5550,7 +5636,7 @@
       <c r="F11" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="51" t="n">
+      <c r="G11" s="53" t="n">
         <f aca="false">[1]Netzplan!G11</f>
         <v>2</v>
       </c>
@@ -5562,70 +5648,77 @@
         <f aca="false">Netzplan!I11</f>
         <v>0.75</v>
       </c>
-      <c r="J11" s="44" t="n">
+      <c r="J11" s="46" t="n">
         <f aca="false">ROUND(G11/(H11*I11),0)</f>
         <v>1</v>
       </c>
-      <c r="K11" s="45" t="n">
+      <c r="K11" s="47" t="n">
         <f aca="false">SUM(L11:BM11)</f>
         <v>1</v>
       </c>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="47"/>
-      <c r="AA11" s="47"/>
-      <c r="AB11" s="47"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="47"/>
-      <c r="AE11" s="47"/>
-      <c r="AF11" s="47"/>
-      <c r="AG11" s="47"/>
-      <c r="AH11" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="52"/>
-      <c r="AJ11" s="50"/>
-      <c r="AK11" s="50"/>
-      <c r="AL11" s="47"/>
-      <c r="AM11" s="47"/>
-      <c r="AN11" s="47"/>
-      <c r="AO11" s="47"/>
-      <c r="AP11" s="47"/>
-      <c r="AQ11" s="47"/>
-      <c r="AR11" s="47"/>
-      <c r="AS11" s="47"/>
-      <c r="AT11" s="47"/>
-      <c r="AU11" s="47"/>
-      <c r="AV11" s="47"/>
-      <c r="AW11" s="47"/>
-      <c r="AX11" s="47"/>
-      <c r="AY11" s="48"/>
-      <c r="AZ11" s="47"/>
-      <c r="BA11" s="47"/>
-      <c r="BB11" s="47"/>
-      <c r="BC11" s="47"/>
-      <c r="BD11" s="47"/>
-      <c r="BE11" s="47"/>
-      <c r="BF11" s="48"/>
-      <c r="BG11" s="47"/>
-      <c r="BH11" s="47"/>
-      <c r="BI11" s="47"/>
-      <c r="BJ11" s="47"/>
-      <c r="BK11" s="47"/>
-      <c r="BL11" s="48"/>
-      <c r="BM11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="49"/>
+      <c r="AH11" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="54"/>
+      <c r="AJ11" s="52"/>
+      <c r="AK11" s="52"/>
+      <c r="AL11" s="49"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="49"/>
+      <c r="AO11" s="49"/>
+      <c r="AP11" s="49"/>
+      <c r="AQ11" s="49"/>
+      <c r="AR11" s="49"/>
+      <c r="AS11" s="49"/>
+      <c r="AT11" s="49"/>
+      <c r="AU11" s="49"/>
+      <c r="AV11" s="49"/>
+      <c r="AW11" s="49"/>
+      <c r="AX11" s="49"/>
+      <c r="AY11" s="50"/>
+      <c r="AZ11" s="49"/>
+      <c r="BA11" s="49"/>
+      <c r="BB11" s="49"/>
+      <c r="BC11" s="49"/>
+      <c r="BD11" s="49"/>
+      <c r="BE11" s="49"/>
+      <c r="BF11" s="50"/>
+      <c r="BG11" s="49"/>
+      <c r="BH11" s="49"/>
+      <c r="BI11" s="49"/>
+      <c r="BJ11" s="49"/>
+      <c r="BK11" s="49"/>
+      <c r="BL11" s="50"/>
+      <c r="BM11" s="51"/>
+      <c r="BN11" s="43"/>
+      <c r="BO11" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP11" s="45" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
@@ -5642,7 +5735,7 @@
       <c r="F12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="51" t="n">
+      <c r="G12" s="53" t="n">
         <f aca="false">[1]Netzplan!G12</f>
         <v>10</v>
       </c>
@@ -5654,110 +5747,115 @@
         <f aca="false">Netzplan!I12</f>
         <v>0.5</v>
       </c>
-      <c r="J12" s="44" t="n">
+      <c r="J12" s="46" t="n">
         <f aca="false">ROUND(G12/(H12*I12),0)</f>
         <v>20</v>
       </c>
-      <c r="K12" s="45" t="n">
+      <c r="K12" s="47" t="n">
         <f aca="false">SUM(L12:BM12)</f>
         <v>20</v>
       </c>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="47"/>
-      <c r="AF12" s="47"/>
-      <c r="AG12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL12" s="47"/>
-      <c r="AM12" s="47"/>
-      <c r="AN12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS12" s="47"/>
-      <c r="AT12" s="47"/>
-      <c r="AU12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX12" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY12" s="48"/>
-      <c r="AZ12" s="47"/>
-      <c r="BA12" s="47"/>
-      <c r="BB12" s="47"/>
-      <c r="BC12" s="47"/>
-      <c r="BD12" s="47"/>
-      <c r="BE12" s="47"/>
-      <c r="BF12" s="48"/>
-      <c r="BG12" s="47"/>
-      <c r="BH12" s="47"/>
-      <c r="BI12" s="52"/>
-      <c r="BJ12" s="47"/>
-      <c r="BK12" s="47"/>
-      <c r="BL12" s="48"/>
-      <c r="BM12" s="49"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="49"/>
+      <c r="AM12" s="49"/>
+      <c r="AN12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="49"/>
+      <c r="AT12" s="49"/>
+      <c r="AU12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="49"/>
+      <c r="BA12" s="49"/>
+      <c r="BB12" s="49"/>
+      <c r="BC12" s="49"/>
+      <c r="BD12" s="49"/>
+      <c r="BE12" s="49"/>
+      <c r="BF12" s="50"/>
+      <c r="BG12" s="49"/>
+      <c r="BH12" s="49"/>
+      <c r="BI12" s="54"/>
+      <c r="BJ12" s="49"/>
+      <c r="BK12" s="49"/>
+      <c r="BL12" s="50"/>
+      <c r="BM12" s="51"/>
+      <c r="BN12" s="43"/>
+      <c r="BO12" s="44"/>
+      <c r="BP12" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>23</v>
       </c>
@@ -5772,7 +5870,7 @@
       <c r="F13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="51" t="n">
+      <c r="G13" s="53" t="n">
         <f aca="false">[1]Netzplan!G13</f>
         <v>3</v>
       </c>
@@ -5784,74 +5882,81 @@
         <f aca="false">Netzplan!I13</f>
         <v>0.75</v>
       </c>
-      <c r="J13" s="44" t="n">
+      <c r="J13" s="46" t="n">
         <f aca="false">ROUND(G13/(H13*I13),0)</f>
         <v>2</v>
       </c>
-      <c r="K13" s="45" t="n">
+      <c r="K13" s="47" t="n">
         <f aca="false">SUM(L13:BM13)</f>
         <v>2</v>
       </c>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="47"/>
-      <c r="V13" s="47"/>
-      <c r="W13" s="47"/>
-      <c r="X13" s="47"/>
-      <c r="Y13" s="47"/>
-      <c r="Z13" s="47"/>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="47"/>
-      <c r="AD13" s="47"/>
-      <c r="AE13" s="47"/>
-      <c r="AF13" s="47"/>
-      <c r="AG13" s="47"/>
-      <c r="AH13" s="47"/>
-      <c r="AI13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="52"/>
-      <c r="AL13" s="47"/>
-      <c r="AM13" s="47"/>
-      <c r="AN13" s="50"/>
-      <c r="AO13" s="50"/>
-      <c r="AP13" s="50"/>
-      <c r="AQ13" s="50"/>
-      <c r="AR13" s="50"/>
-      <c r="AS13" s="47"/>
-      <c r="AT13" s="47"/>
-      <c r="AU13" s="47"/>
-      <c r="AV13" s="47"/>
-      <c r="AW13" s="47"/>
-      <c r="AX13" s="47"/>
-      <c r="AY13" s="48"/>
-      <c r="AZ13" s="47"/>
-      <c r="BA13" s="47"/>
-      <c r="BB13" s="47"/>
-      <c r="BC13" s="47"/>
-      <c r="BD13" s="47"/>
-      <c r="BE13" s="47"/>
-      <c r="BF13" s="48"/>
-      <c r="BG13" s="47"/>
-      <c r="BH13" s="47"/>
-      <c r="BI13" s="47"/>
-      <c r="BJ13" s="47"/>
-      <c r="BK13" s="47"/>
-      <c r="BL13" s="48"/>
-      <c r="BM13" s="49"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="49"/>
+      <c r="AI13" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="54"/>
+      <c r="AL13" s="49"/>
+      <c r="AM13" s="49"/>
+      <c r="AN13" s="52"/>
+      <c r="AO13" s="52"/>
+      <c r="AP13" s="52"/>
+      <c r="AQ13" s="52"/>
+      <c r="AR13" s="52"/>
+      <c r="AS13" s="49"/>
+      <c r="AT13" s="49"/>
+      <c r="AU13" s="49"/>
+      <c r="AV13" s="49"/>
+      <c r="AW13" s="49"/>
+      <c r="AX13" s="49"/>
+      <c r="AY13" s="50"/>
+      <c r="AZ13" s="49"/>
+      <c r="BA13" s="49"/>
+      <c r="BB13" s="49"/>
+      <c r="BC13" s="49"/>
+      <c r="BD13" s="49"/>
+      <c r="BE13" s="49"/>
+      <c r="BF13" s="50"/>
+      <c r="BG13" s="49"/>
+      <c r="BH13" s="49"/>
+      <c r="BI13" s="49"/>
+      <c r="BJ13" s="49"/>
+      <c r="BK13" s="49"/>
+      <c r="BL13" s="50"/>
+      <c r="BM13" s="51"/>
+      <c r="BN13" s="43"/>
+      <c r="BO13" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP13" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -5866,7 +5971,7 @@
       <c r="F14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="51" t="n">
+      <c r="G14" s="53" t="n">
         <f aca="false">[1]Netzplan!G14</f>
         <v>3</v>
       </c>
@@ -5878,74 +5983,81 @@
         <f aca="false">Netzplan!I14</f>
         <v>0.75</v>
       </c>
-      <c r="J14" s="44" t="n">
+      <c r="J14" s="46" t="n">
         <f aca="false">ROUND(G14/(H14*I14),0)</f>
         <v>2</v>
       </c>
-      <c r="K14" s="45" t="n">
+      <c r="K14" s="47" t="n">
         <f aca="false">SUM(L14:BM14)</f>
         <v>2</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="47"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="47"/>
-      <c r="AM14" s="47"/>
-      <c r="AN14" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO14" s="47"/>
-      <c r="AP14" s="52"/>
-      <c r="AQ14" s="50"/>
-      <c r="AR14" s="50"/>
-      <c r="AS14" s="47"/>
-      <c r="AT14" s="47"/>
-      <c r="AU14" s="50"/>
-      <c r="AV14" s="50"/>
-      <c r="AW14" s="50"/>
-      <c r="AX14" s="47"/>
-      <c r="AY14" s="48"/>
-      <c r="AZ14" s="47"/>
-      <c r="BA14" s="47"/>
-      <c r="BB14" s="47"/>
-      <c r="BC14" s="47"/>
-      <c r="BD14" s="47"/>
-      <c r="BE14" s="47"/>
-      <c r="BF14" s="48"/>
-      <c r="BG14" s="47"/>
-      <c r="BH14" s="47"/>
-      <c r="BI14" s="47"/>
-      <c r="BJ14" s="47"/>
-      <c r="BK14" s="47"/>
-      <c r="BL14" s="48"/>
-      <c r="BM14" s="49"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="49"/>
+      <c r="AC14" s="49"/>
+      <c r="AD14" s="49"/>
+      <c r="AE14" s="49"/>
+      <c r="AF14" s="49"/>
+      <c r="AG14" s="49"/>
+      <c r="AH14" s="49"/>
+      <c r="AI14" s="49"/>
+      <c r="AJ14" s="49"/>
+      <c r="AK14" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="49"/>
+      <c r="AM14" s="49"/>
+      <c r="AN14" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="49"/>
+      <c r="AP14" s="54"/>
+      <c r="AQ14" s="52"/>
+      <c r="AR14" s="52"/>
+      <c r="AS14" s="49"/>
+      <c r="AT14" s="49"/>
+      <c r="AU14" s="52"/>
+      <c r="AV14" s="52"/>
+      <c r="AW14" s="52"/>
+      <c r="AX14" s="49"/>
+      <c r="AY14" s="50"/>
+      <c r="AZ14" s="49"/>
+      <c r="BA14" s="49"/>
+      <c r="BB14" s="49"/>
+      <c r="BC14" s="49"/>
+      <c r="BD14" s="49"/>
+      <c r="BE14" s="49"/>
+      <c r="BF14" s="50"/>
+      <c r="BG14" s="49"/>
+      <c r="BH14" s="49"/>
+      <c r="BI14" s="49"/>
+      <c r="BJ14" s="49"/>
+      <c r="BK14" s="49"/>
+      <c r="BL14" s="50"/>
+      <c r="BM14" s="51"/>
+      <c r="BN14" s="43"/>
+      <c r="BO14" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP14" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -5960,7 +6072,7 @@
       <c r="F15" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="51" t="n">
+      <c r="G15" s="53" t="n">
         <f aca="false">[1]Netzplan!G15</f>
         <v>1</v>
       </c>
@@ -5972,72 +6084,79 @@
         <f aca="false">Netzplan!I15</f>
         <v>0.75</v>
       </c>
-      <c r="J15" s="44" t="n">
+      <c r="J15" s="46" t="n">
         <f aca="false">ROUND(G15/(H15*I15),0)</f>
         <v>1</v>
       </c>
-      <c r="K15" s="45" t="n">
+      <c r="K15" s="47" t="n">
         <f aca="false">SUM(L15:BM15)</f>
         <v>1</v>
       </c>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="47"/>
-      <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="47"/>
-      <c r="Y15" s="47"/>
-      <c r="Z15" s="47"/>
-      <c r="AA15" s="47"/>
-      <c r="AB15" s="47"/>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="47"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="47"/>
-      <c r="AG15" s="47"/>
-      <c r="AH15" s="47"/>
-      <c r="AI15" s="47"/>
-      <c r="AJ15" s="47"/>
-      <c r="AK15" s="47"/>
-      <c r="AL15" s="47"/>
-      <c r="AM15" s="47"/>
-      <c r="AN15" s="47"/>
-      <c r="AO15" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP15" s="47"/>
-      <c r="AQ15" s="47"/>
-      <c r="AR15" s="47"/>
-      <c r="AS15" s="47"/>
-      <c r="AT15" s="47"/>
-      <c r="AU15" s="47"/>
-      <c r="AV15" s="50"/>
-      <c r="AW15" s="47"/>
-      <c r="AX15" s="47"/>
-      <c r="AY15" s="48"/>
-      <c r="AZ15" s="47"/>
-      <c r="BA15" s="47"/>
-      <c r="BB15" s="47"/>
-      <c r="BC15" s="47"/>
-      <c r="BD15" s="47"/>
-      <c r="BE15" s="47"/>
-      <c r="BF15" s="48"/>
-      <c r="BG15" s="47"/>
-      <c r="BH15" s="47"/>
-      <c r="BI15" s="47"/>
-      <c r="BJ15" s="47"/>
-      <c r="BK15" s="47"/>
-      <c r="BL15" s="48"/>
-      <c r="BM15" s="49"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="49"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="49"/>
+      <c r="AC15" s="49"/>
+      <c r="AD15" s="49"/>
+      <c r="AE15" s="49"/>
+      <c r="AF15" s="49"/>
+      <c r="AG15" s="49"/>
+      <c r="AH15" s="49"/>
+      <c r="AI15" s="49"/>
+      <c r="AJ15" s="49"/>
+      <c r="AK15" s="49"/>
+      <c r="AL15" s="49"/>
+      <c r="AM15" s="49"/>
+      <c r="AN15" s="49"/>
+      <c r="AO15" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="49"/>
+      <c r="AQ15" s="49"/>
+      <c r="AR15" s="49"/>
+      <c r="AS15" s="49"/>
+      <c r="AT15" s="49"/>
+      <c r="AU15" s="49"/>
+      <c r="AV15" s="52"/>
+      <c r="AW15" s="49"/>
+      <c r="AX15" s="49"/>
+      <c r="AY15" s="50"/>
+      <c r="AZ15" s="49"/>
+      <c r="BA15" s="49"/>
+      <c r="BB15" s="49"/>
+      <c r="BC15" s="49"/>
+      <c r="BD15" s="49"/>
+      <c r="BE15" s="49"/>
+      <c r="BF15" s="50"/>
+      <c r="BG15" s="49"/>
+      <c r="BH15" s="49"/>
+      <c r="BI15" s="49"/>
+      <c r="BJ15" s="49"/>
+      <c r="BK15" s="49"/>
+      <c r="BL15" s="50"/>
+      <c r="BM15" s="51"/>
+      <c r="BN15" s="43"/>
+      <c r="BO15" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP15" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
@@ -6052,7 +6171,7 @@
       <c r="F16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="51" t="n">
+      <c r="G16" s="53" t="n">
         <f aca="false">[1]Netzplan!G16</f>
         <v>5</v>
       </c>
@@ -6064,76 +6183,83 @@
         <f aca="false">Netzplan!I16</f>
         <v>0.75</v>
       </c>
-      <c r="J16" s="44" t="n">
+      <c r="J16" s="46" t="n">
         <f aca="false">ROUND(G16/(H16*I16),0)</f>
         <v>3</v>
       </c>
-      <c r="K16" s="45" t="n">
+      <c r="K16" s="47" t="n">
         <f aca="false">SUM(L16:BM16)</f>
         <v>3</v>
       </c>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="47"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="47"/>
-      <c r="Z16" s="47"/>
-      <c r="AA16" s="47"/>
-      <c r="AB16" s="47"/>
-      <c r="AC16" s="47"/>
-      <c r="AD16" s="47"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="47"/>
-      <c r="AG16" s="47"/>
-      <c r="AH16" s="47"/>
-      <c r="AI16" s="47"/>
-      <c r="AJ16" s="47"/>
-      <c r="AK16" s="47"/>
-      <c r="AL16" s="47"/>
-      <c r="AM16" s="47"/>
-      <c r="AN16" s="47"/>
-      <c r="AO16" s="47"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="49"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="49"/>
+      <c r="AA16" s="49"/>
+      <c r="AB16" s="49"/>
+      <c r="AC16" s="49"/>
+      <c r="AD16" s="49"/>
+      <c r="AE16" s="49"/>
+      <c r="AF16" s="49"/>
+      <c r="AG16" s="49"/>
+      <c r="AH16" s="49"/>
+      <c r="AI16" s="49"/>
+      <c r="AJ16" s="49"/>
+      <c r="AK16" s="49"/>
+      <c r="AL16" s="49"/>
+      <c r="AM16" s="49"/>
+      <c r="AN16" s="49"/>
+      <c r="AO16" s="49"/>
       <c r="AP16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AQ16" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR16" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS16" s="47"/>
-      <c r="AT16" s="47"/>
-      <c r="AU16" s="47"/>
-      <c r="AV16" s="47"/>
-      <c r="AW16" s="50"/>
-      <c r="AX16" s="50"/>
-      <c r="AY16" s="48"/>
-      <c r="AZ16" s="47"/>
-      <c r="BA16" s="47"/>
-      <c r="BB16" s="50"/>
-      <c r="BC16" s="50"/>
-      <c r="BD16" s="50"/>
-      <c r="BE16" s="47"/>
-      <c r="BF16" s="48"/>
-      <c r="BG16" s="47"/>
-      <c r="BH16" s="47"/>
-      <c r="BI16" s="47"/>
-      <c r="BJ16" s="52"/>
-      <c r="BK16" s="47"/>
-      <c r="BL16" s="48"/>
-      <c r="BM16" s="49"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AQ16" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="49"/>
+      <c r="AT16" s="49"/>
+      <c r="AU16" s="49"/>
+      <c r="AV16" s="49"/>
+      <c r="AW16" s="52"/>
+      <c r="AX16" s="52"/>
+      <c r="AY16" s="50"/>
+      <c r="AZ16" s="49"/>
+      <c r="BA16" s="49"/>
+      <c r="BB16" s="52"/>
+      <c r="BC16" s="52"/>
+      <c r="BD16" s="52"/>
+      <c r="BE16" s="49"/>
+      <c r="BF16" s="50"/>
+      <c r="BG16" s="49"/>
+      <c r="BH16" s="49"/>
+      <c r="BI16" s="49"/>
+      <c r="BJ16" s="54"/>
+      <c r="BK16" s="49"/>
+      <c r="BL16" s="50"/>
+      <c r="BM16" s="51"/>
+      <c r="BN16" s="43"/>
+      <c r="BO16" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP16" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
         <v>45</v>
       </c>
@@ -6146,7 +6272,7 @@
         <v>59</v>
       </c>
       <c r="F17" s="38"/>
-      <c r="G17" s="53" t="n">
+      <c r="G17" s="55" t="n">
         <f aca="false">[1]Netzplan!G17</f>
         <v>1</v>
       </c>
@@ -6158,70 +6284,75 @@
         <f aca="false">Netzplan!I17</f>
         <v>1</v>
       </c>
-      <c r="J17" s="44" t="n">
+      <c r="J17" s="46" t="n">
         <f aca="false">ROUND(G17/(H17*I17),0)</f>
         <v>1</v>
       </c>
-      <c r="K17" s="45" t="n">
+      <c r="K17" s="47" t="n">
         <f aca="false">SUM(L17:BM17)</f>
         <v>1</v>
       </c>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
-      <c r="AG17" s="54"/>
-      <c r="AH17" s="54"/>
-      <c r="AI17" s="54"/>
-      <c r="AJ17" s="54"/>
-      <c r="AK17" s="54"/>
-      <c r="AL17" s="54"/>
-      <c r="AM17" s="54"/>
-      <c r="AN17" s="54"/>
-      <c r="AO17" s="54"/>
-      <c r="AP17" s="54"/>
-      <c r="AQ17" s="54"/>
-      <c r="AR17" s="54"/>
-      <c r="AS17" s="54"/>
-      <c r="AT17" s="54"/>
-      <c r="AU17" s="54"/>
-      <c r="AV17" s="54"/>
-      <c r="AW17" s="54"/>
-      <c r="AX17" s="54"/>
-      <c r="AY17" s="55"/>
-      <c r="AZ17" s="54"/>
-      <c r="BA17" s="54"/>
-      <c r="BB17" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC17" s="50"/>
-      <c r="BD17" s="54"/>
-      <c r="BE17" s="54"/>
-      <c r="BF17" s="55"/>
-      <c r="BG17" s="54"/>
-      <c r="BH17" s="54"/>
-      <c r="BI17" s="54"/>
-      <c r="BJ17" s="54"/>
-      <c r="BK17" s="54"/>
-      <c r="BL17" s="55"/>
-      <c r="BM17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="56"/>
+      <c r="AB17" s="56"/>
+      <c r="AC17" s="56"/>
+      <c r="AD17" s="56"/>
+      <c r="AE17" s="56"/>
+      <c r="AF17" s="56"/>
+      <c r="AG17" s="56"/>
+      <c r="AH17" s="56"/>
+      <c r="AI17" s="56"/>
+      <c r="AJ17" s="56"/>
+      <c r="AK17" s="56"/>
+      <c r="AL17" s="56"/>
+      <c r="AM17" s="56"/>
+      <c r="AN17" s="56"/>
+      <c r="AO17" s="56"/>
+      <c r="AP17" s="56"/>
+      <c r="AQ17" s="56"/>
+      <c r="AR17" s="56"/>
+      <c r="AS17" s="56"/>
+      <c r="AT17" s="56"/>
+      <c r="AU17" s="56"/>
+      <c r="AV17" s="56"/>
+      <c r="AW17" s="56"/>
+      <c r="AX17" s="56"/>
+      <c r="AY17" s="57"/>
+      <c r="AZ17" s="56"/>
+      <c r="BA17" s="56"/>
+      <c r="BB17" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC17" s="52"/>
+      <c r="BD17" s="56"/>
+      <c r="BE17" s="56"/>
+      <c r="BF17" s="57"/>
+      <c r="BG17" s="56"/>
+      <c r="BH17" s="56"/>
+      <c r="BI17" s="56"/>
+      <c r="BJ17" s="56"/>
+      <c r="BK17" s="56"/>
+      <c r="BL17" s="57"/>
+      <c r="BM17" s="58"/>
+      <c r="BN17" s="43"/>
+      <c r="BO17" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP17" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>

<commit_message>
Abschnluss Gantt FIAE B
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
+++ b/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="61">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -207,19 +207,21 @@
   <si>
     <t xml:space="preserve">1.3.1, 1.2.8</t>
   </si>
+  <si>
+    <t xml:space="preserve">Grundstruktur fertig</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00\ %"/>
     <numFmt numFmtId="168" formatCode="0\ %"/>
     <numFmt numFmtId="169" formatCode="General"/>
-    <numFmt numFmtId="170" formatCode="0\ %"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -294,7 +296,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +331,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -603,15 +611,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="70" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,6 +639,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -643,7 +655,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -656,6 +680,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,7 +808,7 @@
       <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -814,7 +842,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8215920" y="325080"/>
+          <a:off x="8224920" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -855,8 +883,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5457240" y="479520"/>
-          <a:ext cx="5522040" cy="0"/>
+          <a:off x="5462640" y="479520"/>
+          <a:ext cx="5529600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -896,7 +924,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5478120" y="488160"/>
+          <a:off x="5483160" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -937,7 +965,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5489640" y="488160"/>
+          <a:off x="5495760" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -978,7 +1006,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="488160"/>
+          <a:off x="8252280" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1019,7 +1047,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10994400" y="488160"/>
+          <a:off x="11008440" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1060,7 +1088,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5489640" y="1122120"/>
+          <a:off x="5495760" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1101,7 +1129,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5489640" y="1609560"/>
+          <a:off x="5495760" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1142,7 +1170,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5489640" y="2097720"/>
+          <a:off x="5495760" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1183,7 +1211,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5489640" y="2584800"/>
+          <a:off x="5495760" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1224,7 +1252,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="1122120"/>
+          <a:off x="8252280" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1265,7 +1293,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="1609560"/>
+          <a:off x="8252280" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1306,7 +1334,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="2097720"/>
+          <a:off x="8252280" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1347,7 +1375,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="2584800"/>
+          <a:off x="8252280" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1388,7 +1416,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="3072240"/>
+          <a:off x="8252280" y="3072240"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1429,7 +1457,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="3560400"/>
+          <a:off x="8252280" y="3560400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1470,7 +1498,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="4047480"/>
+          <a:off x="8252280" y="4047480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1511,7 +1539,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="4534920"/>
+          <a:off x="8252280" y="4534920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1552,7 +1580,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8242200" y="5023080"/>
+          <a:off x="8252280" y="5023080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1593,7 +1621,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10994760" y="2097360"/>
+          <a:off x="11008800" y="2097360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1634,7 +1662,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10994760" y="1609560"/>
+          <a:off x="11008800" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1675,7 +1703,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10994760" y="1121760"/>
+          <a:off x="11008800" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1704,15 +1732,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1721,8 +1749,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9597600" y="479160"/>
-          <a:ext cx="535680" cy="6120"/>
+          <a:off x="9603000" y="479520"/>
+          <a:ext cx="535320" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1746,15 +1774,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1763,7 +1791,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10937520" y="485280"/>
+          <a:off x="10942920" y="485640"/>
           <a:ext cx="541080" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1790,13 +1818,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>255600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>3240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1805,8 +1833,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9842760" y="505440"/>
-          <a:ext cx="18360" cy="1950840"/>
+          <a:off x="9848520" y="505800"/>
+          <a:ext cx="18000" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1830,13 +1858,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>12240</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
+      <xdr:colOff>264600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
@@ -1847,7 +1875,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9869760" y="2435040"/>
+          <a:off x="9875160" y="2435040"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1874,13 +1902,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>5040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>244800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1889,7 +1917,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12297960" y="479160"/>
+          <a:off x="12303000" y="479520"/>
           <a:ext cx="1862640" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1914,13 +1942,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
@@ -1931,7 +1959,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10937160" y="2435760"/>
+          <a:off x="10942560" y="2435760"/>
           <a:ext cx="541080" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1973,7 +2001,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12287880" y="2435760"/>
+          <a:off x="12292920" y="2435760"/>
           <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2000,13 +2028,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2015,7 +2043,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11197440" y="483120"/>
+          <a:off x="11202480" y="483480"/>
           <a:ext cx="0" cy="982440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2042,13 +2070,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>253440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>258120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2057,7 +2085,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11193840" y="1455480"/>
+          <a:off x="11198880" y="1455840"/>
           <a:ext cx="275040" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2082,13 +2110,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>155520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
+      <xdr:colOff>12600</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
@@ -2099,8 +2127,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12279960" y="1455840"/>
-          <a:ext cx="565920" cy="7200"/>
+          <a:off x="12285000" y="1455840"/>
+          <a:ext cx="566280" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2141,7 +2169,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14988600" y="480240"/>
+          <a:off x="14993640" y="480240"/>
           <a:ext cx="560520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2183,7 +2211,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12556800" y="1926720"/>
+          <a:off x="12561840" y="1926720"/>
           <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2208,15 +2236,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>265320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>258120</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2225,7 +2253,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="12557520" y="1943640"/>
+          <a:off x="12562920" y="1944000"/>
           <a:ext cx="1345320" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2250,15 +2278,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
+      <xdr:colOff>264240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>265320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2267,7 +2295,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13908960" y="471600"/>
+          <a:off x="13914360" y="471960"/>
           <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2309,7 +2337,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13647240" y="1463040"/>
+          <a:off x="13652280" y="1463040"/>
           <a:ext cx="277920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2351,7 +2379,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16360560" y="478440"/>
+          <a:off x="16365600" y="478440"/>
           <a:ext cx="559800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2393,7 +2421,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17705160" y="478080"/>
+          <a:off x="17710200" y="478080"/>
           <a:ext cx="556560" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2420,13 +2448,13 @@
       <xdr:col>49</xdr:col>
       <xdr:colOff>20520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2435,7 +2463,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19076040" y="485280"/>
+          <a:off x="19081080" y="485640"/>
           <a:ext cx="529200" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2460,15 +2488,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>251280</xdr:colOff>
+      <xdr:colOff>251640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>20880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2477,7 +2505,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20388600" y="480600"/>
+          <a:off x="20394000" y="480960"/>
           <a:ext cx="580680" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2504,13 +2532,13 @@
       <xdr:col>58</xdr:col>
       <xdr:colOff>251640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
       <xdr:colOff>262080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2519,7 +2547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="21741840" y="481680"/>
+          <a:off x="21746880" y="482040"/>
           <a:ext cx="551520" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2544,15 +2572,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>66</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2561,7 +2589,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="23114520" y="481680"/>
+          <a:off x="23119920" y="482040"/>
           <a:ext cx="541080" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2586,13 +2614,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>263880</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>269640</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
@@ -2603,7 +2631,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23376240" y="490320"/>
+          <a:off x="23381640" y="490320"/>
           <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2630,13 +2658,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>7920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>259920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2645,7 +2673,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10948320" y="485280"/>
+          <a:off x="10953360" y="485640"/>
           <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2670,15 +2698,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>268920</xdr:colOff>
+      <xdr:colOff>269280</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>254520</xdr:colOff>
+      <xdr:colOff>254880</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2687,7 +2715,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13643280" y="2437920"/>
+          <a:off x="13648680" y="2438280"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2698,6 +2726,145 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>159480</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9684720" y="1663200"/>
+          <a:ext cx="153360" cy="153000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="10800" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="10800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="10800" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="10800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="10800" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="729fcf"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>29520</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>159480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>149400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12241800" y="2800440"/>
+          <a:ext cx="153360" cy="153000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="10800" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="10800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="10800" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="10800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="10800" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="729fcf"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2817,11 +2984,11 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3364,11 +3531,11 @@
   </sheetPr>
   <dimension ref="A1:BQ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
@@ -4493,24 +4660,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BP17"/>
+  <dimension ref="A1:BP18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="11" ySplit="0" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="BO5" activeCellId="0" sqref="BO5"/>
+      <selection pane="topRight" activeCell="AR18" activeCellId="0" sqref="AR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="5" min="5" style="0" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="9" min="7" style="0" width="11.52"/>
     <col collapsed="true" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="11" style="0" width="3.59"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="11" min="11" style="0" width="3.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="12" style="0" width="3.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -4775,7 +4942,7 @@
       <c r="AA2" s="49"/>
       <c r="AB2" s="49"/>
       <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
+      <c r="AD2" s="50"/>
       <c r="AE2" s="49"/>
       <c r="AF2" s="49"/>
       <c r="AG2" s="49"/>
@@ -4796,21 +4963,21 @@
       <c r="AV2" s="49"/>
       <c r="AW2" s="49"/>
       <c r="AX2" s="49"/>
-      <c r="AY2" s="50"/>
+      <c r="AY2" s="51"/>
       <c r="AZ2" s="49"/>
       <c r="BA2" s="49"/>
       <c r="BB2" s="49"/>
       <c r="BC2" s="49"/>
       <c r="BD2" s="49"/>
       <c r="BE2" s="49"/>
-      <c r="BF2" s="50"/>
+      <c r="BF2" s="51"/>
       <c r="BG2" s="49"/>
       <c r="BH2" s="49"/>
       <c r="BI2" s="49"/>
       <c r="BJ2" s="49"/>
       <c r="BK2" s="49"/>
-      <c r="BL2" s="50"/>
-      <c r="BM2" s="51"/>
+      <c r="BL2" s="51"/>
+      <c r="BM2" s="52"/>
       <c r="BN2" s="43"/>
       <c r="BO2" s="44" t="n">
         <v>1</v>
@@ -4859,7 +5026,7 @@
       <c r="P3" s="49"/>
       <c r="Q3" s="49"/>
       <c r="R3" s="49"/>
-      <c r="S3" s="52" t="n">
+      <c r="S3" s="53" t="n">
         <v>1</v>
       </c>
       <c r="T3" s="49"/>
@@ -4872,7 +5039,7 @@
       <c r="AA3" s="49"/>
       <c r="AB3" s="49"/>
       <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
+      <c r="AD3" s="50"/>
       <c r="AE3" s="49"/>
       <c r="AF3" s="49"/>
       <c r="AG3" s="49"/>
@@ -4893,21 +5060,21 @@
       <c r="AV3" s="49"/>
       <c r="AW3" s="49"/>
       <c r="AX3" s="49"/>
-      <c r="AY3" s="50"/>
+      <c r="AY3" s="51"/>
       <c r="AZ3" s="49"/>
       <c r="BA3" s="49"/>
       <c r="BB3" s="49"/>
       <c r="BC3" s="49"/>
       <c r="BD3" s="49"/>
       <c r="BE3" s="49"/>
-      <c r="BF3" s="50"/>
+      <c r="BF3" s="51"/>
       <c r="BG3" s="49"/>
       <c r="BH3" s="49"/>
       <c r="BI3" s="49"/>
       <c r="BJ3" s="49"/>
       <c r="BK3" s="49"/>
-      <c r="BL3" s="50"/>
-      <c r="BM3" s="51"/>
+      <c r="BL3" s="51"/>
+      <c r="BM3" s="52"/>
       <c r="BN3" s="43" t="n">
         <v>1</v>
       </c>
@@ -4957,16 +5124,16 @@
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
       <c r="S4" s="49"/>
-      <c r="T4" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="52" t="n">
+      <c r="T4" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="53" t="n">
         <v>1</v>
       </c>
       <c r="X4" s="49"/>
@@ -4975,7 +5142,7 @@
       <c r="AA4" s="49"/>
       <c r="AB4" s="49"/>
       <c r="AC4" s="49"/>
-      <c r="AD4" s="49"/>
+      <c r="AD4" s="50"/>
       <c r="AE4" s="49"/>
       <c r="AF4" s="49"/>
       <c r="AG4" s="49"/>
@@ -4996,21 +5163,21 @@
       <c r="AV4" s="49"/>
       <c r="AW4" s="49"/>
       <c r="AX4" s="49"/>
-      <c r="AY4" s="50"/>
+      <c r="AY4" s="51"/>
       <c r="AZ4" s="49"/>
       <c r="BA4" s="49"/>
       <c r="BB4" s="49"/>
       <c r="BC4" s="49"/>
       <c r="BD4" s="49"/>
       <c r="BE4" s="49"/>
-      <c r="BF4" s="50"/>
+      <c r="BF4" s="51"/>
       <c r="BG4" s="49"/>
       <c r="BH4" s="49"/>
       <c r="BI4" s="49"/>
       <c r="BJ4" s="49"/>
       <c r="BK4" s="49"/>
-      <c r="BL4" s="50"/>
-      <c r="BM4" s="51"/>
+      <c r="BL4" s="51"/>
+      <c r="BM4" s="52"/>
       <c r="BN4" s="43" t="n">
         <v>1</v>
       </c>
@@ -5060,13 +5227,13 @@
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
       <c r="S5" s="49"/>
-      <c r="T5" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="52" t="n">
+      <c r="T5" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="53" t="n">
         <v>1</v>
       </c>
       <c r="W5" s="49"/>
@@ -5076,7 +5243,7 @@
       <c r="AA5" s="49"/>
       <c r="AB5" s="49"/>
       <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
+      <c r="AD5" s="50"/>
       <c r="AE5" s="49"/>
       <c r="AF5" s="49"/>
       <c r="AG5" s="49"/>
@@ -5097,21 +5264,21 @@
       <c r="AV5" s="49"/>
       <c r="AW5" s="49"/>
       <c r="AX5" s="49"/>
-      <c r="AY5" s="50"/>
+      <c r="AY5" s="51"/>
       <c r="AZ5" s="49"/>
       <c r="BA5" s="49"/>
       <c r="BB5" s="49"/>
       <c r="BC5" s="49"/>
       <c r="BD5" s="49"/>
       <c r="BE5" s="49"/>
-      <c r="BF5" s="50"/>
+      <c r="BF5" s="51"/>
       <c r="BG5" s="49"/>
       <c r="BH5" s="49"/>
       <c r="BI5" s="49"/>
       <c r="BJ5" s="49"/>
       <c r="BK5" s="49"/>
-      <c r="BL5" s="50"/>
-      <c r="BM5" s="51"/>
+      <c r="BL5" s="51"/>
+      <c r="BM5" s="52"/>
       <c r="BN5" s="43" t="n">
         <v>1</v>
       </c>
@@ -5164,24 +5331,24 @@
       <c r="T6" s="49"/>
       <c r="U6" s="49"/>
       <c r="V6" s="49"/>
-      <c r="W6" s="52" t="n">
+      <c r="W6" s="53" t="n">
         <v>1</v>
       </c>
       <c r="X6" s="49"/>
       <c r="Y6" s="49"/>
-      <c r="Z6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="52"/>
+      <c r="Z6" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="54"/>
       <c r="AE6" s="49"/>
       <c r="AF6" s="49"/>
       <c r="AG6" s="49"/>
@@ -5202,21 +5369,21 @@
       <c r="AV6" s="49"/>
       <c r="AW6" s="49"/>
       <c r="AX6" s="49"/>
-      <c r="AY6" s="50"/>
+      <c r="AY6" s="51"/>
       <c r="AZ6" s="49"/>
       <c r="BA6" s="49"/>
       <c r="BB6" s="49"/>
       <c r="BC6" s="49"/>
       <c r="BD6" s="49"/>
       <c r="BE6" s="49"/>
-      <c r="BF6" s="50"/>
+      <c r="BF6" s="51"/>
       <c r="BG6" s="49"/>
       <c r="BH6" s="49"/>
       <c r="BI6" s="49"/>
       <c r="BJ6" s="49"/>
       <c r="BK6" s="49"/>
-      <c r="BL6" s="50"/>
-      <c r="BM6" s="51"/>
+      <c r="BL6" s="51"/>
+      <c r="BM6" s="52"/>
       <c r="BN6" s="43" t="n">
         <v>1</v>
       </c>
@@ -5280,7 +5447,7 @@
       <c r="AA7" s="49"/>
       <c r="AB7" s="49"/>
       <c r="AC7" s="49"/>
-      <c r="AD7" s="49"/>
+      <c r="AD7" s="50"/>
       <c r="AE7" s="49"/>
       <c r="AF7" s="49"/>
       <c r="AG7" s="49"/>
@@ -5301,21 +5468,21 @@
       <c r="AV7" s="49"/>
       <c r="AW7" s="49"/>
       <c r="AX7" s="49"/>
-      <c r="AY7" s="50"/>
+      <c r="AY7" s="51"/>
       <c r="AZ7" s="49"/>
       <c r="BA7" s="49"/>
       <c r="BB7" s="49"/>
       <c r="BC7" s="49"/>
       <c r="BD7" s="49"/>
       <c r="BE7" s="49"/>
-      <c r="BF7" s="50"/>
+      <c r="BF7" s="51"/>
       <c r="BG7" s="49"/>
       <c r="BH7" s="49"/>
       <c r="BI7" s="49"/>
       <c r="BJ7" s="49"/>
       <c r="BK7" s="49"/>
-      <c r="BL7" s="50"/>
-      <c r="BM7" s="51"/>
+      <c r="BL7" s="51"/>
+      <c r="BM7" s="52"/>
       <c r="BN7" s="43"/>
       <c r="BO7" s="44" t="n">
         <v>1</v>
@@ -5381,7 +5548,7 @@
       <c r="AA8" s="49"/>
       <c r="AB8" s="49"/>
       <c r="AC8" s="49"/>
-      <c r="AD8" s="49"/>
+      <c r="AD8" s="50"/>
       <c r="AE8" s="49"/>
       <c r="AF8" s="49"/>
       <c r="AG8" s="49"/>
@@ -5402,62 +5569,41 @@
       <c r="AV8" s="49"/>
       <c r="AW8" s="49"/>
       <c r="AX8" s="49"/>
-      <c r="AY8" s="50"/>
+      <c r="AY8" s="51"/>
       <c r="AZ8" s="49"/>
       <c r="BA8" s="49"/>
       <c r="BB8" s="49"/>
       <c r="BC8" s="49"/>
       <c r="BD8" s="49"/>
       <c r="BE8" s="49"/>
-      <c r="BF8" s="50"/>
+      <c r="BF8" s="51"/>
       <c r="BG8" s="49"/>
       <c r="BH8" s="49"/>
       <c r="BI8" s="49"/>
       <c r="BJ8" s="49"/>
       <c r="BK8" s="49"/>
-      <c r="BL8" s="50"/>
-      <c r="BM8" s="51"/>
+      <c r="BL8" s="51"/>
+      <c r="BM8" s="52"/>
       <c r="BN8" s="43"/>
       <c r="BO8" s="44" t="n">
         <v>1</v>
       </c>
       <c r="BP8" s="45"/>
     </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="53" t="n">
-        <f aca="false">[1]Netzplan!G9</f>
-        <v>2</v>
-      </c>
-      <c r="H9" s="31" t="str">
-        <f aca="false">Netzplan!H9</f>
-        <v>2</v>
-      </c>
-      <c r="I9" s="28" t="n">
-        <f aca="false">Netzplan!I9</f>
-        <v>0.75</v>
-      </c>
-      <c r="J9" s="46" t="n">
-        <f aca="false">ROUND(G9/(H9*I9),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="47" t="n">
-        <f aca="false">SUM(L9:BM9)</f>
-        <v>1</v>
-      </c>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14"/>
+      <c r="B9" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
       <c r="L9" s="49"/>
       <c r="M9" s="49"/>
       <c r="N9" s="49"/>
@@ -5466,22 +5612,17 @@
       <c r="Q9" s="49"/>
       <c r="R9" s="49"/>
       <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
       <c r="W9" s="49"/>
       <c r="X9" s="49"/>
       <c r="Y9" s="49"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="52"/>
-      <c r="AC9" s="52"/>
-      <c r="AD9" s="52" t="n">
-        <v>1</v>
-      </c>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="50"/>
       <c r="AE9" s="49"/>
       <c r="AF9" s="49"/>
-      <c r="AG9" s="52"/>
+      <c r="AG9" s="49"/>
       <c r="AH9" s="49"/>
       <c r="AI9" s="49"/>
       <c r="AJ9" s="49"/>
@@ -5499,54 +5640,50 @@
       <c r="AV9" s="49"/>
       <c r="AW9" s="49"/>
       <c r="AX9" s="49"/>
-      <c r="AY9" s="50"/>
+      <c r="AY9" s="51"/>
       <c r="AZ9" s="49"/>
       <c r="BA9" s="49"/>
       <c r="BB9" s="49"/>
       <c r="BC9" s="49"/>
       <c r="BD9" s="49"/>
       <c r="BE9" s="49"/>
-      <c r="BF9" s="50"/>
+      <c r="BF9" s="51"/>
       <c r="BG9" s="49"/>
       <c r="BH9" s="49"/>
       <c r="BI9" s="49"/>
       <c r="BJ9" s="49"/>
       <c r="BK9" s="49"/>
-      <c r="BL9" s="50"/>
-      <c r="BM9" s="51"/>
+      <c r="BL9" s="51"/>
+      <c r="BM9" s="52"/>
       <c r="BN9" s="43"/>
-      <c r="BO9" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP9" s="45" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="BO9" s="44"/>
+      <c r="BP9" s="45"/>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="35" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="53" t="n">
-        <f aca="false">[1]Netzplan!G10</f>
+        <v>35</v>
+      </c>
+      <c r="G10" s="55" t="n">
+        <f aca="false">[1]Netzplan!G9</f>
         <v>2</v>
       </c>
       <c r="H10" s="31" t="str">
-        <f aca="false">Netzplan!H10</f>
+        <f aca="false">Netzplan!H9</f>
         <v>2</v>
       </c>
       <c r="I10" s="28" t="n">
-        <f aca="false">Netzplan!I10</f>
+        <f aca="false">Netzplan!I9</f>
         <v>0.75</v>
       </c>
       <c r="J10" s="46" t="n">
@@ -5571,18 +5708,18 @@
       <c r="W10" s="49"/>
       <c r="X10" s="49"/>
       <c r="Y10" s="49"/>
-      <c r="Z10" s="49"/>
-      <c r="AA10" s="49"/>
-      <c r="AB10" s="49"/>
-      <c r="AC10" s="49"/>
-      <c r="AD10" s="49"/>
+      <c r="Z10" s="53"/>
+      <c r="AA10" s="53"/>
+      <c r="AB10" s="53"/>
+      <c r="AC10" s="53"/>
+      <c r="AD10" s="56"/>
       <c r="AE10" s="49"/>
       <c r="AF10" s="49"/>
-      <c r="AG10" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="52"/>
+      <c r="AG10" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="49"/>
       <c r="AJ10" s="49"/>
       <c r="AK10" s="49"/>
       <c r="AL10" s="49"/>
@@ -5598,21 +5735,21 @@
       <c r="AV10" s="49"/>
       <c r="AW10" s="49"/>
       <c r="AX10" s="49"/>
-      <c r="AY10" s="50"/>
+      <c r="AY10" s="51"/>
       <c r="AZ10" s="49"/>
       <c r="BA10" s="49"/>
       <c r="BB10" s="49"/>
       <c r="BC10" s="49"/>
       <c r="BD10" s="49"/>
       <c r="BE10" s="49"/>
-      <c r="BF10" s="50"/>
+      <c r="BF10" s="51"/>
       <c r="BG10" s="49"/>
       <c r="BH10" s="49"/>
       <c r="BI10" s="49"/>
       <c r="BJ10" s="49"/>
       <c r="BK10" s="49"/>
-      <c r="BL10" s="50"/>
-      <c r="BM10" s="51"/>
+      <c r="BL10" s="51"/>
+      <c r="BM10" s="52"/>
       <c r="BN10" s="43"/>
       <c r="BO10" s="44" t="n">
         <v>1</v>
@@ -5623,29 +5760,29 @@
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="53" t="n">
-        <f aca="false">[1]Netzplan!G11</f>
+        <v>37</v>
+      </c>
+      <c r="G11" s="55" t="n">
+        <f aca="false">[1]Netzplan!G10</f>
         <v>2</v>
       </c>
       <c r="H11" s="31" t="str">
-        <f aca="false">Netzplan!H11</f>
+        <f aca="false">Netzplan!H10</f>
         <v>2</v>
       </c>
       <c r="I11" s="28" t="n">
-        <f aca="false">Netzplan!I11</f>
+        <f aca="false">Netzplan!I10</f>
         <v>0.75</v>
       </c>
       <c r="J11" s="46" t="n">
@@ -5674,16 +5811,15 @@
       <c r="AA11" s="49"/>
       <c r="AB11" s="49"/>
       <c r="AC11" s="49"/>
-      <c r="AD11" s="49"/>
+      <c r="AD11" s="50"/>
       <c r="AE11" s="49"/>
       <c r="AF11" s="49"/>
-      <c r="AG11" s="49"/>
       <c r="AH11" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="AI11" s="54"/>
-      <c r="AJ11" s="52"/>
-      <c r="AK11" s="52"/>
+      <c r="AI11" s="53"/>
+      <c r="AJ11" s="49"/>
+      <c r="AK11" s="49"/>
       <c r="AL11" s="49"/>
       <c r="AM11" s="49"/>
       <c r="AN11" s="49"/>
@@ -5697,21 +5833,21 @@
       <c r="AV11" s="49"/>
       <c r="AW11" s="49"/>
       <c r="AX11" s="49"/>
-      <c r="AY11" s="50"/>
+      <c r="AY11" s="51"/>
       <c r="AZ11" s="49"/>
       <c r="BA11" s="49"/>
       <c r="BB11" s="49"/>
       <c r="BC11" s="49"/>
       <c r="BD11" s="49"/>
       <c r="BE11" s="49"/>
-      <c r="BF11" s="50"/>
+      <c r="BF11" s="51"/>
       <c r="BG11" s="49"/>
       <c r="BH11" s="49"/>
       <c r="BI11" s="49"/>
       <c r="BJ11" s="49"/>
       <c r="BK11" s="49"/>
-      <c r="BL11" s="50"/>
-      <c r="BM11" s="51"/>
+      <c r="BL11" s="51"/>
+      <c r="BM11" s="52"/>
       <c r="BN11" s="43"/>
       <c r="BO11" s="44" t="n">
         <v>1</v>
@@ -5722,38 +5858,38 @@
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="35" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="53" t="n">
-        <f aca="false">[1]Netzplan!G12</f>
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="G12" s="55" t="n">
+        <f aca="false">[1]Netzplan!G11</f>
+        <v>2</v>
       </c>
       <c r="H12" s="31" t="str">
-        <f aca="false">Netzplan!H12</f>
-        <v>1</v>
+        <f aca="false">Netzplan!H11</f>
+        <v>2</v>
       </c>
       <c r="I12" s="28" t="n">
-        <f aca="false">Netzplan!I12</f>
-        <v>0.5</v>
+        <f aca="false">Netzplan!I11</f>
+        <v>0.75</v>
       </c>
       <c r="J12" s="46" t="n">
         <f aca="false">ROUND(G12/(H12*I12),0)</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="K12" s="47" t="n">
         <f aca="false">SUM(L12:BM12)</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L12" s="49"/>
       <c r="M12" s="49"/>
@@ -5766,129 +5902,92 @@
       <c r="T12" s="49"/>
       <c r="U12" s="49"/>
       <c r="V12" s="49"/>
-      <c r="W12" s="48" t="n">
-        <v>1</v>
-      </c>
+      <c r="W12" s="49"/>
       <c r="X12" s="49"/>
       <c r="Y12" s="49"/>
-      <c r="Z12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="48" t="n">
-        <v>1</v>
-      </c>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="50"/>
       <c r="AE12" s="49"/>
       <c r="AF12" s="49"/>
-      <c r="AG12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="48" t="n">
-        <v>1</v>
-      </c>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="53"/>
+      <c r="AK12" s="53"/>
       <c r="AL12" s="49"/>
       <c r="AM12" s="49"/>
-      <c r="AN12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR12" s="48" t="n">
-        <v>1</v>
-      </c>
+      <c r="AN12" s="49"/>
+      <c r="AO12" s="49"/>
+      <c r="AP12" s="49"/>
+      <c r="AQ12" s="49"/>
+      <c r="AR12" s="49"/>
       <c r="AS12" s="49"/>
       <c r="AT12" s="49"/>
-      <c r="AU12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY12" s="50"/>
+      <c r="AU12" s="49"/>
+      <c r="AV12" s="49"/>
+      <c r="AW12" s="49"/>
+      <c r="AX12" s="49"/>
+      <c r="AY12" s="51"/>
       <c r="AZ12" s="49"/>
       <c r="BA12" s="49"/>
       <c r="BB12" s="49"/>
       <c r="BC12" s="49"/>
       <c r="BD12" s="49"/>
       <c r="BE12" s="49"/>
-      <c r="BF12" s="50"/>
+      <c r="BF12" s="51"/>
       <c r="BG12" s="49"/>
       <c r="BH12" s="49"/>
-      <c r="BI12" s="54"/>
+      <c r="BI12" s="49"/>
       <c r="BJ12" s="49"/>
       <c r="BK12" s="49"/>
-      <c r="BL12" s="50"/>
-      <c r="BM12" s="51"/>
+      <c r="BL12" s="51"/>
+      <c r="BM12" s="52"/>
       <c r="BN12" s="43"/>
-      <c r="BO12" s="44"/>
+      <c r="BO12" s="44" t="n">
+        <v>1</v>
+      </c>
       <c r="BP12" s="45" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="35" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="53" t="n">
-        <f aca="false">[1]Netzplan!G13</f>
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="G13" s="55" t="n">
+        <f aca="false">[1]Netzplan!G12</f>
+        <v>10</v>
       </c>
       <c r="H13" s="31" t="str">
-        <f aca="false">Netzplan!H13</f>
-        <v>2</v>
+        <f aca="false">Netzplan!H12</f>
+        <v>1</v>
       </c>
       <c r="I13" s="28" t="n">
-        <f aca="false">Netzplan!I13</f>
-        <v>0.75</v>
+        <f aca="false">Netzplan!I12</f>
+        <v>0.5</v>
       </c>
       <c r="J13" s="46" t="n">
         <f aca="false">ROUND(G13/(H13*I13),0)</f>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K13" s="47" t="n">
         <f aca="false">SUM(L13:BM13)</f>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="L13" s="49"/>
       <c r="M13" s="49"/>
@@ -5901,86 +6000,120 @@
       <c r="T13" s="49"/>
       <c r="U13" s="49"/>
       <c r="V13" s="49"/>
-      <c r="W13" s="49"/>
+      <c r="W13" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="X13" s="49"/>
       <c r="Y13" s="49"/>
-      <c r="Z13" s="49"/>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="49"/>
-      <c r="AC13" s="49"/>
-      <c r="AD13" s="49"/>
+      <c r="Z13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="57" t="n">
+        <v>1</v>
+      </c>
       <c r="AE13" s="49"/>
       <c r="AF13" s="49"/>
-      <c r="AG13" s="49"/>
-      <c r="AH13" s="49"/>
-      <c r="AI13" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="54"/>
+      <c r="AG13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="AL13" s="49"/>
       <c r="AM13" s="49"/>
-      <c r="AN13" s="52"/>
-      <c r="AO13" s="52"/>
-      <c r="AP13" s="52"/>
-      <c r="AQ13" s="52"/>
-      <c r="AR13" s="52"/>
+      <c r="AN13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="48" t="n">
+        <v>1</v>
+      </c>
       <c r="AS13" s="49"/>
       <c r="AT13" s="49"/>
-      <c r="AU13" s="49"/>
-      <c r="AV13" s="49"/>
-      <c r="AW13" s="49"/>
-      <c r="AX13" s="49"/>
-      <c r="AY13" s="50"/>
+      <c r="AU13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="51"/>
       <c r="AZ13" s="49"/>
       <c r="BA13" s="49"/>
       <c r="BB13" s="49"/>
       <c r="BC13" s="49"/>
       <c r="BD13" s="49"/>
       <c r="BE13" s="49"/>
-      <c r="BF13" s="50"/>
+      <c r="BF13" s="51"/>
       <c r="BG13" s="49"/>
       <c r="BH13" s="49"/>
-      <c r="BI13" s="49"/>
+      <c r="BI13" s="58"/>
       <c r="BJ13" s="49"/>
       <c r="BK13" s="49"/>
-      <c r="BL13" s="50"/>
-      <c r="BM13" s="51"/>
+      <c r="BL13" s="51"/>
+      <c r="BM13" s="52"/>
       <c r="BN13" s="43"/>
-      <c r="BO13" s="44" t="n">
-        <v>1</v>
-      </c>
+      <c r="BO13" s="44"/>
       <c r="BP13" s="45" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="35" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="53" t="n">
-        <f aca="false">[1]Netzplan!G14</f>
+        <v>41</v>
+      </c>
+      <c r="G14" s="55" t="n">
+        <f aca="false">[1]Netzplan!G13</f>
         <v>3</v>
       </c>
       <c r="H14" s="31" t="str">
-        <f aca="false">Netzplan!H14</f>
+        <f aca="false">Netzplan!H13</f>
         <v>2</v>
       </c>
       <c r="I14" s="28" t="n">
-        <f aca="false">Netzplan!I14</f>
+        <f aca="false">Netzplan!I13</f>
         <v>0.75</v>
       </c>
       <c r="J14" s="46" t="n">
@@ -6009,46 +6142,45 @@
       <c r="AA14" s="49"/>
       <c r="AB14" s="49"/>
       <c r="AC14" s="49"/>
-      <c r="AD14" s="49"/>
+      <c r="AD14" s="50"/>
       <c r="AE14" s="49"/>
       <c r="AF14" s="49"/>
       <c r="AG14" s="49"/>
       <c r="AH14" s="49"/>
-      <c r="AI14" s="49"/>
-      <c r="AJ14" s="49"/>
+      <c r="AJ14" s="49" t="n">
+        <v>1</v>
+      </c>
       <c r="AK14" s="49" t="n">
         <v>1</v>
       </c>
       <c r="AL14" s="49"/>
       <c r="AM14" s="49"/>
-      <c r="AN14" s="49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO14" s="49"/>
-      <c r="AP14" s="54"/>
-      <c r="AQ14" s="52"/>
-      <c r="AR14" s="52"/>
+      <c r="AN14" s="53"/>
+      <c r="AO14" s="53"/>
+      <c r="AP14" s="53"/>
+      <c r="AQ14" s="53"/>
+      <c r="AR14" s="53"/>
       <c r="AS14" s="49"/>
       <c r="AT14" s="49"/>
-      <c r="AU14" s="52"/>
-      <c r="AV14" s="52"/>
-      <c r="AW14" s="52"/>
+      <c r="AU14" s="49"/>
+      <c r="AV14" s="49"/>
+      <c r="AW14" s="49"/>
       <c r="AX14" s="49"/>
-      <c r="AY14" s="50"/>
+      <c r="AY14" s="51"/>
       <c r="AZ14" s="49"/>
       <c r="BA14" s="49"/>
       <c r="BB14" s="49"/>
       <c r="BC14" s="49"/>
       <c r="BD14" s="49"/>
       <c r="BE14" s="49"/>
-      <c r="BF14" s="50"/>
+      <c r="BF14" s="51"/>
       <c r="BG14" s="49"/>
       <c r="BH14" s="49"/>
       <c r="BI14" s="49"/>
       <c r="BJ14" s="49"/>
       <c r="BK14" s="49"/>
-      <c r="BL14" s="50"/>
-      <c r="BM14" s="51"/>
+      <c r="BL14" s="51"/>
+      <c r="BM14" s="52"/>
       <c r="BN14" s="43"/>
       <c r="BO14" s="44" t="n">
         <v>1</v>
@@ -6059,38 +6191,38 @@
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="35" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="53" t="n">
-        <f aca="false">[1]Netzplan!G15</f>
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="G15" s="55" t="n">
+        <f aca="false">[1]Netzplan!G14</f>
+        <v>3</v>
       </c>
       <c r="H15" s="31" t="str">
-        <f aca="false">Netzplan!H15</f>
+        <f aca="false">Netzplan!H14</f>
         <v>2</v>
       </c>
       <c r="I15" s="28" t="n">
-        <f aca="false">Netzplan!I15</f>
+        <f aca="false">Netzplan!I14</f>
         <v>0.75</v>
       </c>
       <c r="J15" s="46" t="n">
         <f aca="false">ROUND(G15/(H15*I15),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="47" t="n">
         <f aca="false">SUM(L15:BM15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="49"/>
       <c r="M15" s="49"/>
@@ -6110,44 +6242,45 @@
       <c r="AA15" s="49"/>
       <c r="AB15" s="49"/>
       <c r="AC15" s="49"/>
-      <c r="AD15" s="49"/>
+      <c r="AD15" s="50"/>
       <c r="AE15" s="49"/>
       <c r="AF15" s="49"/>
       <c r="AG15" s="49"/>
       <c r="AH15" s="49"/>
       <c r="AI15" s="49"/>
       <c r="AJ15" s="49"/>
-      <c r="AK15" s="49"/>
       <c r="AL15" s="49"/>
       <c r="AM15" s="49"/>
-      <c r="AN15" s="49"/>
+      <c r="AN15" s="49" t="n">
+        <v>1</v>
+      </c>
       <c r="AO15" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="AP15" s="49"/>
-      <c r="AQ15" s="49"/>
-      <c r="AR15" s="49"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="53"/>
+      <c r="AR15" s="53"/>
       <c r="AS15" s="49"/>
       <c r="AT15" s="49"/>
-      <c r="AU15" s="49"/>
-      <c r="AV15" s="52"/>
-      <c r="AW15" s="49"/>
+      <c r="AU15" s="53"/>
+      <c r="AV15" s="53"/>
+      <c r="AW15" s="53"/>
       <c r="AX15" s="49"/>
-      <c r="AY15" s="50"/>
+      <c r="AY15" s="51"/>
       <c r="AZ15" s="49"/>
       <c r="BA15" s="49"/>
       <c r="BB15" s="49"/>
       <c r="BC15" s="49"/>
       <c r="BD15" s="49"/>
       <c r="BE15" s="49"/>
-      <c r="BF15" s="50"/>
+      <c r="BF15" s="51"/>
       <c r="BG15" s="49"/>
       <c r="BH15" s="49"/>
       <c r="BI15" s="49"/>
       <c r="BJ15" s="49"/>
       <c r="BK15" s="49"/>
-      <c r="BL15" s="50"/>
-      <c r="BM15" s="51"/>
+      <c r="BL15" s="51"/>
+      <c r="BM15" s="52"/>
       <c r="BN15" s="43"/>
       <c r="BO15" s="44" t="n">
         <v>1</v>
@@ -6156,40 +6289,40 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="35" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="53" t="n">
-        <f aca="false">[1]Netzplan!G16</f>
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="G16" s="55" t="n">
+        <f aca="false">[1]Netzplan!G15</f>
+        <v>1</v>
       </c>
       <c r="H16" s="31" t="str">
-        <f aca="false">Netzplan!H16</f>
+        <f aca="false">Netzplan!H15</f>
         <v>2</v>
       </c>
       <c r="I16" s="28" t="n">
-        <f aca="false">Netzplan!I16</f>
+        <f aca="false">Netzplan!I15</f>
         <v>0.75</v>
       </c>
       <c r="J16" s="46" t="n">
         <f aca="false">ROUND(G16/(H16*I16),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K16" s="47" t="n">
         <f aca="false">SUM(L16:BM16)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L16" s="49"/>
       <c r="M16" s="49"/>
@@ -6209,7 +6342,7 @@
       <c r="AA16" s="49"/>
       <c r="AB16" s="49"/>
       <c r="AC16" s="49"/>
-      <c r="AD16" s="49"/>
+      <c r="AD16" s="50"/>
       <c r="AE16" s="49"/>
       <c r="AF16" s="49"/>
       <c r="AG16" s="49"/>
@@ -6220,37 +6353,31 @@
       <c r="AL16" s="49"/>
       <c r="AM16" s="49"/>
       <c r="AN16" s="49"/>
-      <c r="AO16" s="49"/>
-      <c r="AP16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ16" s="49" t="n">
-        <v>1</v>
-      </c>
+      <c r="AQ16" s="49"/>
       <c r="AR16" s="49" t="n">
         <v>1</v>
       </c>
       <c r="AS16" s="49"/>
       <c r="AT16" s="49"/>
       <c r="AU16" s="49"/>
-      <c r="AV16" s="49"/>
-      <c r="AW16" s="52"/>
-      <c r="AX16" s="52"/>
-      <c r="AY16" s="50"/>
+      <c r="AV16" s="53"/>
+      <c r="AW16" s="49"/>
+      <c r="AX16" s="49"/>
+      <c r="AY16" s="51"/>
       <c r="AZ16" s="49"/>
       <c r="BA16" s="49"/>
-      <c r="BB16" s="52"/>
-      <c r="BC16" s="52"/>
-      <c r="BD16" s="52"/>
+      <c r="BB16" s="49"/>
+      <c r="BC16" s="49"/>
+      <c r="BD16" s="49"/>
       <c r="BE16" s="49"/>
-      <c r="BF16" s="50"/>
+      <c r="BF16" s="51"/>
       <c r="BG16" s="49"/>
       <c r="BH16" s="49"/>
       <c r="BI16" s="49"/>
-      <c r="BJ16" s="54"/>
+      <c r="BJ16" s="49"/>
       <c r="BK16" s="49"/>
-      <c r="BL16" s="50"/>
-      <c r="BM16" s="51"/>
+      <c r="BL16" s="51"/>
+      <c r="BM16" s="52"/>
       <c r="BN16" s="43"/>
       <c r="BO16" s="44" t="n">
         <v>1</v>
@@ -6259,103 +6386,203 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="38"/>
       <c r="G17" s="55" t="n">
-        <f aca="false">[1]Netzplan!G17</f>
-        <v>1</v>
+        <f aca="false">[1]Netzplan!G16</f>
+        <v>5</v>
       </c>
       <c r="H17" s="31" t="str">
-        <f aca="false">Netzplan!H17</f>
-        <v>1</v>
+        <f aca="false">Netzplan!H16</f>
+        <v>2</v>
       </c>
       <c r="I17" s="28" t="n">
-        <f aca="false">Netzplan!I17</f>
-        <v>1</v>
+        <f aca="false">Netzplan!I16</f>
+        <v>0.75</v>
       </c>
       <c r="J17" s="46" t="n">
         <f aca="false">ROUND(G17/(H17*I17),0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="47" t="n">
         <f aca="false">SUM(L17:BM17)</f>
-        <v>1</v>
-      </c>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
-      <c r="Y17" s="56"/>
-      <c r="Z17" s="56"/>
-      <c r="AA17" s="56"/>
-      <c r="AB17" s="56"/>
-      <c r="AC17" s="56"/>
-      <c r="AD17" s="56"/>
-      <c r="AE17" s="56"/>
-      <c r="AF17" s="56"/>
-      <c r="AG17" s="56"/>
-      <c r="AH17" s="56"/>
-      <c r="AI17" s="56"/>
-      <c r="AJ17" s="56"/>
-      <c r="AK17" s="56"/>
-      <c r="AL17" s="56"/>
-      <c r="AM17" s="56"/>
-      <c r="AN17" s="56"/>
-      <c r="AO17" s="56"/>
-      <c r="AP17" s="56"/>
-      <c r="AQ17" s="56"/>
-      <c r="AR17" s="56"/>
-      <c r="AS17" s="56"/>
-      <c r="AT17" s="56"/>
-      <c r="AU17" s="56"/>
-      <c r="AV17" s="56"/>
-      <c r="AW17" s="56"/>
-      <c r="AX17" s="56"/>
-      <c r="AY17" s="57"/>
-      <c r="AZ17" s="56"/>
-      <c r="BA17" s="56"/>
-      <c r="BB17" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC17" s="52"/>
-      <c r="BD17" s="56"/>
-      <c r="BE17" s="56"/>
-      <c r="BF17" s="57"/>
-      <c r="BG17" s="56"/>
-      <c r="BH17" s="56"/>
-      <c r="BI17" s="56"/>
-      <c r="BJ17" s="56"/>
-      <c r="BK17" s="56"/>
-      <c r="BL17" s="57"/>
-      <c r="BM17" s="58"/>
+        <v>3</v>
+      </c>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="49"/>
+      <c r="AG17" s="49"/>
+      <c r="AH17" s="49"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
+      <c r="AK17" s="49"/>
+      <c r="AL17" s="49"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="49"/>
+      <c r="AO17" s="49"/>
+      <c r="AS17" s="49"/>
+      <c r="AT17" s="49"/>
+      <c r="AU17" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX17" s="53"/>
+      <c r="AY17" s="51"/>
+      <c r="AZ17" s="49"/>
+      <c r="BA17" s="49"/>
+      <c r="BB17" s="53"/>
+      <c r="BC17" s="53"/>
+      <c r="BD17" s="53"/>
+      <c r="BE17" s="49"/>
+      <c r="BF17" s="51"/>
+      <c r="BG17" s="49"/>
+      <c r="BH17" s="49"/>
+      <c r="BI17" s="49"/>
+      <c r="BJ17" s="58"/>
+      <c r="BK17" s="49"/>
+      <c r="BL17" s="51"/>
+      <c r="BM17" s="52"/>
       <c r="BN17" s="43"/>
       <c r="BO17" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="BP17" s="45"/>
+      <c r="BP17" s="45" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="59" t="n">
+        <f aca="false">[1]Netzplan!G17</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="31" t="str">
+        <f aca="false">Netzplan!H17</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="28" t="n">
+        <f aca="false">Netzplan!I17</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="46" t="n">
+        <f aca="false">ROUND(G18/(H18*I18),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="47" t="n">
+        <f aca="false">SUM(L18:BM18)</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="60"/>
+      <c r="AF18" s="60"/>
+      <c r="AG18" s="60"/>
+      <c r="AH18" s="60"/>
+      <c r="AI18" s="60"/>
+      <c r="AJ18" s="60"/>
+      <c r="AK18" s="60"/>
+      <c r="AL18" s="60"/>
+      <c r="AM18" s="60"/>
+      <c r="AN18" s="60"/>
+      <c r="AO18" s="60"/>
+      <c r="AP18" s="60"/>
+      <c r="AQ18" s="60"/>
+      <c r="AR18" s="60"/>
+      <c r="AS18" s="60"/>
+      <c r="AT18" s="60"/>
+      <c r="AU18" s="60"/>
+      <c r="AV18" s="60"/>
+      <c r="AW18" s="60"/>
+      <c r="AX18" s="60"/>
+      <c r="AY18" s="62"/>
+      <c r="AZ18" s="60"/>
+      <c r="BA18" s="60"/>
+      <c r="BB18" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="53"/>
+      <c r="BD18" s="60"/>
+      <c r="BE18" s="60"/>
+      <c r="BF18" s="62"/>
+      <c r="BG18" s="60"/>
+      <c r="BH18" s="60"/>
+      <c r="BI18" s="60"/>
+      <c r="BJ18" s="60"/>
+      <c r="BK18" s="60"/>
+      <c r="BL18" s="62"/>
+      <c r="BM18" s="63"/>
+      <c r="BN18" s="43"/>
+      <c r="BO18" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP18" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -6373,18 +6600,19 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
-  <conditionalFormatting sqref="AV15:BM15 L10:AH12 BF12:BH12 BJ12:BM12 BK16:BM16 L13:AJ13 L14:AO14 L15:AT15 L17:BM17 AI10:BM10 AJ11:BM11 AL13:BM13 AQ14:BM14 AW16:BI16 L16:AO16 AQ16:AU16 L1:BM9 AI12:BA12">
+  <conditionalFormatting sqref="AV16:BM16 L13:AH15 BF13:BH13 BJ13:BM13 BK17:BM17 L18:BM18 AJ11:BM11 AJ12:BM12 AP14:BM14 AQ15:BM15 AW17:BI17 L17:AO17 AS17:AU17 L1:BM8 AI13:BA13 L10:AC10 AE10:BM10 L11:AF13 AH11:AI12 AO14:AO15 AL15:AN15 AJ14:AN14 AI15:AJ15 L16:AN16 AQ16:AT16 L9:S9 W9:BM9">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>IF(OR(WEEKDAY(L$1)=7,WEEKDAY(L$1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:BM17">
+  <conditionalFormatting sqref="L2:BM8 L10:AC10 AE10:BM10 L11:AF12 AH11:BM12 L13:BM13 L18:BM18 L14:AH14 AJ14:BM14 L15:AJ15 AL15:BM15 L16:AN16 L17:AO17 AQ16:BM16 AS17:BM17 L9:S9 W9:BM9">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K17">
+  <conditionalFormatting sqref="K2:K18">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>IF(K2&lt;&gt;J2,TRUE())</formula>
     </cfRule>
@@ -6396,5 +6624,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Online Projekt Gantt Lösung
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
+++ b/FIAEB Übungen/Online_Shop.Projekt_FIAE_B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAEB Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839808C0-98EC-478B-96E5-95EBF66AE71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A06BF4-DD89-46FD-9D23-136B20E3793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,12 +388,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FFE8E8E8"/>
       </patternFill>
@@ -468,6 +462,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -857,10 +857,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,6 +884,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,12 +918,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -933,12 +929,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,13 +947,10 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -978,6 +974,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -991,27 +1005,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1026,12 +1022,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gantt-Balken" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1314,251 +1314,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>134280</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Freihandform: Form 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11856600" y="1647720"/>
-          <a:ext cx="126000" cy="155160"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="10800" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="21600"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="0"/>
-              </a:lnTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="729FCF"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465A4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Freihandform: Form 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13880520" y="2462040"/>
-          <a:ext cx="126000" cy="155160"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="10800" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="21600"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="0"/>
-              </a:lnTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="729FCF"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465A4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>128880</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Freihandform: Form 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000030000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17172000" y="2949480"/>
-          <a:ext cx="126000" cy="155160"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="21600" h="21600">
-              <a:moveTo>
-                <a:pt x="10800" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="21600" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="21600"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="10800"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="10800" y="0"/>
-              </a:lnTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="729FCF"/>
-        </a:solidFill>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465A4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1870,20 +1625,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="83"/>
+      <c r="I1" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="81"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -1892,10 +1647,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="47">
-        <v>1</v>
-      </c>
-      <c r="J2" s="46" t="s">
+      <c r="I2" s="45">
+        <v>1</v>
+      </c>
+      <c r="J2" s="44" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="4"/>
@@ -1904,238 +1659,238 @@
     </row>
     <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F3" s="4"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="41"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="44"/>
+      <c r="I4" s="42"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="44"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="24.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="85"/>
+      <c r="G5" s="83"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="86" t="s">
+      <c r="I5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="87"/>
+      <c r="J5" s="85"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="88" t="s">
+      <c r="L5" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="89"/>
+      <c r="M5" s="87"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="47" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="51" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="56" t="s">
+      <c r="L6" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="55" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="F7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="L7" s="40"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="I8" s="92" t="s">
+      <c r="G8" s="89"/>
+      <c r="I8" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="L8" s="94" t="s">
+      <c r="J8" s="91"/>
+      <c r="L8" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="95"/>
+      <c r="M8" s="93"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="L10" s="42"/>
+      <c r="F10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="L10" s="40"/>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="90" t="s">
+      <c r="F11" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="91"/>
-      <c r="I11" s="92" t="s">
+      <c r="G11" s="89"/>
+      <c r="I11" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="93"/>
-      <c r="L11" s="94" t="s">
+      <c r="J11" s="91"/>
+      <c r="L11" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="95"/>
+      <c r="M11" s="93"/>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="55" t="s">
+      <c r="J12" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="59" t="s">
+      <c r="M12" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="L13" s="42"/>
+      <c r="F13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="L13" s="40"/>
     </row>
     <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="I14" s="92" t="s">
+      <c r="G14" s="89"/>
+      <c r="I14" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="93"/>
-      <c r="L14" s="94" t="s">
+      <c r="J14" s="91"/>
+      <c r="L14" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="95"/>
+      <c r="M14" s="93"/>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="58" t="s">
+      <c r="L15" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="F16" s="40"/>
+      <c r="I16" s="40"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="90" t="s">
+      <c r="F17" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="91"/>
-      <c r="I17" s="92" t="s">
+      <c r="G17" s="89"/>
+      <c r="I17" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="93"/>
+      <c r="J17" s="91"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="54" t="s">
+      <c r="I18" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="55" t="s">
+      <c r="J18" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="42"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I20" s="92" t="s">
+      <c r="I20" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="93"/>
+      <c r="J20" s="91"/>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I21" s="54" t="s">
+      <c r="I21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="55" t="s">
+      <c r="J21" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="42"/>
+      <c r="I22" s="40"/>
     </row>
     <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="92" t="s">
+      <c r="I23" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="93"/>
+      <c r="J23" s="91"/>
     </row>
     <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I24" s="54" t="s">
+      <c r="I24" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="55" t="s">
+      <c r="J24" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2143,46 +1898,46 @@
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="96" t="s">
+      <c r="B25" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="I25" s="42"/>
+      <c r="I25" s="40"/>
     </row>
     <row r="26" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="I26" s="92" t="s">
+      <c r="I26" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="J26" s="93"/>
+      <c r="J26" s="91"/>
     </row>
     <row r="27" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="I27" s="54" t="s">
+      <c r="I27" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="55" t="s">
+      <c r="J27" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2190,46 +1945,46 @@
       <c r="A28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
-      <c r="I28" s="42"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="I29" s="92" t="s">
+      <c r="I29" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="93"/>
+      <c r="J29" s="91"/>
     </row>
     <row r="30" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="I30" s="54" t="s">
+      <c r="I30" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="J30" s="55" t="s">
+      <c r="J30" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2237,46 +1992,46 @@
       <c r="A31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="96"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="I31" s="42"/>
+      <c r="I31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="98" t="s">
+      <c r="B32" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="I32" s="92" t="s">
+      <c r="I32" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="93"/>
+      <c r="J32" s="91"/>
     </row>
     <row r="33" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="I33" s="54" t="s">
+      <c r="I33" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="55" t="s">
+      <c r="J33" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2284,11 +2039,11 @@
       <c r="A34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="98" t="s">
+      <c r="B34" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="96"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
@@ -2296,11 +2051,11 @@
       <c r="A35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="98" t="s">
+      <c r="B35" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="98"/>
-      <c r="D35" s="98"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
@@ -2308,11 +2063,11 @@
       <c r="A36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="98" t="s">
+      <c r="B36" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
@@ -2320,11 +2075,11 @@
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
@@ -2332,11 +2087,11 @@
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="98" t="s">
+      <c r="B38" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
@@ -2344,11 +2099,11 @@
       <c r="A39" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
@@ -2356,11 +2111,11 @@
       <c r="A40" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="98"/>
-      <c r="D40" s="98"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
@@ -2368,11 +2123,11 @@
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="99" t="s">
+      <c r="B41" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
+      <c r="C41" s="97"/>
+      <c r="D41" s="97"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
@@ -2430,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ23"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AV4" sqref="AV4"/>
+    <sheetView topLeftCell="P2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3:AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2448,11 +2203,11 @@
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="14" t="s">
         <v>46</v>
       </c>
@@ -2476,11 +2231,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17" t="s">
         <v>52</v>
@@ -2488,7 +2243,7 @@
       <c r="G2" s="18">
         <v>5</v>
       </c>
-      <c r="H2" s="78">
+      <c r="H2" s="76">
         <v>3</v>
       </c>
       <c r="I2" s="19">
@@ -2498,101 +2253,101 @@
         <f t="shared" ref="J2:J17" si="0">ROUND(G2/(H2*I2),0)</f>
         <v>2</v>
       </c>
-      <c r="L2" s="69">
+      <c r="L2" s="67">
         <v>0</v>
       </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="73">
+      <c r="M2" s="68"/>
+      <c r="N2" s="71">
         <f>L2+L4</f>
         <v>2</v>
       </c>
-      <c r="Q2" s="69">
+      <c r="Q2" s="67">
         <f>N2</f>
         <v>2</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="73">
+      <c r="R2" s="68"/>
+      <c r="S2" s="71">
         <f>Q2+Q4</f>
         <v>3</v>
       </c>
-      <c r="V2" s="69">
+      <c r="V2" s="67">
         <f>S2</f>
         <v>3</v>
       </c>
-      <c r="W2" s="70"/>
-      <c r="X2" s="73">
+      <c r="W2" s="68"/>
+      <c r="X2" s="71">
         <f>V2+V4</f>
         <v>6</v>
       </c>
-      <c r="AF2" s="69">
+      <c r="AF2" s="67">
         <f>MAX(X2,AC8,X14)</f>
         <v>10</v>
       </c>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="73">
+      <c r="AG2" s="68"/>
+      <c r="AH2" s="71">
         <f>AF2+AF4</f>
         <v>12</v>
       </c>
-      <c r="AK2" s="69">
+      <c r="AK2" s="67">
         <f>AH2</f>
         <v>12</v>
       </c>
-      <c r="AL2" s="70"/>
-      <c r="AM2" s="73">
+      <c r="AL2" s="68"/>
+      <c r="AM2" s="71">
         <f>AK2+AK4</f>
         <v>14</v>
       </c>
-      <c r="AP2" s="69">
+      <c r="AP2" s="67">
         <f>AM2</f>
         <v>14</v>
       </c>
-      <c r="AQ2" s="70"/>
-      <c r="AR2" s="73">
+      <c r="AQ2" s="68"/>
+      <c r="AR2" s="71">
         <f>AP2+AP4</f>
         <v>16</v>
       </c>
-      <c r="AU2" s="69">
+      <c r="AU2" s="67">
         <f>AR2</f>
         <v>16</v>
       </c>
-      <c r="AV2" s="70"/>
-      <c r="AW2" s="73">
+      <c r="AV2" s="68"/>
+      <c r="AW2" s="71">
         <f>AU2+AU4</f>
         <v>19</v>
       </c>
-      <c r="AZ2" s="69">
+      <c r="AZ2" s="67">
         <f>AW2</f>
         <v>19</v>
       </c>
-      <c r="BA2" s="70"/>
-      <c r="BB2" s="73">
+      <c r="BA2" s="68"/>
+      <c r="BB2" s="71">
         <f>AZ2+AZ4</f>
         <v>22</v>
       </c>
-      <c r="BE2" s="69">
+      <c r="BE2" s="67">
         <f>BB2</f>
         <v>22</v>
       </c>
-      <c r="BF2" s="70"/>
-      <c r="BG2" s="73">
+      <c r="BF2" s="68"/>
+      <c r="BG2" s="71">
         <f>BE2+BE4</f>
         <v>23</v>
       </c>
-      <c r="BJ2" s="69">
+      <c r="BJ2" s="67">
         <f>BG2</f>
         <v>23</v>
       </c>
-      <c r="BK2" s="70"/>
-      <c r="BL2" s="73">
+      <c r="BK2" s="68"/>
+      <c r="BL2" s="71">
         <f>BJ2+BJ4</f>
         <v>28</v>
       </c>
-      <c r="BO2" s="69">
+      <c r="BO2" s="67">
         <f>MAX(BL2,AC14)</f>
         <v>29</v>
       </c>
-      <c r="BP2" s="70"/>
-      <c r="BQ2" s="73">
+      <c r="BP2" s="68"/>
+      <c r="BQ2" s="71">
         <f>BO2+BO4</f>
         <v>30</v>
       </c>
@@ -2601,11 +2356,11 @@
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
       <c r="E3" s="20" t="s">
         <v>16</v>
       </c>
@@ -2615,7 +2370,7 @@
       <c r="G3" s="21">
         <v>1</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="77">
         <v>2</v>
       </c>
       <c r="I3" s="22">
@@ -2625,96 +2380,96 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L3" s="100" t="s">
+      <c r="L3" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="100" t="s">
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="100" t="s">
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="100"/>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="100" t="s">
+      <c r="W3" s="98"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="100"/>
-      <c r="AH3" s="100"/>
-      <c r="AI3" s="60"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="100" t="s">
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="100"/>
-      <c r="AM3" s="100"/>
-      <c r="AN3" s="60"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="100" t="s">
+      <c r="AL3" s="98"/>
+      <c r="AM3" s="98"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="AQ3" s="100"/>
-      <c r="AR3" s="100"/>
-      <c r="AS3" s="60"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="100" t="s">
+      <c r="AQ3" s="98"/>
+      <c r="AR3" s="98"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="AV3" s="100"/>
-      <c r="AW3" s="100"/>
-      <c r="AX3" s="60"/>
-      <c r="AY3" s="61"/>
-      <c r="AZ3" s="100" t="s">
+      <c r="AV3" s="98"/>
+      <c r="AW3" s="98"/>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="BA3" s="100"/>
-      <c r="BB3" s="100"/>
-      <c r="BC3" s="60"/>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="100" t="s">
+      <c r="BA3" s="98"/>
+      <c r="BB3" s="98"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="59"/>
+      <c r="BE3" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="BF3" s="100"/>
-      <c r="BG3" s="100"/>
-      <c r="BH3" s="60"/>
-      <c r="BI3" s="61"/>
-      <c r="BJ3" s="100" t="s">
+      <c r="BF3" s="98"/>
+      <c r="BG3" s="98"/>
+      <c r="BH3" s="58"/>
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="BK3" s="100"/>
-      <c r="BL3" s="100"/>
-      <c r="BM3" s="60"/>
-      <c r="BN3" s="61"/>
-      <c r="BO3" s="100" t="s">
+      <c r="BK3" s="98"/>
+      <c r="BL3" s="98"/>
+      <c r="BM3" s="58"/>
+      <c r="BN3" s="59"/>
+      <c r="BO3" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="BP3" s="100"/>
-      <c r="BQ3" s="100"/>
+      <c r="BP3" s="98"/>
+      <c r="BQ3" s="98"/>
     </row>
     <row r="4" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
@@ -2724,7 +2479,7 @@
       <c r="G4" s="21">
         <v>4</v>
       </c>
-      <c r="H4" s="79">
+      <c r="H4" s="77">
         <v>2</v>
       </c>
       <c r="I4" s="22">
@@ -2735,149 +2490,149 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L4" s="74">
+      <c r="L4" s="72">
         <f>J2</f>
         <v>2</v>
       </c>
-      <c r="M4" s="75">
+      <c r="M4" s="73">
         <f>N5-N2</f>
         <v>0</v>
       </c>
-      <c r="N4" s="76">
+      <c r="N4" s="74">
         <f>MIN(Q2,Q14)-N2</f>
         <v>0</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="Q4" s="74">
+      <c r="O4" s="41"/>
+      <c r="Q4" s="72">
         <f>J3</f>
         <v>1</v>
       </c>
-      <c r="R4" s="75">
+      <c r="R4" s="73">
         <f>S5-S2</f>
         <v>1</v>
       </c>
-      <c r="S4" s="76">
+      <c r="S4" s="74">
         <f>MIN(V2,V8)-S2</f>
         <v>0</v>
       </c>
-      <c r="T4" s="43"/>
-      <c r="V4" s="74">
+      <c r="T4" s="41"/>
+      <c r="V4" s="72">
         <f>J4</f>
         <v>3</v>
       </c>
-      <c r="W4" s="75">
+      <c r="W4" s="73">
         <f>X5-X2</f>
         <v>5</v>
       </c>
-      <c r="X4" s="76">
+      <c r="X4" s="74">
         <f>AF2-X2</f>
         <v>4</v>
       </c>
-      <c r="AE4" s="67"/>
-      <c r="AF4" s="74">
+      <c r="AE4" s="65"/>
+      <c r="AF4" s="72">
         <f>J9</f>
         <v>2</v>
       </c>
-      <c r="AG4" s="75">
+      <c r="AG4" s="73">
         <f>AH5-AH2</f>
         <v>1</v>
       </c>
-      <c r="AH4" s="76">
+      <c r="AH4" s="74">
         <f>AK2-AH2</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="74">
+      <c r="AK4" s="72">
         <f>J10</f>
         <v>2</v>
       </c>
-      <c r="AL4" s="75">
+      <c r="AL4" s="73">
         <f>AM5-AM2</f>
         <v>1</v>
       </c>
-      <c r="AM4" s="76">
+      <c r="AM4" s="74">
         <f>AP2-AM2</f>
         <v>0</v>
       </c>
-      <c r="AP4" s="74">
+      <c r="AP4" s="72">
         <f>J11</f>
         <v>2</v>
       </c>
-      <c r="AQ4" s="75">
+      <c r="AQ4" s="73">
         <f>AR5-AR2</f>
         <v>1</v>
       </c>
-      <c r="AR4" s="76">
+      <c r="AR4" s="74">
         <f>AU2-AR2</f>
         <v>0</v>
       </c>
-      <c r="AU4" s="74">
+      <c r="AU4" s="72">
         <f>J13</f>
         <v>3</v>
       </c>
-      <c r="AV4" s="75">
+      <c r="AV4" s="73">
         <f>AW5-AW2</f>
         <v>1</v>
       </c>
-      <c r="AW4" s="76">
+      <c r="AW4" s="74">
         <f>AZ2-AW2</f>
         <v>0</v>
       </c>
-      <c r="AZ4" s="74">
+      <c r="AZ4" s="72">
         <f>J14</f>
         <v>3</v>
       </c>
-      <c r="BA4" s="75">
+      <c r="BA4" s="73">
         <f>BB5-BB2</f>
         <v>1</v>
       </c>
-      <c r="BB4" s="76">
+      <c r="BB4" s="74">
         <f>BE2-BB2</f>
         <v>0</v>
       </c>
-      <c r="BE4" s="74">
+      <c r="BE4" s="72">
         <f>J15</f>
         <v>1</v>
       </c>
-      <c r="BF4" s="75">
+      <c r="BF4" s="73">
         <f>BG5-BG2</f>
         <v>1</v>
       </c>
-      <c r="BG4" s="76">
+      <c r="BG4" s="74">
         <f>BJ2-BG2</f>
         <v>0</v>
       </c>
-      <c r="BJ4" s="74">
+      <c r="BJ4" s="72">
         <f>J16</f>
         <v>5</v>
       </c>
-      <c r="BK4" s="75">
+      <c r="BK4" s="73">
         <f>BL5-BL2</f>
         <v>1</v>
       </c>
-      <c r="BL4" s="76">
+      <c r="BL4" s="74">
         <f>BO2-BL2</f>
         <v>1</v>
       </c>
-      <c r="BN4" s="61"/>
-      <c r="BO4" s="74">
+      <c r="BN4" s="59"/>
+      <c r="BO4" s="72">
         <f>J17</f>
         <v>1</v>
       </c>
-      <c r="BP4" s="75">
+      <c r="BP4" s="73">
         <f>BQ5-BQ2</f>
         <v>0</v>
       </c>
-      <c r="BQ4" s="76"/>
+      <c r="BQ4" s="74"/>
     </row>
     <row r="5" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
@@ -2887,7 +2642,7 @@
       <c r="G5" s="21">
         <v>3</v>
       </c>
-      <c r="H5" s="79">
+      <c r="H5" s="77">
         <v>1</v>
       </c>
       <c r="I5" s="22">
@@ -2897,106 +2652,106 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L5" s="71">
+      <c r="L5" s="69">
         <f>N5-L4</f>
         <v>0</v>
       </c>
-      <c r="M5" s="70"/>
-      <c r="N5" s="72">
+      <c r="M5" s="68"/>
+      <c r="N5" s="70">
         <f>MIN(Q5,Q17)</f>
         <v>2</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="Q5" s="71">
+      <c r="O5" s="60"/>
+      <c r="Q5" s="69">
         <f>S5-Q4</f>
         <v>3</v>
       </c>
-      <c r="R5" s="70"/>
-      <c r="S5" s="72">
+      <c r="R5" s="68"/>
+      <c r="S5" s="70">
         <f>MIN(V5,V11)</f>
         <v>4</v>
       </c>
-      <c r="T5" s="62"/>
-      <c r="V5" s="71">
+      <c r="T5" s="60"/>
+      <c r="V5" s="69">
         <f>X5-V4</f>
         <v>8</v>
       </c>
-      <c r="W5" s="70"/>
-      <c r="X5" s="72">
+      <c r="W5" s="68"/>
+      <c r="X5" s="70">
         <f>AF5</f>
         <v>11</v>
       </c>
-      <c r="AD5" s="62"/>
-      <c r="AF5" s="71">
+      <c r="AD5" s="60"/>
+      <c r="AF5" s="69">
         <f>AH5-AF4</f>
         <v>11</v>
       </c>
-      <c r="AG5" s="70"/>
-      <c r="AH5" s="72">
+      <c r="AG5" s="68"/>
+      <c r="AH5" s="70">
         <f>AK5</f>
         <v>13</v>
       </c>
-      <c r="AK5" s="71">
+      <c r="AK5" s="69">
         <f>AM5-AK4</f>
         <v>13</v>
       </c>
-      <c r="AL5" s="70"/>
-      <c r="AM5" s="72">
+      <c r="AL5" s="68"/>
+      <c r="AM5" s="70">
         <f>AP5</f>
         <v>15</v>
       </c>
-      <c r="AP5" s="71">
+      <c r="AP5" s="69">
         <f>AR5-AP4</f>
         <v>15</v>
       </c>
-      <c r="AQ5" s="70"/>
-      <c r="AR5" s="72">
+      <c r="AQ5" s="68"/>
+      <c r="AR5" s="70">
         <f>AU5</f>
         <v>17</v>
       </c>
-      <c r="AU5" s="71">
+      <c r="AU5" s="69">
         <f>AW5-AU4</f>
         <v>17</v>
       </c>
-      <c r="AV5" s="70"/>
-      <c r="AW5" s="72">
+      <c r="AV5" s="68"/>
+      <c r="AW5" s="70">
         <f>AZ5</f>
         <v>20</v>
       </c>
-      <c r="AZ5" s="71">
+      <c r="AZ5" s="69">
         <f>BB5-AZ4</f>
         <v>20</v>
       </c>
-      <c r="BA5" s="70"/>
-      <c r="BB5" s="72">
+      <c r="BA5" s="68"/>
+      <c r="BB5" s="70">
         <f>BE5</f>
         <v>23</v>
       </c>
-      <c r="BE5" s="71">
+      <c r="BE5" s="69">
         <f>BG5-BE4</f>
         <v>23</v>
       </c>
-      <c r="BF5" s="70"/>
-      <c r="BG5" s="72">
+      <c r="BF5" s="68"/>
+      <c r="BG5" s="70">
         <f>BJ5</f>
         <v>24</v>
       </c>
-      <c r="BJ5" s="71">
+      <c r="BJ5" s="69">
         <f>BL5-BJ4</f>
         <v>24</v>
       </c>
-      <c r="BK5" s="70"/>
-      <c r="BL5" s="72">
+      <c r="BK5" s="68"/>
+      <c r="BL5" s="70">
         <f>BO5</f>
         <v>29</v>
       </c>
-      <c r="BM5" s="62"/>
-      <c r="BO5" s="71">
+      <c r="BM5" s="60"/>
+      <c r="BO5" s="69">
         <f>BQ5-BO4</f>
         <v>29</v>
       </c>
-      <c r="BP5" s="70"/>
-      <c r="BQ5" s="72">
+      <c r="BP5" s="68"/>
+      <c r="BQ5" s="70">
         <f>BQ2</f>
         <v>30</v>
       </c>
@@ -3005,11 +2760,11 @@
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="23" t="s">
         <v>27</v>
       </c>
@@ -3019,7 +2774,7 @@
       <c r="G6" s="1">
         <v>7</v>
       </c>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="22">
@@ -3029,21 +2784,21 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="O6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="AD6" s="62"/>
-      <c r="AE6" s="62"/>
-      <c r="BM6" s="62"/>
+      <c r="O6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="60"/>
+      <c r="BM6" s="60"/>
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
       <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
@@ -3053,7 +2808,7 @@
       <c r="G7" s="21">
         <v>1</v>
       </c>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I7" s="22">
@@ -3063,21 +2818,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="AD7" s="62"/>
-      <c r="AE7" s="62"/>
-      <c r="BM7" s="62"/>
+      <c r="O7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="BM7" s="60"/>
     </row>
     <row r="8" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="23" t="s">
         <v>22</v>
       </c>
@@ -3087,7 +2842,7 @@
       <c r="G8" s="1">
         <v>3</v>
       </c>
-      <c r="H8" s="79" t="s">
+      <c r="H8" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I8" s="22">
@@ -3097,39 +2852,39 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="O8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="V8" s="69">
+      <c r="O8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="V8" s="67">
         <f>S2</f>
         <v>3</v>
       </c>
-      <c r="W8" s="70"/>
-      <c r="X8" s="73">
+      <c r="W8" s="68"/>
+      <c r="X8" s="71">
         <f>V8+V10</f>
         <v>5</v>
       </c>
-      <c r="AA8" s="69">
+      <c r="AA8" s="67">
         <f>X8</f>
         <v>5</v>
       </c>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="73">
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="71">
         <f>AA8+AA10</f>
         <v>10</v>
       </c>
-      <c r="AD8" s="62"/>
-      <c r="AE8" s="62"/>
-      <c r="BM8" s="62"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="60"/>
+      <c r="BM8" s="60"/>
     </row>
     <row r="9" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
       <c r="E9" s="23" t="s">
         <v>56</v>
       </c>
@@ -3139,7 +2894,7 @@
       <c r="G9" s="1">
         <v>2</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I9" s="22">
@@ -3149,33 +2904,33 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="V9" s="100" t="s">
+      <c r="O9" s="60"/>
+      <c r="T9" s="60"/>
+      <c r="V9" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="W9" s="100"/>
-      <c r="X9" s="100"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="100" t="s">
+      <c r="W9" s="98"/>
+      <c r="X9" s="98"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="59"/>
+      <c r="AA9" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="AB9" s="100"/>
-      <c r="AC9" s="100"/>
-      <c r="AD9" s="66"/>
-      <c r="AE9" s="62"/>
-      <c r="BM9" s="62"/>
+      <c r="AB9" s="98"/>
+      <c r="AC9" s="98"/>
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="60"/>
+      <c r="BM9" s="60"/>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
       <c r="E10" s="23" t="s">
         <v>33</v>
       </c>
@@ -3185,7 +2940,7 @@
       <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="79" t="s">
+      <c r="H10" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I10" s="22">
@@ -3195,44 +2950,44 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O10" s="62"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="74">
+      <c r="O10" s="60"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="72">
         <f>J5</f>
         <v>2</v>
       </c>
-      <c r="W10" s="75">
+      <c r="W10" s="73">
         <f>X11-X8</f>
         <v>1</v>
       </c>
-      <c r="X10" s="76">
+      <c r="X10" s="74">
         <f>AA8-X8</f>
         <v>0</v>
       </c>
-      <c r="AA10" s="74">
+      <c r="AA10" s="72">
         <f>J6</f>
         <v>5</v>
       </c>
-      <c r="AB10" s="75">
+      <c r="AB10" s="73">
         <f>AC11-AC8</f>
         <v>1</v>
       </c>
-      <c r="AC10" s="76">
+      <c r="AC10" s="74">
         <f>AF2-AC8</f>
         <v>0</v>
       </c>
-      <c r="AE10" s="62"/>
-      <c r="BM10" s="62"/>
+      <c r="AE10" s="60"/>
+      <c r="BM10" s="60"/>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
       <c r="E11" s="23" t="s">
         <v>35</v>
       </c>
@@ -3242,7 +2997,7 @@
       <c r="G11" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="79" t="s">
+      <c r="H11" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="22">
@@ -3252,37 +3007,37 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O11" s="62"/>
-      <c r="V11" s="71">
+      <c r="O11" s="60"/>
+      <c r="V11" s="69">
         <f>X11-V10</f>
         <v>4</v>
       </c>
-      <c r="W11" s="70"/>
-      <c r="X11" s="72">
+      <c r="W11" s="68"/>
+      <c r="X11" s="70">
         <f>AA11</f>
         <v>6</v>
       </c>
-      <c r="AA11" s="71">
+      <c r="AA11" s="69">
         <f>AC11-AA10</f>
         <v>6</v>
       </c>
-      <c r="AB11" s="70"/>
-      <c r="AC11" s="72">
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="70">
         <f>AF5</f>
         <v>11</v>
       </c>
-      <c r="AE11" s="62"/>
-      <c r="BM11" s="62"/>
+      <c r="AE11" s="60"/>
+      <c r="BM11" s="60"/>
     </row>
     <row r="12" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
@@ -3292,7 +3047,7 @@
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="79">
+      <c r="H12" s="77">
         <v>1</v>
       </c>
       <c r="I12" s="22">
@@ -3302,24 +3057,24 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O12" s="62"/>
-      <c r="Z12" s="65"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
-      <c r="AC12" s="65"/>
-      <c r="AD12" s="65"/>
-      <c r="AE12" s="68"/>
-      <c r="BM12" s="62"/>
+      <c r="O12" s="60"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63"/>
+      <c r="AE12" s="66"/>
+      <c r="BM12" s="60"/>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="23" t="s">
         <v>37</v>
       </c>
@@ -3329,7 +3084,7 @@
       <c r="G13" s="1">
         <v>3</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I13" s="22">
@@ -3339,19 +3094,19 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="Y13" s="62"/>
-      <c r="BM13" s="62"/>
+      <c r="O13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="BM13" s="60"/>
     </row>
     <row r="14" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
@@ -3361,7 +3116,7 @@
       <c r="G14" s="1">
         <v>3</v>
       </c>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I14" s="22">
@@ -3371,46 +3126,46 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="O14" s="62"/>
-      <c r="Q14" s="69">
+      <c r="O14" s="60"/>
+      <c r="Q14" s="67">
         <f>N2</f>
         <v>2</v>
       </c>
-      <c r="R14" s="70"/>
-      <c r="S14" s="73">
+      <c r="R14" s="68"/>
+      <c r="S14" s="71">
         <f>Q14+Q16</f>
         <v>3</v>
       </c>
-      <c r="V14" s="69">
+      <c r="V14" s="67">
         <f>S14</f>
         <v>3</v>
       </c>
-      <c r="W14" s="70"/>
-      <c r="X14" s="73">
+      <c r="W14" s="68"/>
+      <c r="X14" s="71">
         <f>V14+V16</f>
         <v>9</v>
       </c>
-      <c r="Y14" s="66"/>
-      <c r="AA14" s="69">
+      <c r="Y14" s="64"/>
+      <c r="AA14" s="67">
         <f>X14</f>
         <v>9</v>
       </c>
-      <c r="AB14" s="70"/>
-      <c r="AC14" s="73">
+      <c r="AB14" s="68"/>
+      <c r="AC14" s="71">
         <f>AA14+AA16</f>
         <v>29</v>
       </c>
-      <c r="BM14" s="62"/>
+      <c r="BM14" s="60"/>
     </row>
     <row r="15" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="23" t="s">
         <v>41</v>
       </c>
@@ -3420,7 +3175,7 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I15" s="22">
@@ -3430,73 +3185,73 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O15" s="62"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="100" t="s">
+      <c r="O15" s="60"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="100"/>
-      <c r="S15" s="100"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="100" t="s">
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="59"/>
+      <c r="V15" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="W15" s="100"/>
-      <c r="X15" s="100"/>
-      <c r="Y15" s="60"/>
-      <c r="Z15" s="61"/>
-      <c r="AA15" s="100" t="s">
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="59"/>
+      <c r="AA15" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="AB15" s="100"/>
-      <c r="AC15" s="100"/>
-      <c r="AD15" s="60"/>
-      <c r="AE15" s="65"/>
-      <c r="AF15" s="65"/>
-      <c r="AG15" s="65"/>
-      <c r="AH15" s="65"/>
-      <c r="AI15" s="65"/>
-      <c r="AJ15" s="65"/>
-      <c r="AK15" s="65"/>
-      <c r="AL15" s="65"/>
-      <c r="AM15" s="65"/>
-      <c r="AN15" s="65"/>
-      <c r="AO15" s="65"/>
-      <c r="AP15" s="65"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="65"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="65"/>
-      <c r="AW15" s="65"/>
-      <c r="AX15" s="65"/>
-      <c r="AY15" s="65"/>
-      <c r="AZ15" s="65"/>
-      <c r="BA15" s="65"/>
-      <c r="BB15" s="65"/>
-      <c r="BC15" s="65"/>
-      <c r="BD15" s="65"/>
-      <c r="BE15" s="65"/>
-      <c r="BF15" s="65"/>
-      <c r="BG15" s="65"/>
-      <c r="BH15" s="65"/>
-      <c r="BI15" s="65"/>
-      <c r="BJ15" s="65"/>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="68"/>
+      <c r="AB15" s="98"/>
+      <c r="AC15" s="98"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="63"/>
+      <c r="AF15" s="63"/>
+      <c r="AG15" s="63"/>
+      <c r="AH15" s="63"/>
+      <c r="AI15" s="63"/>
+      <c r="AJ15" s="63"/>
+      <c r="AK15" s="63"/>
+      <c r="AL15" s="63"/>
+      <c r="AM15" s="63"/>
+      <c r="AN15" s="63"/>
+      <c r="AO15" s="63"/>
+      <c r="AP15" s="63"/>
+      <c r="AQ15" s="63"/>
+      <c r="AR15" s="63"/>
+      <c r="AS15" s="63"/>
+      <c r="AT15" s="63"/>
+      <c r="AU15" s="63"/>
+      <c r="AV15" s="63"/>
+      <c r="AW15" s="63"/>
+      <c r="AX15" s="63"/>
+      <c r="AY15" s="63"/>
+      <c r="AZ15" s="63"/>
+      <c r="BA15" s="63"/>
+      <c r="BB15" s="63"/>
+      <c r="BC15" s="63"/>
+      <c r="BD15" s="63"/>
+      <c r="BE15" s="63"/>
+      <c r="BF15" s="63"/>
+      <c r="BG15" s="63"/>
+      <c r="BH15" s="63"/>
+      <c r="BI15" s="63"/>
+      <c r="BJ15" s="63"/>
+      <c r="BK15" s="63"/>
+      <c r="BL15" s="63"/>
+      <c r="BM15" s="66"/>
     </row>
     <row r="16" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="23" t="s">
         <v>29</v>
       </c>
@@ -3506,7 +3261,7 @@
       <c r="G16" s="1">
         <v>5</v>
       </c>
-      <c r="H16" s="79" t="s">
+      <c r="H16" s="77" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="22">
@@ -3516,39 +3271,39 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="Q16" s="74">
+      <c r="Q16" s="72">
         <f>J7</f>
         <v>1</v>
       </c>
-      <c r="R16" s="75">
+      <c r="R16" s="73">
         <f>S17-S14</f>
         <v>0</v>
       </c>
-      <c r="S16" s="76">
+      <c r="S16" s="74">
         <f>V14-S14</f>
         <v>0</v>
       </c>
-      <c r="V16" s="74">
+      <c r="V16" s="72">
         <f>J8</f>
         <v>6</v>
       </c>
-      <c r="W16" s="75">
+      <c r="W16" s="73">
         <f>X17-X14</f>
         <v>0</v>
       </c>
-      <c r="X16" s="76">
+      <c r="X16" s="74">
         <f>MIN(AA14,AF2)-X14</f>
         <v>0</v>
       </c>
-      <c r="AA16" s="74">
+      <c r="AA16" s="72">
         <f>J12</f>
         <v>20</v>
       </c>
-      <c r="AB16" s="75">
+      <c r="AB16" s="73">
         <f>AC17-AC14</f>
         <v>0</v>
       </c>
-      <c r="AC16" s="76">
+      <c r="AC16" s="74">
         <f>BO2-AC14</f>
         <v>0</v>
       </c>
@@ -3557,11 +3312,11 @@
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="24" t="s">
         <v>58</v>
       </c>
@@ -3569,7 +3324,7 @@
       <c r="G17" s="26">
         <v>1</v>
       </c>
-      <c r="H17" s="80" t="s">
+      <c r="H17" s="78" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="22">
@@ -3579,41 +3334,41 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q17" s="71">
+      <c r="Q17" s="69">
         <f>S17-Q16</f>
         <v>2</v>
       </c>
-      <c r="R17" s="70"/>
-      <c r="S17" s="72">
+      <c r="R17" s="68"/>
+      <c r="S17" s="70">
         <f>V17</f>
         <v>3</v>
       </c>
-      <c r="V17" s="71">
+      <c r="V17" s="69">
         <f>X17-V16</f>
         <v>3</v>
       </c>
-      <c r="W17" s="70"/>
-      <c r="X17" s="72">
+      <c r="W17" s="68"/>
+      <c r="X17" s="70">
         <f>MIN(AA17,AF5)</f>
         <v>9</v>
       </c>
-      <c r="AA17" s="71">
+      <c r="AA17" s="69">
         <f>AC17-AA16</f>
         <v>9</v>
       </c>
-      <c r="AB17" s="70"/>
-      <c r="AC17" s="72">
+      <c r="AB17" s="68"/>
+      <c r="AC17" s="70">
         <f>BO5</f>
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="75" t="s">
         <v>75</v>
       </c>
       <c r="C19" t="s">
@@ -3621,11 +3376,11 @@
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="73" t="s">
+      <c r="B20" s="68"/>
+      <c r="C20" s="71" t="s">
         <v>66</v>
       </c>
       <c r="D20" t="s">
@@ -3633,20 +3388,20 @@
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="100" t="s">
+      <c r="A21" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="74" t="s">
         <v>70</v>
       </c>
       <c r="D22" t="s">
@@ -3654,11 +3409,11 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="72" t="s">
+      <c r="B23" s="68"/>
+      <c r="C23" s="70" t="s">
         <v>71</v>
       </c>
       <c r="D23" t="s">
@@ -3802,18 +3557,18 @@
   <dimension ref="A1:BN17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="11" topLeftCell="AU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15:XFD15"/>
+      <pane xSplit="11" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="16.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="11.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="9" width="11.5703125" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="3.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="3.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="65" width="3.5703125" customWidth="1"/>
+    <col min="7" max="9" width="11.5703125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="10" max="10" width="11.5703125" collapsed="1"/>
+    <col min="11" max="11" width="3.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="65" width="3.5703125" customWidth="1"/>
     <col min="66" max="66" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3821,11 +3576,11 @@
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="14" t="s">
         <v>46</v>
       </c>
@@ -4015,11 +3770,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17" t="s">
         <v>52</v>
@@ -4042,7 +3797,7 @@
       </c>
       <c r="K2" s="32">
         <f t="shared" ref="K2:K8" si="0">SUM(L2:BM2)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L2" s="33">
         <v>1</v>
@@ -4050,15 +3805,9 @@
       <c r="M2" s="33">
         <v>1</v>
       </c>
-      <c r="N2" s="33">
-        <v>1</v>
-      </c>
-      <c r="O2" s="33">
-        <v>1</v>
-      </c>
-      <c r="P2" s="33">
-        <v>1</v>
-      </c>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
@@ -4116,11 +3865,11 @@
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
       <c r="E3" s="20" t="s">
         <v>16</v>
       </c>
@@ -4149,14 +3898,14 @@
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="33">
-        <v>1</v>
-      </c>
+      <c r="S3" s="33"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
@@ -4211,11 +3960,11 @@
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
@@ -4240,28 +3989,26 @@
       </c>
       <c r="K4" s="32">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="10">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="33">
-        <v>1</v>
-      </c>
-      <c r="U4" s="33">
-        <v>1</v>
-      </c>
-      <c r="V4" s="33">
-        <v>1</v>
-      </c>
-      <c r="W4" s="33">
-        <v>1</v>
-      </c>
+      <c r="S4" s="10">
+        <v>1</v>
+      </c>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
@@ -4312,11 +4059,11 @@
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
@@ -4341,25 +4088,23 @@
       </c>
       <c r="K5" s="32">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
-      <c r="T5" s="33">
-        <v>1</v>
-      </c>
-      <c r="U5" s="33">
-        <v>1</v>
-      </c>
-      <c r="V5" s="33">
-        <v>1</v>
-      </c>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
@@ -4411,11 +4156,11 @@
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="23" t="s">
         <v>27</v>
       </c>
@@ -4449,27 +4194,27 @@
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="S6" s="10">
+        <v>1</v>
+      </c>
+      <c r="T6" s="10">
+        <v>1</v>
+      </c>
+      <c r="U6" s="10">
+        <v>1</v>
+      </c>
+      <c r="V6" s="10">
+        <v>1</v>
+      </c>
       <c r="W6" s="33">
         <v>1</v>
       </c>
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
-      <c r="Z6" s="33">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="33">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="33">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="33">
-        <v>1</v>
-      </c>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33"/>
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
       <c r="AF6" s="10"/>
@@ -4514,11 +4259,11 @@
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
       <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
@@ -4547,15 +4292,15 @@
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="10">
-        <v>1</v>
-      </c>
+      <c r="S7" s="100"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -4589,10 +4334,10 @@
       <c r="AY7" s="34"/>
       <c r="AZ7" s="10"/>
       <c r="BA7" s="10"/>
-      <c r="BB7" s="36"/>
-      <c r="BC7" s="36"/>
-      <c r="BD7" s="36"/>
-      <c r="BE7" s="36"/>
+      <c r="BB7" s="101"/>
+      <c r="BC7" s="101"/>
+      <c r="BD7" s="101"/>
+      <c r="BE7" s="101"/>
       <c r="BF7" s="34"/>
       <c r="BG7" s="10"/>
       <c r="BH7" s="10"/>
@@ -4609,11 +4354,11 @@
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="23" t="s">
         <v>22</v>
       </c>
@@ -4638,26 +4383,32 @@
       </c>
       <c r="K8" s="32">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="O8" s="10">
+        <v>1</v>
+      </c>
+      <c r="P8" s="10">
+        <v>1</v>
+      </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="33"/>
+      <c r="S8" s="10">
+        <v>1</v>
+      </c>
+      <c r="T8" s="33">
+        <v>1</v>
+      </c>
       <c r="U8" s="33">
         <v>1</v>
       </c>
       <c r="V8" s="33">
         <v>1</v>
       </c>
-      <c r="W8" s="10">
-        <v>1</v>
-      </c>
+      <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
@@ -4708,11 +4459,11 @@
       <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
       <c r="E9" s="23" t="s">
         <v>56</v>
       </c>
@@ -4753,19 +4504,19 @@
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
+      <c r="Z9" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>1</v>
+      </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="33"/>
       <c r="AE9" s="10"/>
       <c r="AF9" s="10"/>
-      <c r="AG9" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="10">
-        <v>1</v>
-      </c>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="10"/>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="10"/>
       <c r="AK9" s="10"/>
@@ -4805,11 +4556,11 @@
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
       <c r="E10" s="23" t="s">
         <v>33</v>
       </c>
@@ -4852,19 +4603,19 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="10">
+        <v>1</v>
+      </c>
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="33"/>
-      <c r="AI10" s="33">
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="10">
-        <v>1</v>
-      </c>
+      <c r="AI10" s="33"/>
+      <c r="AJ10" s="10"/>
       <c r="AK10" s="10"/>
       <c r="AL10" s="10"/>
       <c r="AM10" s="10"/>
@@ -4902,11 +4653,11 @@
       <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
       <c r="E11" s="23" t="s">
         <v>35</v>
       </c>
@@ -4951,20 +4702,20 @@
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
-      <c r="AD11" s="10"/>
+      <c r="AD11" s="10">
+        <v>1</v>
+      </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="10"/>
-      <c r="AG11" s="10"/>
+      <c r="AG11" s="10">
+        <v>1</v>
+      </c>
       <c r="AH11" s="10"/>
       <c r="AJ11" s="33"/>
-      <c r="AK11" s="33">
-        <v>1</v>
-      </c>
+      <c r="AK11" s="33"/>
       <c r="AL11" s="10"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="10">
-        <v>1</v>
-      </c>
+      <c r="AN11" s="10"/>
       <c r="AO11" s="10"/>
       <c r="AP11" s="10"/>
       <c r="AQ11" s="10"/>
@@ -4998,11 +4749,11 @@
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
@@ -5040,7 +4791,9 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
-      <c r="W12" s="33"/>
+      <c r="W12" s="33">
+        <v>1</v>
+      </c>
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="33">
@@ -5109,9 +4862,7 @@
       <c r="AY12" s="34"/>
       <c r="AZ12" s="10"/>
       <c r="BA12" s="10"/>
-      <c r="BB12" s="10">
-        <v>1</v>
-      </c>
+      <c r="BB12" s="10"/>
       <c r="BC12" s="10"/>
       <c r="BD12" s="10"/>
       <c r="BE12" s="10"/>
@@ -5130,11 +4881,11 @@
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="23" t="s">
         <v>37</v>
       </c>
@@ -5183,21 +4934,21 @@
       <c r="AE13" s="10"/>
       <c r="AF13" s="10"/>
       <c r="AG13" s="10"/>
-      <c r="AH13" s="10"/>
-      <c r="AI13" s="10"/>
-      <c r="AJ13" s="10"/>
+      <c r="AH13" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="10">
+        <v>1</v>
+      </c>
       <c r="AL13" s="10"/>
       <c r="AM13" s="10"/>
       <c r="AN13" s="33"/>
-      <c r="AO13" s="33">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="33">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="10">
-        <v>1</v>
-      </c>
+      <c r="AO13" s="33"/>
+      <c r="AP13" s="33"/>
+      <c r="AQ13" s="10"/>
       <c r="AR13" s="10"/>
       <c r="AS13" s="10"/>
       <c r="AT13" s="10"/>
@@ -5228,11 +4979,11 @@
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
@@ -5284,23 +5035,23 @@
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
+      <c r="AK14" s="10">
+        <v>1</v>
+      </c>
       <c r="AL14" s="10"/>
       <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
+      <c r="AN14" s="10">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ14" s="33"/>
-      <c r="AR14" s="33">
-        <v>1</v>
-      </c>
+      <c r="AR14" s="33"/>
       <c r="AS14" s="10"/>
       <c r="AT14" s="10"/>
-      <c r="AU14" s="33">
-        <v>1</v>
-      </c>
-      <c r="AV14" s="10">
-        <v>1</v>
-      </c>
+      <c r="AU14" s="33"/>
+      <c r="AV14" s="10"/>
       <c r="AW14" s="10"/>
       <c r="AX14" s="10"/>
       <c r="AY14" s="34"/>
@@ -5326,11 +5077,11 @@
       <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="23" t="s">
         <v>41</v>
       </c>
@@ -5387,7 +5138,9 @@
       <c r="AM15" s="10"/>
       <c r="AN15" s="10"/>
       <c r="AO15" s="10"/>
-      <c r="AP15" s="10"/>
+      <c r="AP15" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
       <c r="AS15" s="10"/>
@@ -5399,9 +5152,7 @@
       <c r="AY15" s="34"/>
       <c r="AZ15" s="10"/>
       <c r="BA15" s="10"/>
-      <c r="BB15" s="10">
-        <v>1</v>
-      </c>
+      <c r="BB15" s="10"/>
       <c r="BC15" s="10"/>
       <c r="BD15" s="10"/>
       <c r="BE15" s="10"/>
@@ -5421,11 +5172,11 @@
       <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="23" t="s">
         <v>29</v>
       </c>
@@ -5450,7 +5201,7 @@
       </c>
       <c r="K16" s="32">
         <f>SUM(L16:BM16)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -5483,27 +5234,31 @@
       <c r="AN16" s="10"/>
       <c r="AO16" s="10"/>
       <c r="AP16" s="10"/>
-      <c r="AQ16" s="10"/>
-      <c r="AR16" s="10"/>
+      <c r="AQ16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="10">
+        <v>1</v>
+      </c>
       <c r="AS16" s="10"/>
       <c r="AT16" s="10"/>
-      <c r="AU16" s="10"/>
-      <c r="AV16" s="10"/>
-      <c r="AW16" s="33"/>
+      <c r="AU16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="33">
+        <v>1</v>
+      </c>
       <c r="AX16" s="33"/>
       <c r="AY16" s="34"/>
       <c r="AZ16" s="10"/>
       <c r="BA16" s="10"/>
       <c r="BB16" s="33"/>
-      <c r="BC16" s="10">
-        <v>1</v>
-      </c>
-      <c r="BD16" s="10">
-        <v>1</v>
-      </c>
-      <c r="BE16" s="10">
-        <v>1</v>
-      </c>
+      <c r="BC16" s="10"/>
+      <c r="BD16" s="10"/>
+      <c r="BE16" s="10"/>
       <c r="BF16" s="34"/>
       <c r="BG16" s="10"/>
       <c r="BH16" s="10"/>
@@ -5519,11 +5274,11 @@
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="24" t="s">
         <v>58</v>
       </c>
@@ -5536,11 +5291,11 @@
         <f>Netzplan!H17</f>
         <v>1</v>
       </c>
-      <c r="I17" s="37">
+      <c r="I17" s="35">
         <f>Netzplan!I17</f>
         <v>1</v>
       </c>
-      <c r="J17" s="38">
+      <c r="J17" s="36">
         <f>Netzplan!J17</f>
         <v>1</v>
       </c>
@@ -5587,22 +5342,22 @@
       <c r="AV17" s="12"/>
       <c r="AW17" s="12"/>
       <c r="AX17" s="12"/>
-      <c r="AY17" s="39"/>
+      <c r="AY17" s="37"/>
       <c r="AZ17" s="12"/>
       <c r="BA17" s="12"/>
-      <c r="BB17" s="12"/>
+      <c r="BB17" s="12">
+        <v>1</v>
+      </c>
       <c r="BC17" s="33"/>
       <c r="BD17" s="12"/>
       <c r="BE17" s="12"/>
-      <c r="BF17" s="39"/>
+      <c r="BF17" s="37"/>
       <c r="BG17" s="12"/>
       <c r="BH17" s="12"/>
-      <c r="BI17" s="12">
-        <v>1</v>
-      </c>
+      <c r="BI17" s="12"/>
       <c r="BJ17" s="12"/>
       <c r="BK17" s="12"/>
-      <c r="BL17" s="39"/>
+      <c r="BL17" s="37"/>
       <c r="BM17" s="12"/>
       <c r="BN17" t="s">
         <v>60</v>
@@ -5633,7 +5388,7 @@
       <formula>IF(K2&lt;&gt;J2,TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI10:BM10 L10:AH12 AJ11:BM11 AI12:BA12 BF12:BH12 BJ12:BM12 L13:AJ13 AL13:BM13 L14:AO14 AQ14:BM14 L15:AT15 AV15:BM15 L16:AU16 AW16:BI16 BK16:BM16 L17:BA17 BC17:BM17 L1:BM9">
+  <conditionalFormatting sqref="AI10:BM10 L10:AH12 AJ11:BM11 BF12:BH12 BJ12:BM12 L13:AJ13 AL13:BM13 L14:AO14 AQ14:BM14 L15:AT15 AV15:BM15 L16:AU16 AW16:BI16 BK16:BM16 L17:BA17 BC17:BM17 L1:BM9 AG12:BA12">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>IF(OR(WEEKDAY(L$1)=7,WEEKDAY(L$1)=1),1,0)</formula>
     </cfRule>
@@ -5649,6 +5404,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>